<commit_message>
Update automatico via Actualizar 05-10-2020 05-40-59
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="668" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F71B3D90-C4B7-4873-AB29-5C06961016F4}"/>
+  <xr:revisionPtr revIDLastSave="740" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A97B96DF-7FB2-400F-8A27-7A04074535CF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="362">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -876,15 +876,24 @@
     <t>Hospital San Lorenzo</t>
   </si>
   <si>
+    <t>09</t>
+  </si>
+  <si>
     <t>Gracias a Dios</t>
   </si>
   <si>
+    <t>0901</t>
+  </si>
+  <si>
     <t xml:space="preserve">Puerto Lempira </t>
   </si>
   <si>
     <t>Hospital Puerto Lempira</t>
   </si>
   <si>
+    <t>1501</t>
+  </si>
+  <si>
     <t>Juticalpa</t>
   </si>
   <si>
@@ -894,6 +903,9 @@
     <t>Hospital Trochez Montalvan</t>
   </si>
   <si>
+    <t>1503</t>
+  </si>
+  <si>
     <t>Catacamas</t>
   </si>
   <si>
@@ -903,6 +915,9 @@
     <t>Clínica Medicentro</t>
   </si>
   <si>
+    <t>1206</t>
+  </si>
+  <si>
     <t>Guajiquiro</t>
   </si>
   <si>
@@ -912,21 +927,33 @@
     <t>Centro de Salud El Guajiquiro</t>
   </si>
   <si>
+    <t>1208</t>
+  </si>
+  <si>
     <t>Marcala</t>
   </si>
   <si>
     <t>Centro de Salud Marcala</t>
   </si>
   <si>
+    <t>1212</t>
+  </si>
+  <si>
     <t>San José</t>
   </si>
   <si>
+    <t>1201</t>
+  </si>
+  <si>
     <t>Hospital Montecillos</t>
   </si>
   <si>
     <t>Hospital Roberto Suazo Córdova</t>
   </si>
   <si>
+    <t>0301</t>
+  </si>
+  <si>
     <t>Hospital Regional Santa Teresa</t>
   </si>
   <si>
@@ -936,12 +963,18 @@
     <t>Hospital Privado de Comayagua</t>
   </si>
   <si>
+    <t>1001</t>
+  </si>
+  <si>
     <t>La Esperanza</t>
   </si>
   <si>
     <t>Hospital Enrique Aguila Cerrato</t>
   </si>
   <si>
+    <t>0107</t>
+  </si>
+  <si>
     <t>Tela</t>
   </si>
   <si>
@@ -954,21 +987,27 @@
     <t>Santa Barbará</t>
   </si>
   <si>
+    <t>1601</t>
+  </si>
+  <si>
     <t>Hospital Santa Barbará Integrado</t>
   </si>
   <si>
+    <t>1626</t>
+  </si>
+  <si>
     <t>Trinidad</t>
   </si>
   <si>
     <t>Clínica de Emergencia Trinidad</t>
   </si>
   <si>
-    <t>Sula</t>
-  </si>
-  <si>
     <t>Hospital Sula Socorro de lo Atlto</t>
   </si>
   <si>
+    <t>1615</t>
+  </si>
+  <si>
     <t>Petoa</t>
   </si>
   <si>
@@ -978,9 +1017,15 @@
     <t>Centro Médico Integral de Occidente</t>
   </si>
   <si>
+    <t>07</t>
+  </si>
+  <si>
     <t>El Paraíso</t>
   </si>
   <si>
+    <t>0704</t>
+  </si>
+  <si>
     <t>Centro Médico San Francisco</t>
   </si>
   <si>
@@ -993,6 +1038,9 @@
     <t>Centro de Salud San Antonio Sulaco Yoro</t>
   </si>
   <si>
+    <t>1811</t>
+  </si>
+  <si>
     <t>Yorito</t>
   </si>
   <si>
@@ -1002,36 +1050,51 @@
     <t>Centro de Salud La Sabana</t>
   </si>
   <si>
+    <t>1801</t>
+  </si>
+  <si>
     <t>Clínica Médica Dra. Chávez</t>
   </si>
   <si>
     <t>Hospital Manuel de Jesus Subirana</t>
   </si>
   <si>
-    <t>El Rosario</t>
-  </si>
-  <si>
     <t>ACTS Clinic</t>
   </si>
   <si>
+    <t>1313</t>
+  </si>
+  <si>
     <t>Lepaera</t>
   </si>
   <si>
     <t>Centro de Salud Lepaera</t>
   </si>
   <si>
+    <t>1322</t>
+  </si>
+  <si>
     <t>Santa Cruz</t>
   </si>
   <si>
     <t xml:space="preserve">Cesamo de Santa Cruz </t>
   </si>
   <si>
+    <t>1306</t>
+  </si>
+  <si>
     <t>Gualcinse</t>
   </si>
   <si>
     <t>Hospital del Sur Dr. Lempira</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>1701</t>
+  </si>
+  <si>
     <t>Nacaome</t>
   </si>
   <si>
@@ -1041,13 +1104,19 @@
     <t>Centro Médico Juárez</t>
   </si>
   <si>
+    <t>1707</t>
+  </si>
+  <si>
     <t>Langue</t>
   </si>
   <si>
     <t>Centro de Salud de Langue</t>
   </si>
   <si>
-    <t>Guascorán</t>
+    <t>1706</t>
+  </si>
+  <si>
+    <t>Goascorán</t>
   </si>
   <si>
     <t>Medicenter</t>
@@ -1377,7 +1446,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1501,6 +1570,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1546,7 +1626,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1555,6 +1635,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2037,8 +2118,8 @@
   <dimension ref="A1:W135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="D96:D135"/>
+      <pane ySplit="1" topLeftCell="D106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J114" sqref="J114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8556,7 +8637,7 @@
         <v>-87.443899000000002</v>
       </c>
     </row>
-    <row r="97" spans="2:23">
+    <row r="97" spans="2:23" ht="15">
       <c r="B97" s="1" t="s">
         <v>23</v>
       </c>
@@ -8566,17 +8647,32 @@
       <c r="D97" s="1">
         <v>3</v>
       </c>
+      <c r="E97" s="7">
+        <v>9</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>280</v>
+      </c>
       <c r="G97" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="7">
+        <v>1</v>
+      </c>
+      <c r="J97" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="S97" s="1" t="s">
         <v>246</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="V97" s="2">
         <v>15.265726000000001</v>
@@ -8585,7 +8681,7 @@
         <v>-83.781515999999996</v>
       </c>
     </row>
-    <row r="98" spans="2:23">
+    <row r="98" spans="2:23" ht="15">
       <c r="B98" s="1" t="s">
         <v>23</v>
       </c>
@@ -8594,18 +8690,33 @@
       </c>
       <c r="D98" s="1">
         <v>3</v>
+      </c>
+      <c r="E98" s="7">
+        <v>15</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H98" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I98" s="7">
+        <v>1</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>285</v>
+      </c>
       <c r="K98" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="S98" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U98" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="V98" s="2">
         <v>14.665319</v>
@@ -8614,7 +8725,7 @@
         <v>-86.225899999999996</v>
       </c>
     </row>
-    <row r="99" spans="2:23">
+    <row r="99" spans="2:23" ht="15">
       <c r="B99" s="1" t="s">
         <v>23</v>
       </c>
@@ -8623,18 +8734,33 @@
       </c>
       <c r="D99" s="1">
         <v>3</v>
+      </c>
+      <c r="E99" s="7">
+        <v>15</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H99" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I99" s="7">
+        <v>1</v>
+      </c>
+      <c r="J99" s="7" t="s">
+        <v>285</v>
+      </c>
       <c r="K99" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="S99" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="V99" s="2">
         <v>14.671486</v>
@@ -8643,7 +8769,7 @@
         <v>-86.221147999999999</v>
       </c>
     </row>
-    <row r="100" spans="2:23">
+    <row r="100" spans="2:23" ht="15">
       <c r="B100" s="1" t="s">
         <v>23</v>
       </c>
@@ -8652,18 +8778,33 @@
       </c>
       <c r="D100" s="1">
         <v>3</v>
+      </c>
+      <c r="E100" s="7">
+        <v>15</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H100" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I100" s="7">
+        <v>3</v>
+      </c>
+      <c r="J100" s="7" t="s">
+        <v>289</v>
+      </c>
       <c r="K100" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="S100" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="V100" s="2">
         <v>14.853908000000001</v>
@@ -8672,7 +8813,7 @@
         <v>-85.894442999999995</v>
       </c>
     </row>
-    <row r="101" spans="2:23">
+    <row r="101" spans="2:23" ht="15">
       <c r="B101" s="1" t="s">
         <v>23</v>
       </c>
@@ -8681,18 +8822,33 @@
       </c>
       <c r="D101" s="1">
         <v>3</v>
+      </c>
+      <c r="E101" s="7">
+        <v>15</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H101" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I101" s="7">
+        <v>3</v>
+      </c>
+      <c r="J101" s="7" t="s">
+        <v>289</v>
+      </c>
       <c r="K101" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="S101" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="V101" s="2">
         <v>14.851229</v>
@@ -8701,7 +8857,7 @@
         <v>-85.895388999999994</v>
       </c>
     </row>
-    <row r="102" spans="2:23">
+    <row r="102" spans="2:23" ht="15">
       <c r="B102" s="1" t="s">
         <v>23</v>
       </c>
@@ -8710,12 +8866,27 @@
       </c>
       <c r="D102" s="1">
         <v>3</v>
+      </c>
+      <c r="E102" s="7">
+        <v>15</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="H102" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="7">
+        <v>3</v>
+      </c>
+      <c r="J102" s="7" t="s">
+        <v>289</v>
+      </c>
       <c r="K102" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="S102" s="1" t="s">
         <v>72</v>
@@ -8730,7 +8901,7 @@
         <v>-85.895661000000004</v>
       </c>
     </row>
-    <row r="103" spans="2:23">
+    <row r="103" spans="2:23" ht="15">
       <c r="B103" s="1" t="s">
         <v>23</v>
       </c>
@@ -8739,18 +8910,33 @@
       </c>
       <c r="D103" s="1">
         <v>3</v>
+      </c>
+      <c r="E103" s="7">
+        <v>12</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H103" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I103" s="7">
+        <v>6</v>
+      </c>
+      <c r="J103" s="7" t="s">
+        <v>293</v>
+      </c>
       <c r="K103" s="1" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="V103" s="2">
         <v>14.120423000000001</v>
@@ -8759,7 +8945,7 @@
         <v>-87.829441000000003</v>
       </c>
     </row>
-    <row r="104" spans="2:23">
+    <row r="104" spans="2:23" ht="15">
       <c r="B104" s="1" t="s">
         <v>23</v>
       </c>
@@ -8768,18 +8954,33 @@
       </c>
       <c r="D104" s="1">
         <v>3</v>
+      </c>
+      <c r="E104" s="7">
+        <v>12</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H104" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I104" s="7">
+        <v>8</v>
+      </c>
+      <c r="J104" s="7" t="s">
+        <v>297</v>
+      </c>
       <c r="K104" s="1" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="V104" s="2">
         <v>14.159074</v>
@@ -8788,7 +8989,7 @@
         <v>-88.036270999999999</v>
       </c>
     </row>
-    <row r="105" spans="2:23">
+    <row r="105" spans="2:23" ht="15">
       <c r="B105" s="1" t="s">
         <v>23</v>
       </c>
@@ -8797,15 +8998,30 @@
       </c>
       <c r="D105" s="1">
         <v>3</v>
+      </c>
+      <c r="E105" s="7">
+        <v>12</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H105" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="7">
+        <v>12</v>
+      </c>
+      <c r="J105" s="7" t="s">
+        <v>300</v>
+      </c>
       <c r="K105" s="1" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="S105" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>44</v>
@@ -8817,7 +9033,7 @@
         <v>-87.959114999999997</v>
       </c>
     </row>
-    <row r="106" spans="2:23">
+    <row r="106" spans="2:23" ht="15">
       <c r="B106" s="1" t="s">
         <v>23</v>
       </c>
@@ -8826,10 +9042,25 @@
       </c>
       <c r="D106" s="1">
         <v>3</v>
+      </c>
+      <c r="E106" s="7">
+        <v>12</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H106" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I106" s="7">
+        <v>1</v>
+      </c>
+      <c r="J106" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="K106" s="1" t="s">
         <v>63</v>
       </c>
@@ -8837,7 +9068,7 @@
         <v>179</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="V106" s="2">
         <v>14.319006</v>
@@ -8846,7 +9077,7 @@
         <v>-87.680940000000007</v>
       </c>
     </row>
-    <row r="107" spans="2:23">
+    <row r="107" spans="2:23" ht="15">
       <c r="B107" s="1" t="s">
         <v>23</v>
       </c>
@@ -8855,10 +9086,25 @@
       </c>
       <c r="D107" s="1">
         <v>3</v>
+      </c>
+      <c r="E107" s="7">
+        <v>12</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="H107" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I107" s="7">
+        <v>1</v>
+      </c>
+      <c r="J107" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="K107" s="1" t="s">
         <v>63</v>
       </c>
@@ -8866,7 +9112,7 @@
         <v>179</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="V107" s="2">
         <v>14.322329999999999</v>
@@ -8875,7 +9121,7 @@
         <v>-87.678188000000006</v>
       </c>
     </row>
-    <row r="108" spans="2:23">
+    <row r="108" spans="2:23" ht="15">
       <c r="B108" s="1" t="s">
         <v>23</v>
       </c>
@@ -8884,10 +9130,25 @@
       </c>
       <c r="D108" s="1">
         <v>3</v>
+      </c>
+      <c r="E108" s="7">
+        <v>3</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H108" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I108" s="7">
+        <v>1</v>
+      </c>
+      <c r="J108" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="K108" s="1" t="s">
         <v>189</v>
       </c>
@@ -8895,7 +9156,7 @@
         <v>179</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="V108" s="2">
         <v>14.453317999999999</v>
@@ -8904,7 +9165,7 @@
         <v>-87.642769000000001</v>
       </c>
     </row>
-    <row r="109" spans="2:23">
+    <row r="109" spans="2:23" ht="15">
       <c r="B109" s="1" t="s">
         <v>23</v>
       </c>
@@ -8913,10 +9174,25 @@
       </c>
       <c r="D109" s="1">
         <v>3</v>
+      </c>
+      <c r="E109" s="7">
+        <v>3</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H109" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I109" s="7">
+        <v>1</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="K109" s="1" t="s">
         <v>189</v>
       </c>
@@ -8924,7 +9200,7 @@
         <v>179</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="V109" s="2">
         <v>14.456941</v>
@@ -8933,7 +9209,7 @@
         <v>-87.635479000000004</v>
       </c>
     </row>
-    <row r="110" spans="2:23">
+    <row r="110" spans="2:23" ht="15">
       <c r="B110" s="1" t="s">
         <v>23</v>
       </c>
@@ -8942,10 +9218,25 @@
       </c>
       <c r="D110" s="1">
         <v>3</v>
+      </c>
+      <c r="E110" s="7">
+        <v>3</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H110" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I110" s="7">
+        <v>1</v>
+      </c>
+      <c r="J110" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="K110" s="1" t="s">
         <v>189</v>
       </c>
@@ -8953,7 +9244,7 @@
         <v>179</v>
       </c>
       <c r="U110" s="1" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="V110" s="2">
         <v>14.460008999999999</v>
@@ -8962,7 +9253,7 @@
         <v>-87.638285999999994</v>
       </c>
     </row>
-    <row r="111" spans="2:23">
+    <row r="111" spans="2:23" ht="15">
       <c r="B111" s="1" t="s">
         <v>23</v>
       </c>
@@ -8971,10 +9262,25 @@
       </c>
       <c r="D111" s="1">
         <v>3</v>
+      </c>
+      <c r="E111" s="7">
+        <v>3</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="H111" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I111" s="7">
+        <v>18</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>190</v>
+      </c>
       <c r="K111" s="1" t="s">
         <v>191</v>
       </c>
@@ -8991,7 +9297,7 @@
         <v>-87.844590999999994</v>
       </c>
     </row>
-    <row r="112" spans="2:23">
+    <row r="112" spans="2:23" ht="15">
       <c r="B112" s="1" t="s">
         <v>23</v>
       </c>
@@ -9000,18 +9306,33 @@
       </c>
       <c r="D112" s="1">
         <v>3</v>
+      </c>
+      <c r="E112" s="7">
+        <v>10</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>134</v>
       </c>
+      <c r="H112" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I112" s="7">
+        <v>1</v>
+      </c>
+      <c r="J112" s="7" t="s">
+        <v>309</v>
+      </c>
       <c r="K112" s="1" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="S112" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="V112" s="2">
         <v>14.314704000000001</v>
@@ -9020,7 +9341,7 @@
         <v>-88.160505999999998</v>
       </c>
     </row>
-    <row r="113" spans="2:23">
+    <row r="113" spans="2:23" ht="15">
       <c r="B113" s="1" t="s">
         <v>23</v>
       </c>
@@ -9029,18 +9350,33 @@
       </c>
       <c r="D113" s="1">
         <v>3</v>
+      </c>
+      <c r="E113" s="7">
+        <v>1</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H113" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="7">
+        <v>7</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>312</v>
+      </c>
       <c r="K113" s="1" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="S113" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="V113" s="2">
         <v>15.754151999999999</v>
@@ -9049,7 +9385,7 @@
         <v>-87.489628999999994</v>
       </c>
     </row>
-    <row r="114" spans="2:23">
+    <row r="114" spans="2:23" ht="15">
       <c r="B114" s="1" t="s">
         <v>23</v>
       </c>
@@ -9059,14 +9395,23 @@
       <c r="D114" s="1">
         <v>3</v>
       </c>
+      <c r="E114" s="7">
+        <v>9</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>280</v>
+      </c>
       <c r="G114" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="S114" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="V114" s="2">
         <v>15.908462</v>
@@ -9075,7 +9420,7 @@
         <v>-84.814170000000004</v>
       </c>
     </row>
-    <row r="115" spans="2:23">
+    <row r="115" spans="2:23" ht="15">
       <c r="B115" s="1" t="s">
         <v>23</v>
       </c>
@@ -9085,17 +9430,32 @@
       <c r="D115" s="1">
         <v>3</v>
       </c>
+      <c r="E115" s="7">
+        <v>16</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G115" s="1" t="s">
-        <v>305</v>
+        <v>316</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I115" s="7">
+        <v>1</v>
+      </c>
+      <c r="J115" s="7" t="s">
+        <v>317</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="S115" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="V115" s="2">
         <v>14.925007000000001</v>
@@ -9104,7 +9464,7 @@
         <v>-88.237927999999997</v>
       </c>
     </row>
-    <row r="116" spans="2:23">
+    <row r="116" spans="2:23" ht="15">
       <c r="B116" s="1" t="s">
         <v>23</v>
       </c>
@@ -9114,17 +9474,32 @@
       <c r="D116" s="1">
         <v>3</v>
       </c>
+      <c r="E116" s="7">
+        <v>16</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G116" s="1" t="s">
-        <v>305</v>
+        <v>316</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="7">
+        <v>26</v>
+      </c>
+      <c r="J116" s="7" t="s">
+        <v>319</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="S116" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="V116" s="2">
         <v>15.143121000000001</v>
@@ -9143,17 +9518,23 @@
       <c r="D117" s="1">
         <v>3</v>
       </c>
+      <c r="E117" s="7">
+        <v>16</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G117" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="K117" s="1" t="s">
-        <v>309</v>
+        <v>316</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="S117" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="V117" s="2">
         <v>15.247275</v>
@@ -9162,7 +9543,7 @@
         <v>-88.552238000000003</v>
       </c>
     </row>
-    <row r="118" spans="2:23">
+    <row r="118" spans="2:23" ht="15">
       <c r="B118" s="1" t="s">
         <v>23</v>
       </c>
@@ -9172,17 +9553,32 @@
       <c r="D118" s="1">
         <v>3</v>
       </c>
+      <c r="E118" s="7">
+        <v>16</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G118" s="1" t="s">
-        <v>305</v>
+        <v>316</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I118" s="7">
+        <v>15</v>
+      </c>
+      <c r="J118" s="7" t="s">
+        <v>323</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="S118" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="V118" s="2">
         <v>15.273072000000001</v>
@@ -9191,7 +9587,7 @@
         <v>-88.284302999999994</v>
       </c>
     </row>
-    <row r="119" spans="2:23">
+    <row r="119" spans="2:23" ht="15">
       <c r="B119" s="1" t="s">
         <v>23</v>
       </c>
@@ -9201,8 +9597,23 @@
       <c r="D119" s="1">
         <v>3</v>
       </c>
+      <c r="E119" s="7">
+        <v>16</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="G119" s="1" t="s">
-        <v>305</v>
+        <v>316</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="7">
+        <v>17</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>239</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>240</v>
@@ -9211,7 +9622,7 @@
         <v>179</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="V119" s="2">
         <v>15.348732999999999</v>
@@ -9220,7 +9631,7 @@
         <v>-88.403704000000005</v>
       </c>
     </row>
-    <row r="120" spans="2:23">
+    <row r="120" spans="2:23" ht="15">
       <c r="B120" s="1" t="s">
         <v>23</v>
       </c>
@@ -9230,17 +9641,32 @@
       <c r="D120" s="1">
         <v>3</v>
       </c>
+      <c r="E120" s="7">
+        <v>7</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>327</v>
+      </c>
       <c r="G120" s="1" t="s">
-        <v>314</v>
+        <v>328</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I120" s="7">
+        <v>4</v>
+      </c>
+      <c r="J120" s="7" t="s">
+        <v>329</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="S120" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="V120" s="2">
         <v>13.861846</v>
@@ -9249,7 +9675,7 @@
         <v>-86.554258000000004</v>
       </c>
     </row>
-    <row r="121" spans="2:23">
+    <row r="121" spans="2:23" ht="15">
       <c r="B121" s="1" t="s">
         <v>23</v>
       </c>
@@ -9259,17 +9685,32 @@
       <c r="D121" s="1">
         <v>3</v>
       </c>
+      <c r="E121" s="7">
+        <v>7</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>327</v>
+      </c>
       <c r="G121" s="1" t="s">
-        <v>314</v>
+        <v>328</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I121" s="7">
+        <v>4</v>
+      </c>
+      <c r="J121" s="7" t="s">
+        <v>329</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="S121" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="V121" s="2">
         <v>13.865371</v>
@@ -9278,7 +9719,7 @@
         <v>-86.562415000000001</v>
       </c>
     </row>
-    <row r="122" spans="2:23">
+    <row r="122" spans="2:23" ht="15">
       <c r="B122" s="1" t="s">
         <v>23</v>
       </c>
@@ -9288,14 +9729,23 @@
       <c r="D122" s="1">
         <v>3</v>
       </c>
+      <c r="E122" s="7">
+        <v>18</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="G122" s="1" t="s">
-        <v>317</v>
+        <v>332</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="S122" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="V122" s="2">
         <v>14.985823</v>
@@ -9304,7 +9754,7 @@
         <v>-87.294527000000002</v>
       </c>
     </row>
-    <row r="123" spans="2:23">
+    <row r="123" spans="2:23" ht="15">
       <c r="B123" s="1" t="s">
         <v>23</v>
       </c>
@@ -9313,18 +9763,33 @@
       </c>
       <c r="D123" s="1">
         <v>3</v>
+      </c>
+      <c r="E123" s="7">
+        <v>18</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="H123" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I123" s="8">
+        <v>11</v>
+      </c>
+      <c r="J123" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="K123" s="1" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="S123" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>320</v>
+        <v>336</v>
       </c>
       <c r="V123" s="2">
         <v>15.065429</v>
@@ -9343,14 +9808,23 @@
       <c r="D124" s="1">
         <v>3</v>
       </c>
+      <c r="E124" s="7">
+        <v>18</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="G124" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="H124" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="S124" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="V124" s="2">
         <v>15.108616</v>
@@ -9359,7 +9833,7 @@
         <v>-87.280530999999996</v>
       </c>
     </row>
-    <row r="125" spans="2:23">
+    <row r="125" spans="2:23" ht="15">
       <c r="B125" s="1" t="s">
         <v>23</v>
       </c>
@@ -9368,10 +9842,25 @@
       </c>
       <c r="D125" s="1">
         <v>3</v>
+      </c>
+      <c r="E125" s="7">
+        <v>18</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="H125" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I125" s="7">
+        <v>1</v>
+      </c>
+      <c r="J125" s="7" t="s">
+        <v>338</v>
+      </c>
       <c r="K125" s="1" t="s">
         <v>162</v>
       </c>
@@ -9379,7 +9868,7 @@
         <v>72</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
       <c r="V125" s="2">
         <v>15.137855999999999</v>
@@ -9388,7 +9877,7 @@
         <v>-87.125667000000007</v>
       </c>
     </row>
-    <row r="126" spans="2:23">
+    <row r="126" spans="2:23" ht="15">
       <c r="B126" s="1" t="s">
         <v>23</v>
       </c>
@@ -9397,10 +9886,25 @@
       </c>
       <c r="D126" s="1">
         <v>3</v>
+      </c>
+      <c r="E126" s="7">
+        <v>18</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="H126" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I126" s="7">
+        <v>1</v>
+      </c>
+      <c r="J126" s="7" t="s">
+        <v>338</v>
+      </c>
       <c r="K126" s="1" t="s">
         <v>162</v>
       </c>
@@ -9408,7 +9912,7 @@
         <v>179</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>323</v>
+        <v>340</v>
       </c>
       <c r="V126" s="2">
         <v>15.137337</v>
@@ -9427,17 +9931,23 @@
       <c r="D127" s="1">
         <v>3</v>
       </c>
+      <c r="E127" s="7">
+        <v>18</v>
+      </c>
+      <c r="F127" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="G127" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="K127" s="1" t="s">
-        <v>324</v>
+      <c r="H127" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="S127" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>325</v>
+        <v>341</v>
       </c>
       <c r="V127" s="2">
         <v>15.276194</v>
@@ -9446,7 +9956,7 @@
         <v>-87.324967999999998</v>
       </c>
     </row>
-    <row r="128" spans="2:23">
+    <row r="128" spans="2:23" ht="15">
       <c r="B128" s="1" t="s">
         <v>23</v>
       </c>
@@ -9455,18 +9965,33 @@
       </c>
       <c r="D128" s="1">
         <v>3</v>
+      </c>
+      <c r="E128" s="7">
+        <v>13</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H128" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I128" s="7">
+        <v>13</v>
+      </c>
+      <c r="J128" s="7" t="s">
+        <v>342</v>
+      </c>
       <c r="K128" s="1" t="s">
-        <v>326</v>
+        <v>343</v>
       </c>
       <c r="S128" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="V128" s="2">
         <v>14.780340000000001</v>
@@ -9475,7 +10000,7 @@
         <v>-88.588606999999996</v>
       </c>
     </row>
-    <row r="129" spans="2:23">
+    <row r="129" spans="2:23" ht="15">
       <c r="B129" s="1" t="s">
         <v>23</v>
       </c>
@@ -9484,18 +10009,33 @@
       </c>
       <c r="D129" s="1">
         <v>3</v>
+      </c>
+      <c r="E129" s="7">
+        <v>13</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H129" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I129" s="7">
+        <v>22</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>345</v>
+      </c>
       <c r="K129" s="1" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
       <c r="S129" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>329</v>
+        <v>347</v>
       </c>
       <c r="V129" s="2">
         <v>14.329539</v>
@@ -9504,7 +10044,7 @@
         <v>-88.522634999999994</v>
       </c>
     </row>
-    <row r="130" spans="2:23">
+    <row r="130" spans="2:23" ht="15">
       <c r="B130" s="1" t="s">
         <v>23</v>
       </c>
@@ -9513,18 +10053,33 @@
       </c>
       <c r="D130" s="1">
         <v>3</v>
+      </c>
+      <c r="E130" s="7">
+        <v>13</v>
+      </c>
+      <c r="F130" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H130" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I130" s="7">
+        <v>6</v>
+      </c>
+      <c r="J130" s="7" t="s">
+        <v>348</v>
+      </c>
       <c r="K130" s="1" t="s">
-        <v>330</v>
+        <v>349</v>
       </c>
       <c r="S130" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>331</v>
+        <v>350</v>
       </c>
       <c r="V130" s="2">
         <v>14.126211</v>
@@ -9543,9 +10098,18 @@
       <c r="D131" s="1">
         <v>3</v>
       </c>
+      <c r="E131" s="7">
+        <v>13</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>142</v>
+      </c>
       <c r="G131" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H131" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="S131" s="1" t="s">
         <v>36</v>
       </c>
@@ -9559,7 +10123,7 @@
         <v>-88.651722000000007</v>
       </c>
     </row>
-    <row r="132" spans="2:23">
+    <row r="132" spans="2:23" ht="15">
       <c r="B132" s="1" t="s">
         <v>23</v>
       </c>
@@ -9568,18 +10132,33 @@
       </c>
       <c r="D132" s="1">
         <v>3</v>
+      </c>
+      <c r="E132" s="7">
+        <v>17</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="H132" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I132" s="7">
+        <v>1</v>
+      </c>
+      <c r="J132" s="7" t="s">
+        <v>352</v>
+      </c>
       <c r="K132" s="1" t="s">
-        <v>332</v>
+        <v>353</v>
       </c>
       <c r="S132" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>333</v>
+        <v>354</v>
       </c>
       <c r="V132" s="2">
         <v>13.530787999999999</v>
@@ -9588,7 +10167,7 @@
         <v>-87.498217999999994</v>
       </c>
     </row>
-    <row r="133" spans="2:23">
+    <row r="133" spans="2:23" ht="15">
       <c r="B133" s="1" t="s">
         <v>23</v>
       </c>
@@ -9597,18 +10176,33 @@
       </c>
       <c r="D133" s="1">
         <v>3</v>
+      </c>
+      <c r="E133" s="7">
+        <v>17</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="H133" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I133" s="7">
+        <v>1</v>
+      </c>
+      <c r="J133" s="7" t="s">
+        <v>352</v>
+      </c>
       <c r="K133" s="1" t="s">
-        <v>332</v>
+        <v>353</v>
       </c>
       <c r="S133" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>334</v>
+        <v>355</v>
       </c>
       <c r="V133" s="2">
         <v>13.532709000000001</v>
@@ -9617,7 +10211,7 @@
         <v>-87.492543999999995</v>
       </c>
     </row>
-    <row r="134" spans="2:23">
+    <row r="134" spans="2:23" ht="15">
       <c r="B134" s="1" t="s">
         <v>23</v>
       </c>
@@ -9626,18 +10220,33 @@
       </c>
       <c r="D134" s="1">
         <v>3</v>
+      </c>
+      <c r="E134" s="7">
+        <v>17</v>
+      </c>
+      <c r="F134" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="H134" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I134" s="7">
+        <v>7</v>
+      </c>
+      <c r="J134" s="7" t="s">
+        <v>356</v>
+      </c>
       <c r="K134" s="1" t="s">
-        <v>335</v>
+        <v>357</v>
       </c>
       <c r="S134" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>336</v>
+        <v>358</v>
       </c>
       <c r="V134" s="2">
         <v>13.62003</v>
@@ -9646,7 +10255,7 @@
         <v>-87.657388999999995</v>
       </c>
     </row>
-    <row r="135" spans="2:23">
+    <row r="135" spans="2:23" ht="15">
       <c r="B135" s="1" t="s">
         <v>23</v>
       </c>
@@ -9655,18 +10264,33 @@
       </c>
       <c r="D135" s="1">
         <v>3</v>
+      </c>
+      <c r="E135" s="7">
+        <v>17</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="H135" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I135" s="7">
+        <v>6</v>
+      </c>
+      <c r="J135" s="7" t="s">
+        <v>359</v>
+      </c>
       <c r="K135" s="1" t="s">
-        <v>337</v>
+        <v>360</v>
       </c>
       <c r="S135" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>338</v>
+        <v>361</v>
       </c>
       <c r="V135" s="2">
         <v>13.610545</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-11-2020 17-45-31
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="740" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A97B96DF-7FB2-400F-8A27-7A04074535CF}"/>
+  <xr:revisionPtr revIDLastSave="756" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{79201995-0D06-4727-B7F9-DF366F1F47F5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="362">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -786,6 +786,9 @@
     <t>Hospital General San Felipe</t>
   </si>
   <si>
+    <t>07</t>
+  </si>
+  <si>
     <t>El Paraiso</t>
   </si>
   <si>
@@ -861,6 +864,9 @@
     <t>Hospital San Marcos de Ocotepeque</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>Valle</t>
   </si>
   <si>
@@ -1017,9 +1023,6 @@
     <t>Centro Médico Integral de Occidente</t>
   </si>
   <si>
-    <t>07</t>
-  </si>
-  <si>
     <t>El Paraíso</t>
   </si>
   <si>
@@ -1087,9 +1090,6 @@
   </si>
   <si>
     <t>Hospital del Sur Dr. Lempira</t>
-  </si>
-  <si>
-    <t>17</t>
   </si>
   <si>
     <t>1701</t>
@@ -2118,8 +2118,8 @@
   <dimension ref="A1:W135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="D106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J114" sqref="J114"/>
+      <pane ySplit="1" topLeftCell="L2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86:F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -2138,7 +2138,7 @@
     <col min="12" max="12" width="12.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="20.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="15" style="1" customWidth="1"/>
     <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
@@ -7808,8 +7808,8 @@
       <c r="E84" s="1">
         <v>8</v>
       </c>
-      <c r="F84" s="1">
-        <v>8</v>
+      <c r="F84" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>39</v>
@@ -7876,8 +7876,8 @@
       <c r="E85" s="1">
         <v>8</v>
       </c>
-      <c r="F85" s="1">
-        <v>8</v>
+      <c r="F85" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>39</v>
@@ -7941,14 +7941,14 @@
       <c r="D86" s="1">
         <v>3</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="7">
         <v>7</v>
       </c>
-      <c r="F86" s="1">
-        <v>7</v>
+      <c r="F86" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>27</v>
@@ -7957,22 +7957,22 @@
         <v>3</v>
       </c>
       <c r="J86" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="P86" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q86" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="R86" s="1" t="s">
         <v>35</v>
@@ -7984,7 +7984,7 @@
         <v>247</v>
       </c>
       <c r="U86" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="V86" s="2">
         <v>13.991413</v>
@@ -8006,8 +8006,8 @@
       <c r="E87" s="1">
         <v>11</v>
       </c>
-      <c r="F87" s="1">
-        <v>11</v>
+      <c r="F87" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>56</v>
@@ -8046,7 +8046,7 @@
         <v>247</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="V87" s="2">
         <v>16.317903000000001</v>
@@ -8068,8 +8068,8 @@
       <c r="E88" s="1">
         <v>5</v>
       </c>
-      <c r="F88" s="1">
-        <v>5</v>
+      <c r="F88" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>85</v>
@@ -8114,7 +8114,7 @@
         <v>247</v>
       </c>
       <c r="U88" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="V88" s="2">
         <v>15.524452999999999</v>
@@ -8136,8 +8136,8 @@
       <c r="E89" s="1">
         <v>5</v>
       </c>
-      <c r="F89" s="1">
-        <v>5</v>
+      <c r="F89" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>85</v>
@@ -8182,7 +8182,7 @@
         <v>247</v>
       </c>
       <c r="U89" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="V89" s="2">
         <v>15.500176</v>
@@ -8204,8 +8204,8 @@
       <c r="E90" s="1">
         <v>5</v>
       </c>
-      <c r="F90" s="1">
-        <v>5</v>
+      <c r="F90" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>85</v>
@@ -8220,7 +8220,7 @@
         <v>92</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>30</v>
@@ -8232,7 +8232,7 @@
         <v>94</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="P90" s="1" t="s">
         <v>33</v>
@@ -8250,7 +8250,7 @@
         <v>247</v>
       </c>
       <c r="U90" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="V90" s="2">
         <v>15.814730000000001</v>
@@ -8272,8 +8272,8 @@
       <c r="E91" s="1">
         <v>6</v>
       </c>
-      <c r="F91" s="1">
-        <v>6</v>
+      <c r="F91" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>98</v>
@@ -8318,7 +8318,7 @@
         <v>247</v>
       </c>
       <c r="U91" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="V91" s="2">
         <v>13.303027999999999</v>
@@ -8340,8 +8340,8 @@
       <c r="E92" s="1">
         <v>1</v>
       </c>
-      <c r="F92" s="1">
-        <v>1</v>
+      <c r="F92" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>26</v>
@@ -8380,7 +8380,7 @@
         <v>247</v>
       </c>
       <c r="U92" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="V92" s="2">
         <v>15.769266</v>
@@ -8415,22 +8415,22 @@
         <v>1</v>
       </c>
       <c r="J93" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P93" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="R93" s="1" t="s">
         <v>35</v>
@@ -8442,7 +8442,7 @@
         <v>247</v>
       </c>
       <c r="U93" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="V93" s="2">
         <v>14.768719000000001</v>
@@ -8477,22 +8477,22 @@
         <v>1</v>
       </c>
       <c r="J94" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="R94" s="1" t="s">
         <v>35</v>
@@ -8504,7 +8504,7 @@
         <v>247</v>
       </c>
       <c r="U94" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="V94" s="2">
         <v>15.920894000000001</v>
@@ -8530,7 +8530,7 @@
         <v>14</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>27</v>
@@ -8539,22 +8539,22 @@
         <v>13</v>
       </c>
       <c r="J95" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="P95" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="R95" s="1" t="s">
         <v>35</v>
@@ -8566,7 +8566,7 @@
         <v>247</v>
       </c>
       <c r="U95" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="V95" s="2">
         <v>14.412167999999999</v>
@@ -8585,14 +8585,14 @@
       <c r="D96" s="1">
         <v>3</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96" s="7">
         <v>17</v>
       </c>
-      <c r="F96" s="1">
-        <v>17</v>
+      <c r="F96" s="7" t="s">
+        <v>276</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>27</v>
@@ -8601,22 +8601,22 @@
         <v>9</v>
       </c>
       <c r="J96" s="7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="P96" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q96" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="R96" s="1" t="s">
         <v>35</v>
@@ -8628,7 +8628,7 @@
         <v>247</v>
       </c>
       <c r="U96" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="V96" s="2">
         <v>13.435276</v>
@@ -8651,10 +8651,10 @@
         <v>9</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>27</v>
@@ -8663,16 +8663,19 @@
         <v>1</v>
       </c>
       <c r="J97" s="7" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S97" s="1" t="s">
         <v>246</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="V97" s="2">
         <v>15.265726000000001</v>
@@ -8707,16 +8710,19 @@
         <v>1</v>
       </c>
       <c r="J98" s="7" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S98" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U98" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="V98" s="2">
         <v>14.665319</v>
@@ -8751,16 +8757,19 @@
         <v>1</v>
       </c>
       <c r="J99" s="7" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S99" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="V99" s="2">
         <v>14.671486</v>
@@ -8795,16 +8804,19 @@
         <v>3</v>
       </c>
       <c r="J100" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S100" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="V100" s="2">
         <v>14.853908000000001</v>
@@ -8839,16 +8851,19 @@
         <v>3</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S101" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="V101" s="2">
         <v>14.851229</v>
@@ -8883,10 +8898,13 @@
         <v>3</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S102" s="1" t="s">
         <v>72</v>
@@ -8927,16 +8945,19 @@
         <v>6</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="V103" s="2">
         <v>14.120423000000001</v>
@@ -8971,16 +8992,19 @@
         <v>8</v>
       </c>
       <c r="J104" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S104" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="K104" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="S104" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="U104" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="V104" s="2">
         <v>14.159074</v>
@@ -9015,13 +9039,16 @@
         <v>12</v>
       </c>
       <c r="J105" s="7" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S105" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>44</v>
@@ -9059,16 +9086,19 @@
         <v>1</v>
       </c>
       <c r="J106" s="7" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="L106" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S106" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="V106" s="2">
         <v>14.319006</v>
@@ -9103,16 +9133,19 @@
         <v>1</v>
       </c>
       <c r="J107" s="7" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="L107" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S107" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="V107" s="2">
         <v>14.322329999999999</v>
@@ -9147,16 +9180,19 @@
         <v>1</v>
       </c>
       <c r="J108" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="L108" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S108" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="V108" s="2">
         <v>14.453317999999999</v>
@@ -9191,16 +9227,19 @@
         <v>1</v>
       </c>
       <c r="J109" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="L109" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S109" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="V109" s="2">
         <v>14.456941</v>
@@ -9235,16 +9274,19 @@
         <v>1</v>
       </c>
       <c r="J110" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="L110" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S110" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U110" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="V110" s="2">
         <v>14.460008999999999</v>
@@ -9284,6 +9326,9 @@
       <c r="K111" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="L111" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S111" s="1" t="s">
         <v>179</v>
       </c>
@@ -9323,16 +9368,19 @@
         <v>1</v>
       </c>
       <c r="J112" s="7" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S112" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="V112" s="2">
         <v>14.314704000000001</v>
@@ -9367,16 +9415,19 @@
         <v>7</v>
       </c>
       <c r="J113" s="7" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S113" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="V113" s="2">
         <v>15.754151999999999</v>
@@ -9399,19 +9450,22 @@
         <v>9</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S114" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="V114" s="2">
         <v>15.908462</v>
@@ -9437,7 +9491,7 @@
         <v>237</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>27</v>
@@ -9446,16 +9500,19 @@
         <v>1</v>
       </c>
       <c r="J115" s="7" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S115" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="V115" s="2">
         <v>14.925007000000001</v>
@@ -9481,7 +9538,7 @@
         <v>237</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>27</v>
@@ -9490,16 +9547,19 @@
         <v>26</v>
       </c>
       <c r="J116" s="7" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S116" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="V116" s="2">
         <v>15.143121000000001</v>
@@ -9525,16 +9585,19 @@
         <v>237</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="L117" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S117" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="V117" s="2">
         <v>15.247275</v>
@@ -9560,7 +9623,7 @@
         <v>237</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>27</v>
@@ -9569,16 +9632,19 @@
         <v>15</v>
       </c>
       <c r="J118" s="7" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S118" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="V118" s="2">
         <v>15.273072000000001</v>
@@ -9604,7 +9670,7 @@
         <v>237</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>27</v>
@@ -9618,11 +9684,14 @@
       <c r="K119" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="L119" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S119" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="V119" s="2">
         <v>15.348732999999999</v>
@@ -9645,10 +9714,10 @@
         <v>7</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>327</v>
+        <v>250</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>27</v>
@@ -9657,16 +9726,19 @@
         <v>4</v>
       </c>
       <c r="J120" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="K120" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="K120" s="1" t="s">
-        <v>328</v>
+      <c r="L120" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S120" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="V120" s="2">
         <v>13.861846</v>
@@ -9689,10 +9761,10 @@
         <v>7</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>327</v>
+        <v>250</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>27</v>
@@ -9701,16 +9773,19 @@
         <v>4</v>
       </c>
       <c r="J121" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="K121" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="K121" s="1" t="s">
-        <v>328</v>
+      <c r="L121" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S121" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="V121" s="2">
         <v>13.865371</v>
@@ -9736,16 +9811,19 @@
         <v>161</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="L122" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S122" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="V122" s="2">
         <v>14.985823</v>
@@ -9780,16 +9858,19 @@
         <v>11</v>
       </c>
       <c r="J123" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
+      </c>
+      <c r="L123" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S123" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="V123" s="2">
         <v>15.065429</v>
@@ -9820,11 +9901,14 @@
       <c r="H124" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="L124" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S124" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="V124" s="2">
         <v>15.108616</v>
@@ -9859,16 +9943,19 @@
         <v>1</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="L125" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S125" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="V125" s="2">
         <v>15.137855999999999</v>
@@ -9903,16 +9990,19 @@
         <v>1</v>
       </c>
       <c r="J126" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="L126" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S126" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="V126" s="2">
         <v>15.137337</v>
@@ -9943,11 +10033,14 @@
       <c r="H127" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="L127" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S127" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="V127" s="2">
         <v>15.276194</v>
@@ -9982,16 +10075,19 @@
         <v>13</v>
       </c>
       <c r="J128" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S128" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="V128" s="2">
         <v>14.780340000000001</v>
@@ -10026,16 +10122,19 @@
         <v>22</v>
       </c>
       <c r="J129" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S129" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="V129" s="2">
         <v>14.329539</v>
@@ -10070,16 +10169,19 @@
         <v>6</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
+      </c>
+      <c r="L130" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S130" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="V130" s="2">
         <v>14.126211</v>
@@ -10110,6 +10212,9 @@
       <c r="H131" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="L131" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S131" s="1" t="s">
         <v>36</v>
       </c>
@@ -10137,10 +10242,10 @@
         <v>17</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>27</v>
@@ -10154,6 +10259,9 @@
       <c r="K132" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="L132" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S132" s="1" t="s">
         <v>72</v>
       </c>
@@ -10181,10 +10289,10 @@
         <v>17</v>
       </c>
       <c r="F133" s="7" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>27</v>
@@ -10198,6 +10306,9 @@
       <c r="K133" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="L133" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S133" s="1" t="s">
         <v>179</v>
       </c>
@@ -10225,10 +10336,10 @@
         <v>17</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>27</v>
@@ -10242,6 +10353,9 @@
       <c r="K134" s="1" t="s">
         <v>357</v>
       </c>
+      <c r="L134" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="S134" s="1" t="s">
         <v>36</v>
       </c>
@@ -10269,10 +10383,10 @@
         <v>17</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>27</v>
@@ -10285,6 +10399,9 @@
       </c>
       <c r="K135" s="1" t="s">
         <v>360</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="S135" s="1" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-11-2020 20-46-11
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="756" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{79201995-0D06-4727-B7F9-DF366F1F47F5}"/>
+  <xr:revisionPtr revIDLastSave="843" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA9E8751-C9A3-43D5-A9FE-6822D5740C1F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$139</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$145</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="369">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -1092,9 +1092,6 @@
     <t>Hospital del Sur Dr. Lempira</t>
   </si>
   <si>
-    <t>1701</t>
-  </si>
-  <si>
     <t>Nacaome</t>
   </si>
   <si>
@@ -1104,22 +1101,46 @@
     <t>Centro Médico Juárez</t>
   </si>
   <si>
-    <t>1707</t>
-  </si>
-  <si>
     <t>Langue</t>
   </si>
   <si>
     <t>Centro de Salud de Langue</t>
   </si>
   <si>
-    <t>1706</t>
-  </si>
-  <si>
     <t>Goascorán</t>
   </si>
   <si>
     <t>Medicenter</t>
+  </si>
+  <si>
+    <t>Guanaja</t>
+  </si>
+  <si>
+    <t>HND-1102</t>
+  </si>
+  <si>
+    <t>Cesamo</t>
+  </si>
+  <si>
+    <t>Sabana Bay</t>
+  </si>
+  <si>
+    <t>José Santos Guardiola</t>
+  </si>
+  <si>
+    <t>Oak Ridge</t>
+  </si>
+  <si>
+    <t>HND-1103</t>
+  </si>
+  <si>
+    <t>San Fernando</t>
+  </si>
+  <si>
+    <t>HND-1410</t>
+  </si>
+  <si>
+    <t>HND-</t>
   </si>
 </sst>
 </file>
@@ -1626,7 +1647,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1636,50 +1657,52 @@
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -1784,8 +1807,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W139" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W139" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W145" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W145" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -2115,11 +2138,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W135"/>
+  <dimension ref="A1:W145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="L2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E86" sqref="E86:F86"/>
+      <pane ySplit="1" topLeftCell="U131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U139" sqref="U139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8671,6 +8694,12 @@
       <c r="L97" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P97" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R97" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S97" s="1" t="s">
         <v>246</v>
       </c>
@@ -8718,6 +8747,12 @@
       <c r="L98" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P98" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R98" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S98" s="1" t="s">
         <v>179</v>
       </c>
@@ -8765,6 +8800,12 @@
       <c r="L99" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S99" s="1" t="s">
         <v>179</v>
       </c>
@@ -8812,6 +8853,12 @@
       <c r="L100" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P100" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R100" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S100" s="1" t="s">
         <v>179</v>
       </c>
@@ -8859,6 +8906,12 @@
       <c r="L101" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P101" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R101" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S101" s="1" t="s">
         <v>72</v>
       </c>
@@ -8906,6 +8959,12 @@
       <c r="L102" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S102" s="1" t="s">
         <v>72</v>
       </c>
@@ -8953,6 +9012,12 @@
       <c r="L103" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P103" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R103" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S103" s="1" t="s">
         <v>297</v>
       </c>
@@ -9000,6 +9065,12 @@
       <c r="L104" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P104" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R104" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S104" s="1" t="s">
         <v>297</v>
       </c>
@@ -9047,6 +9118,12 @@
       <c r="L105" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P105" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S105" s="1" t="s">
         <v>297</v>
       </c>
@@ -9094,6 +9171,12 @@
       <c r="L106" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P106" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S106" s="1" t="s">
         <v>179</v>
       </c>
@@ -9141,6 +9224,12 @@
       <c r="L107" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P107" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R107" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S107" s="1" t="s">
         <v>179</v>
       </c>
@@ -9188,6 +9277,12 @@
       <c r="L108" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P108" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R108" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S108" s="1" t="s">
         <v>179</v>
       </c>
@@ -9235,6 +9330,12 @@
       <c r="L109" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P109" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R109" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S109" s="1" t="s">
         <v>179</v>
       </c>
@@ -9282,6 +9383,12 @@
       <c r="L110" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P110" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R110" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S110" s="1" t="s">
         <v>179</v>
       </c>
@@ -9329,6 +9436,12 @@
       <c r="L111" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P111" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R111" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S111" s="1" t="s">
         <v>179</v>
       </c>
@@ -9376,6 +9489,12 @@
       <c r="L112" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P112" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R112" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S112" s="1" t="s">
         <v>179</v>
       </c>
@@ -9423,6 +9542,12 @@
       <c r="L113" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P113" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S113" s="1" t="s">
         <v>179</v>
       </c>
@@ -9461,6 +9586,12 @@
       <c r="L114" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P114" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S114" s="1" t="s">
         <v>36</v>
       </c>
@@ -9508,6 +9639,12 @@
       <c r="L115" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P115" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R115" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S115" s="1" t="s">
         <v>179</v>
       </c>
@@ -9555,6 +9692,12 @@
       <c r="L116" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P116" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R116" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S116" s="1" t="s">
         <v>72</v>
       </c>
@@ -9593,6 +9736,12 @@
       <c r="L117" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R117" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S117" s="1" t="s">
         <v>179</v>
       </c>
@@ -9640,6 +9789,12 @@
       <c r="L118" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P118" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R118" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S118" s="1" t="s">
         <v>179</v>
       </c>
@@ -9687,6 +9842,12 @@
       <c r="L119" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P119" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R119" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S119" s="1" t="s">
         <v>179</v>
       </c>
@@ -9734,6 +9895,12 @@
       <c r="L120" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P120" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R120" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S120" s="1" t="s">
         <v>179</v>
       </c>
@@ -9781,6 +9948,12 @@
       <c r="L121" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P121" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R121" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S121" s="1" t="s">
         <v>179</v>
       </c>
@@ -9819,6 +9992,12 @@
       <c r="L122" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P122" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R122" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S122" s="1" t="s">
         <v>36</v>
       </c>
@@ -9866,6 +10045,12 @@
       <c r="L123" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P123" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R123" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S123" s="1" t="s">
         <v>36</v>
       </c>
@@ -9904,6 +10089,12 @@
       <c r="L124" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P124" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R124" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S124" s="1" t="s">
         <v>36</v>
       </c>
@@ -9951,6 +10142,12 @@
       <c r="L125" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P125" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R125" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S125" s="1" t="s">
         <v>72</v>
       </c>
@@ -9998,6 +10195,12 @@
       <c r="L126" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P126" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R126" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S126" s="1" t="s">
         <v>179</v>
       </c>
@@ -10036,6 +10239,12 @@
       <c r="L127" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P127" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R127" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S127" s="1" t="s">
         <v>72</v>
       </c>
@@ -10083,6 +10292,12 @@
       <c r="L128" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P128" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R128" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S128" s="1" t="s">
         <v>36</v>
       </c>
@@ -10130,6 +10345,12 @@
       <c r="L129" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P129" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R129" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S129" s="1" t="s">
         <v>36</v>
       </c>
@@ -10177,6 +10398,12 @@
       <c r="L130" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P130" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R130" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S130" s="1" t="s">
         <v>179</v>
       </c>
@@ -10215,6 +10442,12 @@
       <c r="L131" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="P131" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R131" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S131" s="1" t="s">
         <v>36</v>
       </c>
@@ -10253,20 +10486,26 @@
       <c r="I132" s="7">
         <v>1</v>
       </c>
-      <c r="J132" s="7" t="s">
+      <c r="J132" s="9">
+        <v>1701</v>
+      </c>
+      <c r="K132" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="K132" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="L132" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="P132" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R132" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="S132" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="V132" s="2">
         <v>13.530787999999999</v>
@@ -10300,20 +10539,26 @@
       <c r="I133" s="7">
         <v>1</v>
       </c>
-      <c r="J133" s="7" t="s">
+      <c r="J133" s="9">
+        <v>1701</v>
+      </c>
+      <c r="K133" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="K133" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="L133" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="P133" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R133" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="S133" s="1" t="s">
         <v>179</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="V133" s="2">
         <v>13.532709000000001</v>
@@ -10347,20 +10592,26 @@
       <c r="I134" s="7">
         <v>7</v>
       </c>
-      <c r="J134" s="7" t="s">
-        <v>356</v>
+      <c r="J134" s="9">
+        <v>1707</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L134" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="P134" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R134" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="S134" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="V134" s="2">
         <v>13.62003</v>
@@ -10394,26 +10645,484 @@
       <c r="I135" s="7">
         <v>6</v>
       </c>
-      <c r="J135" s="7" t="s">
-        <v>359</v>
+      <c r="J135" s="9">
+        <v>1706</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="L135" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="P135" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R135" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="S135" s="1" t="s">
         <v>72</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="V135" s="2">
         <v>13.610545</v>
       </c>
       <c r="W135" s="2">
         <v>-87.752651</v>
+      </c>
+    </row>
+    <row r="136" spans="2:23" ht="15">
+      <c r="B136" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D136" s="1">
+        <v>3</v>
+      </c>
+      <c r="E136" s="10">
+        <v>11</v>
+      </c>
+      <c r="F136" s="10">
+        <v>11</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I136" s="1">
+        <v>2</v>
+      </c>
+      <c r="J136" s="9">
+        <v>1102</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M136" s="1">
+        <v>1</v>
+      </c>
+      <c r="N136" s="1">
+        <v>110201</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q136" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="R136" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S136" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V136" s="2">
+        <v>16.439831999999999</v>
+      </c>
+      <c r="W136" s="2">
+        <v>-85.887030999999993</v>
+      </c>
+    </row>
+    <row r="137" spans="2:23">
+      <c r="B137" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D137" s="1">
+        <v>3</v>
+      </c>
+      <c r="E137" s="10">
+        <v>11</v>
+      </c>
+      <c r="F137" s="10">
+        <v>11</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I137" s="1">
+        <v>2</v>
+      </c>
+      <c r="J137" s="9">
+        <v>1102</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q137" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="R137" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S137" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V137" s="2">
+        <v>16.484898000000001</v>
+      </c>
+      <c r="W137" s="2">
+        <v>-85.844579999999993</v>
+      </c>
+    </row>
+    <row r="138" spans="2:23">
+      <c r="B138" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D138" s="1">
+        <v>3</v>
+      </c>
+      <c r="E138" s="10">
+        <v>11</v>
+      </c>
+      <c r="F138" s="10">
+        <v>11</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I138" s="10">
+        <v>3</v>
+      </c>
+      <c r="J138" s="10">
+        <v>1103</v>
+      </c>
+      <c r="K138" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M138" s="1">
+        <v>3</v>
+      </c>
+      <c r="N138" s="1">
+        <v>110303</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="P138" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q138" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="R138" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S138" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V138" s="2">
+        <v>16.438224000000002</v>
+      </c>
+      <c r="W138" s="2">
+        <v>-86.146834999999996</v>
+      </c>
+    </row>
+    <row r="139" spans="2:23">
+      <c r="B139" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D139" s="1">
+        <v>3</v>
+      </c>
+      <c r="E139" s="10">
+        <v>14</v>
+      </c>
+      <c r="F139" s="10">
+        <v>14</v>
+      </c>
+      <c r="G139" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I139" s="10">
+        <v>10</v>
+      </c>
+      <c r="J139" s="10">
+        <v>1410</v>
+      </c>
+      <c r="K139" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M139" s="1">
+        <v>1</v>
+      </c>
+      <c r="N139" s="1">
+        <v>141001</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="P139" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q139" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="R139" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S139" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V139" s="2">
+        <v>14.680396999999999</v>
+      </c>
+      <c r="W139" s="2">
+        <v>-89.111785999999995</v>
+      </c>
+    </row>
+    <row r="140" spans="2:23">
+      <c r="B140" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D140" s="1">
+        <v>3</v>
+      </c>
+      <c r="E140" s="10"/>
+      <c r="F140" s="10"/>
+      <c r="G140" s="10"/>
+      <c r="H140" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I140" s="10"/>
+      <c r="J140" s="10"/>
+      <c r="K140" s="10"/>
+      <c r="L140" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P140" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q140" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="R140" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S140" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="141" spans="2:23">
+      <c r="B141" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D141" s="1">
+        <v>3</v>
+      </c>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I141" s="10"/>
+      <c r="J141" s="10"/>
+      <c r="K141" s="10"/>
+      <c r="L141" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P141" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q141" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S141" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="142" spans="2:23">
+      <c r="B142" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D142" s="1">
+        <v>3</v>
+      </c>
+      <c r="E142" s="10"/>
+      <c r="F142" s="10"/>
+      <c r="G142" s="10"/>
+      <c r="H142" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I142" s="10"/>
+      <c r="J142" s="10"/>
+      <c r="K142" s="10"/>
+      <c r="L142" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P142" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q142" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="R142" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S142" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="143" spans="2:23">
+      <c r="B143" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D143" s="1">
+        <v>3</v>
+      </c>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
+      <c r="H143" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I143" s="10"/>
+      <c r="J143" s="10"/>
+      <c r="K143" s="10"/>
+      <c r="L143" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P143" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q143" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="R143" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S143" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="144" spans="2:23">
+      <c r="B144" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D144" s="1">
+        <v>3</v>
+      </c>
+      <c r="E144" s="10"/>
+      <c r="F144" s="10"/>
+      <c r="G144" s="10"/>
+      <c r="H144" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I144" s="10"/>
+      <c r="J144" s="10"/>
+      <c r="K144" s="10"/>
+      <c r="L144" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P144" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q144" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="R144" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S144" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="145" spans="2:19">
+      <c r="B145" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D145" s="1">
+        <v>3</v>
+      </c>
+      <c r="E145" s="10"/>
+      <c r="F145" s="10"/>
+      <c r="G145" s="10"/>
+      <c r="H145" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I145" s="10"/>
+      <c r="J145" s="10"/>
+      <c r="K145" s="10"/>
+      <c r="L145" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P145" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q145" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="R145" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S145" s="1" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-12-2020 08-47-57
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1195" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3A83A47F-7C1E-4275-9EE0-F26CB5F2BF34}"/>
+  <xr:revisionPtr revIDLastSave="1357" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A188120A-4053-41D4-8566-701DDE9CB935}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$173</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2406" uniqueCount="490">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -1362,7 +1362,148 @@
     <t>HND-0510</t>
   </si>
   <si>
-    <t>HND-</t>
+    <t>0203</t>
+  </si>
+  <si>
+    <t>Iriona</t>
+  </si>
+  <si>
+    <t>020309</t>
+  </si>
+  <si>
+    <t>Sangrelaya</t>
+  </si>
+  <si>
+    <t>HND-0203</t>
+  </si>
+  <si>
+    <t>0204</t>
+  </si>
+  <si>
+    <t>Limón</t>
+  </si>
+  <si>
+    <t>020401</t>
+  </si>
+  <si>
+    <t>HND-0204</t>
+  </si>
+  <si>
+    <t>0210</t>
+  </si>
+  <si>
+    <t>Bonito Oriental</t>
+  </si>
+  <si>
+    <t>021001</t>
+  </si>
+  <si>
+    <t>HND-0210</t>
+  </si>
+  <si>
+    <t>0205</t>
+  </si>
+  <si>
+    <t>Sabá</t>
+  </si>
+  <si>
+    <t>020511</t>
+  </si>
+  <si>
+    <t>Elixir</t>
+  </si>
+  <si>
+    <t>HND-0205</t>
+  </si>
+  <si>
+    <t>0320</t>
+  </si>
+  <si>
+    <t>Las Lajas</t>
+  </si>
+  <si>
+    <t>032001</t>
+  </si>
+  <si>
+    <t>HND-0320</t>
+  </si>
+  <si>
+    <t>0321</t>
+  </si>
+  <si>
+    <t>Taulabé</t>
+  </si>
+  <si>
+    <t>032101</t>
+  </si>
+  <si>
+    <t>HND-0321</t>
+  </si>
+  <si>
+    <t>0303</t>
+  </si>
+  <si>
+    <t>El Rosario</t>
+  </si>
+  <si>
+    <t>030301</t>
+  </si>
+  <si>
+    <t>HND-0303</t>
+  </si>
+  <si>
+    <t>0319</t>
+  </si>
+  <si>
+    <t>Villa de San Antonio</t>
+  </si>
+  <si>
+    <t>031901</t>
+  </si>
+  <si>
+    <t>HND-0319</t>
+  </si>
+  <si>
+    <t>Cucuyagua</t>
+  </si>
+  <si>
+    <t>HND-0406</t>
+  </si>
+  <si>
+    <t>Dulce Nombre</t>
+  </si>
+  <si>
+    <t>HND-0408</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>San Nicolas</t>
+  </si>
+  <si>
+    <t>HND-0419</t>
+  </si>
+  <si>
+    <t>Nueva Arcadia</t>
+  </si>
+  <si>
+    <t>041301</t>
+  </si>
+  <si>
+    <t>La Entrada</t>
+  </si>
+  <si>
+    <t>HND-0413</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>041001</t>
+  </si>
+  <si>
+    <t>HND-0410</t>
   </si>
 </sst>
 </file>
@@ -2032,8 +2173,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W161" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W161" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W173" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W173" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -2363,11 +2504,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W161"/>
+  <dimension ref="A1:W173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="U154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W162" sqref="W162"/>
+      <pane ySplit="1" topLeftCell="U162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W174" sqref="W174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -8653,8 +8794,8 @@
       <c r="E93" s="1">
         <v>4</v>
       </c>
-      <c r="F93" s="11">
-        <v>4</v>
+      <c r="F93" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>78</v>
@@ -12495,7 +12636,7 @@
         <v>-87.890918999999997</v>
       </c>
     </row>
-    <row r="161" spans="2:19">
+    <row r="161" spans="2:23">
       <c r="B161" s="1" t="s">
         <v>23</v>
       </c>
@@ -12505,27 +12646,785 @@
       <c r="D161" s="1">
         <v>3</v>
       </c>
-      <c r="E161" s="7"/>
-      <c r="F161" s="10"/>
+      <c r="E161" s="7">
+        <v>2</v>
+      </c>
+      <c r="F161" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="H161" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J161" s="11"/>
+      <c r="I161" s="1">
+        <v>3</v>
+      </c>
+      <c r="J161" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="K161" s="1" t="s">
+        <v>443</v>
+      </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N161" s="11"/>
+      <c r="M161" s="1">
+        <v>9</v>
+      </c>
+      <c r="N161" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="O161" s="1" t="s">
+        <v>445</v>
+      </c>
       <c r="P161" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S161" s="1" t="s">
         <v>361</v>
+      </c>
+      <c r="V161" s="2">
+        <v>15.966279</v>
+      </c>
+      <c r="W161" s="2">
+        <v>-85.096109999999996</v>
+      </c>
+    </row>
+    <row r="162" spans="2:23">
+      <c r="B162" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D162" s="1">
+        <v>3</v>
+      </c>
+      <c r="E162" s="7">
+        <v>2</v>
+      </c>
+      <c r="F162" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I162" s="1">
+        <v>4</v>
+      </c>
+      <c r="J162" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="K162" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="L162" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M162" s="1">
+        <v>1</v>
+      </c>
+      <c r="N162" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="O162" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="P162" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q162" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="R162" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S162" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V162" s="2">
+        <v>15.864474080000001</v>
+      </c>
+      <c r="W162" s="2">
+        <v>-85.506744999999995</v>
+      </c>
+    </row>
+    <row r="163" spans="2:23">
+      <c r="B163" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D163" s="1">
+        <v>3</v>
+      </c>
+      <c r="E163" s="7">
+        <v>2</v>
+      </c>
+      <c r="F163" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I163" s="1">
+        <v>10</v>
+      </c>
+      <c r="J163" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="K163" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="L163" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M163" s="1">
+        <v>1</v>
+      </c>
+      <c r="N163" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="O163" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="P163" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q163" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="R163" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S163" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V163" s="2">
+        <v>15.748343</v>
+      </c>
+      <c r="W163" s="2">
+        <v>-85.735150000000004</v>
+      </c>
+    </row>
+    <row r="164" spans="2:23">
+      <c r="B164" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D164" s="1">
+        <v>3</v>
+      </c>
+      <c r="E164" s="7">
+        <v>2</v>
+      </c>
+      <c r="F164" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I164" s="1">
+        <v>5</v>
+      </c>
+      <c r="J164" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="K164" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="L164" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M164" s="1">
+        <v>11</v>
+      </c>
+      <c r="N164" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="O164" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="P164" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q164" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="R164" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S164" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V164" s="2">
+        <v>15.534311000000001</v>
+      </c>
+      <c r="W164" s="2">
+        <v>-86.273984999999996</v>
+      </c>
+    </row>
+    <row r="165" spans="2:23">
+      <c r="B165" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D165" s="1">
+        <v>3</v>
+      </c>
+      <c r="E165" s="7">
+        <v>3</v>
+      </c>
+      <c r="F165" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I165" s="1">
+        <v>20</v>
+      </c>
+      <c r="J165" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="K165" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="L165" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M165" s="1">
+        <v>1</v>
+      </c>
+      <c r="N165" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="O165" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="P165" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q165" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="R165" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S165" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V165" s="2">
+        <v>14.894002</v>
+      </c>
+      <c r="W165" s="2">
+        <v>-87.579126000000002</v>
+      </c>
+    </row>
+    <row r="166" spans="2:23">
+      <c r="B166" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D166" s="1">
+        <v>3</v>
+      </c>
+      <c r="E166" s="7">
+        <v>3</v>
+      </c>
+      <c r="F166" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I166" s="1">
+        <v>21</v>
+      </c>
+      <c r="J166" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="L166" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M166" s="1">
+        <v>1</v>
+      </c>
+      <c r="N166" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="O166" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P166" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q166" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="R166" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S166" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V166" s="2">
+        <v>14.690765000000001</v>
+      </c>
+      <c r="W166" s="2">
+        <v>-87.965248000000003</v>
+      </c>
+    </row>
+    <row r="167" spans="2:23">
+      <c r="B167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D167" s="1">
+        <v>3</v>
+      </c>
+      <c r="E167" s="7">
+        <v>3</v>
+      </c>
+      <c r="F167" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I167" s="1">
+        <v>3</v>
+      </c>
+      <c r="J167" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="K167" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="L167" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M167" s="1">
+        <v>1</v>
+      </c>
+      <c r="N167" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="O167" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="P167" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q167" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="R167" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S167" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V167" s="2">
+        <v>14.575887</v>
+      </c>
+      <c r="W167" s="2">
+        <v>-87.728960000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="2:23">
+      <c r="B168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D168" s="1">
+        <v>3</v>
+      </c>
+      <c r="E168" s="7">
+        <v>3</v>
+      </c>
+      <c r="F168" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I168" s="1">
+        <v>19</v>
+      </c>
+      <c r="J168" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="K168" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="L168" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M168" s="1">
+        <v>1</v>
+      </c>
+      <c r="N168" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="O168" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="P168" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q168" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="R168" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S168" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V168" s="2">
+        <v>14.323912999999999</v>
+      </c>
+      <c r="W168" s="2">
+        <v>-87.613690000000005</v>
+      </c>
+    </row>
+    <row r="169" spans="2:23">
+      <c r="B169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D169" s="1">
+        <v>3</v>
+      </c>
+      <c r="E169" s="7">
+        <v>4</v>
+      </c>
+      <c r="F169" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I169" s="1">
+        <v>6</v>
+      </c>
+      <c r="J169" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K169" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="L169" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N169" s="11"/>
+      <c r="O169" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="P169" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q169" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="R169" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S169" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V169" s="2">
+        <v>14.645818</v>
+      </c>
+      <c r="W169" s="2">
+        <v>-88.873898999999994</v>
+      </c>
+    </row>
+    <row r="170" spans="2:23">
+      <c r="B170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D170" s="1">
+        <v>3</v>
+      </c>
+      <c r="E170" s="7">
+        <v>4</v>
+      </c>
+      <c r="F170" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I170" s="1">
+        <v>8</v>
+      </c>
+      <c r="J170" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="L170" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N170" s="11"/>
+      <c r="O170" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="P170" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q170" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="R170" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S170" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V170" s="2">
+        <v>14.845943</v>
+      </c>
+      <c r="W170" s="2">
+        <v>-88.831519999999998</v>
+      </c>
+    </row>
+    <row r="171" spans="2:23">
+      <c r="B171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D171" s="1">
+        <v>3</v>
+      </c>
+      <c r="E171" s="7">
+        <v>4</v>
+      </c>
+      <c r="F171" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I171" s="1">
+        <v>19</v>
+      </c>
+      <c r="J171" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="K171" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="L171" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N171" s="11"/>
+      <c r="O171" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="P171" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q171" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="R171" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S171" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V171" s="2">
+        <v>15.001557999999999</v>
+      </c>
+      <c r="W171" s="2">
+        <v>-88.751771000000005</v>
+      </c>
+    </row>
+    <row r="172" spans="2:23">
+      <c r="B172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D172" s="1">
+        <v>3</v>
+      </c>
+      <c r="E172" s="7">
+        <v>4</v>
+      </c>
+      <c r="F172" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I172" s="1">
+        <v>13</v>
+      </c>
+      <c r="J172" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="L172" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M172" s="1">
+        <v>1</v>
+      </c>
+      <c r="N172" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="O172" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="P172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q172" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="R172" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S172" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V172" s="2">
+        <v>15.061814</v>
+      </c>
+      <c r="W172" s="2">
+        <v>-88.746099000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="2:23">
+      <c r="B173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D173" s="1">
+        <v>3</v>
+      </c>
+      <c r="E173" s="7">
+        <v>4</v>
+      </c>
+      <c r="F173" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I173" s="1">
+        <v>10</v>
+      </c>
+      <c r="J173" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="K173" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="L173" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M173" s="1">
+        <v>1</v>
+      </c>
+      <c r="N173" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="O173" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="P173" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q173" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="R173" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S173" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="V173" s="2">
+        <v>15.024939</v>
+      </c>
+      <c r="W173" s="2">
+        <v>-88.835689000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-12-2020 21-49-12
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1549" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7DC51802-B862-4593-8830-0CEA0063C6BD}"/>
+  <xr:revisionPtr revIDLastSave="1713" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{318E6431-4DD6-499D-8600-711C45D284FB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$194</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$196</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="601">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -894,6 +894,9 @@
     <t xml:space="preserve">Puerto Lempira </t>
   </si>
   <si>
+    <t>HND-0901</t>
+  </si>
+  <si>
     <t>Hospital Puerto Lempira</t>
   </si>
   <si>
@@ -903,6 +906,9 @@
     <t>Juticalpa</t>
   </si>
   <si>
+    <t>HND-1501</t>
+  </si>
+  <si>
     <t>Hospital San Francisco</t>
   </si>
   <si>
@@ -915,6 +921,9 @@
     <t>Catacamas</t>
   </si>
   <si>
+    <t>HND-1503</t>
+  </si>
+  <si>
     <t>Hospital y Clínica Campos</t>
   </si>
   <si>
@@ -927,6 +936,9 @@
     <t>Guajiquiro</t>
   </si>
   <si>
+    <t>HND-1206</t>
+  </si>
+  <si>
     <t xml:space="preserve">centro de salud </t>
   </si>
   <si>
@@ -939,6 +951,9 @@
     <t>Marcala</t>
   </si>
   <si>
+    <t>HND-1208</t>
+  </si>
+  <si>
     <t>Centro de Salud Marcala</t>
   </si>
   <si>
@@ -948,9 +963,15 @@
     <t>San José</t>
   </si>
   <si>
+    <t>HND-1212</t>
+  </si>
+  <si>
     <t>1201</t>
   </si>
   <si>
+    <t>HND-1201</t>
+  </si>
+  <si>
     <t>Hospital Montecillos</t>
   </si>
   <si>
@@ -960,9 +981,15 @@
     <t>0301</t>
   </si>
   <si>
+    <t>HND-0301</t>
+  </si>
+  <si>
     <t>Hospital Regional Santa Teresa</t>
   </si>
   <si>
+    <t>HND0301</t>
+  </si>
+  <si>
     <t>Hospital del Valle</t>
   </si>
   <si>
@@ -975,6 +1002,9 @@
     <t>La Esperanza</t>
   </si>
   <si>
+    <t>HND-1001</t>
+  </si>
+  <si>
     <t>Hospital Enrique Aguila Cerrato</t>
   </si>
   <si>
@@ -984,6 +1014,9 @@
     <t>Tela</t>
   </si>
   <si>
+    <t>HND-0107</t>
+  </si>
+  <si>
     <t>Hospital Tela Integrado</t>
   </si>
   <si>
@@ -996,6 +1029,9 @@
     <t>1601</t>
   </si>
   <si>
+    <t>HND-1601</t>
+  </si>
+  <si>
     <t>Hospital Santa Barbará Integrado</t>
   </si>
   <si>
@@ -1005,6 +1041,9 @@
     <t>Trinidad</t>
   </si>
   <si>
+    <t>HND-1626</t>
+  </si>
+  <si>
     <t>Clínica de Emergencia Trinidad</t>
   </si>
   <si>
@@ -1017,6 +1056,9 @@
     <t>Petoa</t>
   </si>
   <si>
+    <t>HND-1615</t>
+  </si>
+  <si>
     <t>Hospital Luz de Vida</t>
   </si>
   <si>
@@ -1029,6 +1071,9 @@
     <t>0704</t>
   </si>
   <si>
+    <t>HND-0704</t>
+  </si>
+  <si>
     <t>Centro Médico San Francisco</t>
   </si>
   <si>
@@ -1047,6 +1092,9 @@
     <t>Yorito</t>
   </si>
   <si>
+    <t>HND-1811</t>
+  </si>
+  <si>
     <t>Centro de Salud Yorito</t>
   </si>
   <si>
@@ -1056,6 +1104,9 @@
     <t>1801</t>
   </si>
   <si>
+    <t>HND-1801</t>
+  </si>
+  <si>
     <t>Clínica Médica Dra. Chávez</t>
   </si>
   <si>
@@ -1071,6 +1122,9 @@
     <t>Lepaera</t>
   </si>
   <si>
+    <t>HND-1313</t>
+  </si>
+  <si>
     <t>Centro de Salud Lepaera</t>
   </si>
   <si>
@@ -1080,6 +1134,9 @@
     <t>Santa Cruz</t>
   </si>
   <si>
+    <t>HND-1322</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cesamo de Santa Cruz </t>
   </si>
   <si>
@@ -1089,12 +1146,18 @@
     <t>Gualcinse</t>
   </si>
   <si>
+    <t>HND-1306</t>
+  </si>
+  <si>
     <t>Hospital del Sur Dr. Lempira</t>
   </si>
   <si>
     <t>Nacaome</t>
   </si>
   <si>
+    <t>HND-1701</t>
+  </si>
+  <si>
     <t>Policlínica Nacaome</t>
   </si>
   <si>
@@ -1104,12 +1167,18 @@
     <t>Langue</t>
   </si>
   <si>
+    <t>HND-1707</t>
+  </si>
+  <si>
     <t>Centro de Salud de Langue</t>
   </si>
   <si>
     <t>Goascorán</t>
   </si>
   <si>
+    <t>HND-1706</t>
+  </si>
+  <si>
     <t>Medicenter</t>
   </si>
   <si>
@@ -1633,6 +1702,138 @@
   </si>
   <si>
     <t>San Ignacio</t>
+  </si>
+  <si>
+    <t>081901</t>
+  </si>
+  <si>
+    <t>HND-0819</t>
+  </si>
+  <si>
+    <t>0803</t>
+  </si>
+  <si>
+    <t>Cedros</t>
+  </si>
+  <si>
+    <t>080301</t>
+  </si>
+  <si>
+    <t>HND-0803</t>
+  </si>
+  <si>
+    <t>0902</t>
+  </si>
+  <si>
+    <t>Brus Laguna</t>
+  </si>
+  <si>
+    <t>090204</t>
+  </si>
+  <si>
+    <t>Cocobila</t>
+  </si>
+  <si>
+    <t>HND-0902</t>
+  </si>
+  <si>
+    <t>090202</t>
+  </si>
+  <si>
+    <t>Barra del Patuca</t>
+  </si>
+  <si>
+    <t>0903</t>
+  </si>
+  <si>
+    <t>Ahuas</t>
+  </si>
+  <si>
+    <t>090332</t>
+  </si>
+  <si>
+    <t>Bank-Raya</t>
+  </si>
+  <si>
+    <t>HND-0903</t>
+  </si>
+  <si>
+    <t>0904</t>
+  </si>
+  <si>
+    <t>Juan Francisco Bulnes</t>
+  </si>
+  <si>
+    <t>090407</t>
+  </si>
+  <si>
+    <t>Kraos-Sirpe</t>
+  </si>
+  <si>
+    <t>HND-0904</t>
+  </si>
+  <si>
+    <t>1517</t>
+  </si>
+  <si>
+    <t>San Esteban</t>
+  </si>
+  <si>
+    <t>151719</t>
+  </si>
+  <si>
+    <t>San Martin</t>
+  </si>
+  <si>
+    <t>HND-1517</t>
+  </si>
+  <si>
+    <t>1510</t>
+  </si>
+  <si>
+    <t>Guata</t>
+  </si>
+  <si>
+    <t>151001</t>
+  </si>
+  <si>
+    <t>HND-1510</t>
+  </si>
+  <si>
+    <t>1514</t>
+  </si>
+  <si>
+    <t>Manguile</t>
+  </si>
+  <si>
+    <t>151401</t>
+  </si>
+  <si>
+    <t>HND-1514</t>
+  </si>
+  <si>
+    <t>1512</t>
+  </si>
+  <si>
+    <t>Jano</t>
+  </si>
+  <si>
+    <t>151201</t>
+  </si>
+  <si>
+    <t>HND-1512</t>
+  </si>
+  <si>
+    <t>1518</t>
+  </si>
+  <si>
+    <t>San Francisco de Becerra</t>
+  </si>
+  <si>
+    <t>151801</t>
+  </si>
+  <si>
+    <t>HND-1518</t>
   </si>
   <si>
     <t>HND-</t>
@@ -2159,48 +2360,48 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -2305,8 +2506,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W194" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W194" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W196" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W196" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -2636,11 +2837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W194"/>
+  <dimension ref="A1:W196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="K175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N184" sqref="N184"/>
+      <pane ySplit="1" topLeftCell="G106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K114" sqref="K114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -2659,7 +2860,7 @@
     <col min="12" max="12" width="12.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.5703125" style="1" customWidth="1"/>
     <col min="16" max="16" width="20.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="15" style="1" customWidth="1"/>
     <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
@@ -9203,6 +9404,9 @@
       <c r="P97" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q97" s="1" t="s">
+        <v>286</v>
+      </c>
       <c r="R97" s="1" t="s">
         <v>35</v>
       </c>
@@ -9210,7 +9414,7 @@
         <v>246</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="V97" s="2">
         <v>15.265726000000001</v>
@@ -9245,10 +9449,10 @@
         <v>1</v>
       </c>
       <c r="J98" s="10" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L98" s="1" t="s">
         <v>30</v>
@@ -9257,6 +9461,9 @@
       <c r="P98" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q98" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="R98" s="1" t="s">
         <v>35</v>
       </c>
@@ -9264,7 +9471,7 @@
         <v>179</v>
       </c>
       <c r="U98" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="V98" s="2">
         <v>14.665319</v>
@@ -9299,10 +9506,10 @@
         <v>1</v>
       </c>
       <c r="J99" s="10" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L99" s="1" t="s">
         <v>30</v>
@@ -9311,6 +9518,9 @@
       <c r="P99" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q99" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="R99" s="1" t="s">
         <v>35</v>
       </c>
@@ -9318,7 +9528,7 @@
         <v>179</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="V99" s="2">
         <v>14.671486</v>
@@ -9353,10 +9563,10 @@
         <v>3</v>
       </c>
       <c r="J100" s="10" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L100" s="1" t="s">
         <v>30</v>
@@ -9365,6 +9575,9 @@
       <c r="P100" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q100" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="R100" s="1" t="s">
         <v>35</v>
       </c>
@@ -9372,7 +9585,7 @@
         <v>179</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="V100" s="2">
         <v>14.853908000000001</v>
@@ -9407,10 +9620,10 @@
         <v>3</v>
       </c>
       <c r="J101" s="10" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L101" s="1" t="s">
         <v>30</v>
@@ -9419,6 +9632,9 @@
       <c r="P101" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q101" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="R101" s="1" t="s">
         <v>35</v>
       </c>
@@ -9426,7 +9642,7 @@
         <v>72</v>
       </c>
       <c r="U101" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="V101" s="2">
         <v>14.851229</v>
@@ -9461,10 +9677,10 @@
         <v>3</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L102" s="1" t="s">
         <v>30</v>
@@ -9473,6 +9689,9 @@
       <c r="P102" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q102" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="R102" s="1" t="s">
         <v>35</v>
       </c>
@@ -9515,10 +9734,10 @@
         <v>6</v>
       </c>
       <c r="J103" s="10" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="L103" s="1" t="s">
         <v>30</v>
@@ -9527,14 +9746,17 @@
       <c r="P103" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q103" s="1" t="s">
+        <v>300</v>
+      </c>
       <c r="R103" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="V103" s="2">
         <v>14.120423000000001</v>
@@ -9569,10 +9791,10 @@
         <v>8</v>
       </c>
       <c r="J104" s="10" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="L104" s="1" t="s">
         <v>30</v>
@@ -9581,14 +9803,17 @@
       <c r="P104" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q104" s="1" t="s">
+        <v>305</v>
+      </c>
       <c r="R104" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="V104" s="2">
         <v>14.159074</v>
@@ -9623,10 +9848,10 @@
         <v>12</v>
       </c>
       <c r="J105" s="10" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="L105" s="1" t="s">
         <v>30</v>
@@ -9635,11 +9860,14 @@
       <c r="P105" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q105" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="R105" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S105" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>44</v>
@@ -9677,7 +9905,7 @@
         <v>1</v>
       </c>
       <c r="J106" s="10" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>63</v>
@@ -9689,6 +9917,9 @@
       <c r="P106" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q106" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="R106" s="1" t="s">
         <v>35</v>
       </c>
@@ -9696,7 +9927,7 @@
         <v>179</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="V106" s="2">
         <v>14.319006</v>
@@ -9731,7 +9962,7 @@
         <v>1</v>
       </c>
       <c r="J107" s="10" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>63</v>
@@ -9743,6 +9974,9 @@
       <c r="P107" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q107" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="R107" s="1" t="s">
         <v>35</v>
       </c>
@@ -9750,7 +9984,7 @@
         <v>179</v>
       </c>
       <c r="U107" s="1" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="V107" s="2">
         <v>14.322329999999999</v>
@@ -9785,7 +10019,7 @@
         <v>1</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>189</v>
@@ -9797,6 +10031,9 @@
       <c r="P108" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q108" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="R108" s="1" t="s">
         <v>35</v>
       </c>
@@ -9804,7 +10041,7 @@
         <v>179</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="V108" s="2">
         <v>14.453317999999999</v>
@@ -9839,7 +10076,7 @@
         <v>1</v>
       </c>
       <c r="J109" s="10" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>189</v>
@@ -9851,6 +10088,9 @@
       <c r="P109" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q109" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="R109" s="1" t="s">
         <v>35</v>
       </c>
@@ -9858,7 +10098,7 @@
         <v>179</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="V109" s="2">
         <v>14.456941</v>
@@ -9893,7 +10133,7 @@
         <v>1</v>
       </c>
       <c r="J110" s="10" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>189</v>
@@ -9905,6 +10145,9 @@
       <c r="P110" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q110" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="R110" s="1" t="s">
         <v>35</v>
       </c>
@@ -9912,7 +10155,7 @@
         <v>179</v>
       </c>
       <c r="U110" s="1" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="V110" s="2">
         <v>14.460008999999999</v>
@@ -9959,6 +10202,9 @@
       <c r="P111" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q111" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="R111" s="1" t="s">
         <v>35</v>
       </c>
@@ -10001,10 +10247,10 @@
         <v>1</v>
       </c>
       <c r="J112" s="10" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="L112" s="1" t="s">
         <v>30</v>
@@ -10013,6 +10259,9 @@
       <c r="P112" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q112" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="R112" s="1" t="s">
         <v>35</v>
       </c>
@@ -10020,7 +10269,7 @@
         <v>179</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="V112" s="2">
         <v>14.314704000000001</v>
@@ -10055,10 +10304,10 @@
         <v>7</v>
       </c>
       <c r="J113" s="10" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="L113" s="1" t="s">
         <v>30</v>
@@ -10067,6 +10316,9 @@
       <c r="P113" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q113" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="R113" s="1" t="s">
         <v>35</v>
       </c>
@@ -10074,7 +10326,7 @@
         <v>179</v>
       </c>
       <c r="U113" s="1" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="V113" s="2">
         <v>15.754151999999999</v>
@@ -10120,7 +10372,7 @@
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="V114" s="2">
         <v>15.908462</v>
@@ -10146,7 +10398,7 @@
         <v>237</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>27</v>
@@ -10155,10 +10407,10 @@
         <v>1</v>
       </c>
       <c r="J115" s="10" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="L115" s="1" t="s">
         <v>30</v>
@@ -10167,6 +10419,9 @@
       <c r="P115" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q115" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="R115" s="1" t="s">
         <v>35</v>
       </c>
@@ -10174,7 +10429,7 @@
         <v>179</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="V115" s="2">
         <v>14.925007000000001</v>
@@ -10200,7 +10455,7 @@
         <v>237</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>27</v>
@@ -10209,10 +10464,10 @@
         <v>26</v>
       </c>
       <c r="J116" s="10" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="L116" s="1" t="s">
         <v>30</v>
@@ -10221,6 +10476,9 @@
       <c r="P116" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q116" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="R116" s="1" t="s">
         <v>35</v>
       </c>
@@ -10228,7 +10486,7 @@
         <v>72</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="V116" s="2">
         <v>15.143121000000001</v>
@@ -10254,7 +10512,7 @@
         <v>237</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>27</v>
@@ -10274,7 +10532,7 @@
         <v>179</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="V117" s="2">
         <v>15.247275</v>
@@ -10300,7 +10558,7 @@
         <v>237</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>27</v>
@@ -10309,10 +10567,10 @@
         <v>15</v>
       </c>
       <c r="J118" s="10" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="L118" s="1" t="s">
         <v>30</v>
@@ -10321,6 +10579,9 @@
       <c r="P118" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q118" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="R118" s="1" t="s">
         <v>35</v>
       </c>
@@ -10328,7 +10589,7 @@
         <v>179</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="V118" s="2">
         <v>15.273072000000001</v>
@@ -10354,7 +10615,7 @@
         <v>237</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>27</v>
@@ -10375,6 +10636,9 @@
       <c r="P119" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q119" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="R119" s="1" t="s">
         <v>35</v>
       </c>
@@ -10382,7 +10646,7 @@
         <v>179</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>328</v>
+        <v>342</v>
       </c>
       <c r="V119" s="2">
         <v>15.348732999999999</v>
@@ -10408,7 +10672,7 @@
         <v>250</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>27</v>
@@ -10417,10 +10681,10 @@
         <v>4</v>
       </c>
       <c r="J120" s="10" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="L120" s="1" t="s">
         <v>30</v>
@@ -10429,6 +10693,9 @@
       <c r="P120" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q120" s="1" t="s">
+        <v>345</v>
+      </c>
       <c r="R120" s="1" t="s">
         <v>35</v>
       </c>
@@ -10436,7 +10703,7 @@
         <v>179</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="V120" s="2">
         <v>13.861846</v>
@@ -10462,7 +10729,7 @@
         <v>250</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>27</v>
@@ -10471,10 +10738,10 @@
         <v>4</v>
       </c>
       <c r="J121" s="10" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="L121" s="1" t="s">
         <v>30</v>
@@ -10483,6 +10750,9 @@
       <c r="P121" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q121" s="1" t="s">
+        <v>345</v>
+      </c>
       <c r="R121" s="1" t="s">
         <v>35</v>
       </c>
@@ -10490,7 +10760,7 @@
         <v>179</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="V121" s="2">
         <v>13.865371</v>
@@ -10516,7 +10786,7 @@
         <v>161</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>27</v>
@@ -10536,7 +10806,7 @@
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="V122" s="2">
         <v>14.985823</v>
@@ -10571,10 +10841,10 @@
         <v>11</v>
       </c>
       <c r="J123" s="13" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="L123" s="1" t="s">
         <v>30</v>
@@ -10583,6 +10853,9 @@
       <c r="P123" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q123" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="R123" s="1" t="s">
         <v>35</v>
       </c>
@@ -10590,7 +10863,7 @@
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>337</v>
+        <v>353</v>
       </c>
       <c r="V123" s="2">
         <v>15.065429</v>
@@ -10636,7 +10909,7 @@
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>338</v>
+        <v>354</v>
       </c>
       <c r="V124" s="2">
         <v>15.108616</v>
@@ -10671,7 +10944,7 @@
         <v>1</v>
       </c>
       <c r="J125" s="10" t="s">
-        <v>339</v>
+        <v>355</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>162</v>
@@ -10683,6 +10956,9 @@
       <c r="P125" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q125" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="R125" s="1" t="s">
         <v>35</v>
       </c>
@@ -10690,7 +10966,7 @@
         <v>72</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="V125" s="2">
         <v>15.137855999999999</v>
@@ -10725,7 +11001,7 @@
         <v>1</v>
       </c>
       <c r="J126" s="10" t="s">
-        <v>339</v>
+        <v>355</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>162</v>
@@ -10737,6 +11013,9 @@
       <c r="P126" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q126" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="R126" s="1" t="s">
         <v>35</v>
       </c>
@@ -10744,7 +11023,7 @@
         <v>179</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>341</v>
+        <v>358</v>
       </c>
       <c r="V126" s="2">
         <v>15.137337</v>
@@ -10790,7 +11069,7 @@
         <v>72</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="V127" s="2">
         <v>15.276194</v>
@@ -10825,10 +11104,10 @@
         <v>13</v>
       </c>
       <c r="J128" s="10" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>344</v>
+        <v>361</v>
       </c>
       <c r="L128" s="1" t="s">
         <v>30</v>
@@ -10837,6 +11116,9 @@
       <c r="P128" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q128" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="R128" s="1" t="s">
         <v>35</v>
       </c>
@@ -10844,7 +11126,7 @@
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>345</v>
+        <v>363</v>
       </c>
       <c r="V128" s="2">
         <v>14.780340000000001</v>
@@ -10879,10 +11161,10 @@
         <v>22</v>
       </c>
       <c r="J129" s="10" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>347</v>
+        <v>365</v>
       </c>
       <c r="L129" s="1" t="s">
         <v>30</v>
@@ -10891,6 +11173,9 @@
       <c r="P129" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q129" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="R129" s="1" t="s">
         <v>35</v>
       </c>
@@ -10898,7 +11183,7 @@
         <v>36</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>348</v>
+        <v>367</v>
       </c>
       <c r="V129" s="2">
         <v>14.329539</v>
@@ -10933,10 +11218,10 @@
         <v>6</v>
       </c>
       <c r="J130" s="10" t="s">
-        <v>349</v>
+        <v>368</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
       <c r="L130" s="1" t="s">
         <v>30</v>
@@ -10945,6 +11230,9 @@
       <c r="P130" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q130" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="R130" s="1" t="s">
         <v>35</v>
       </c>
@@ -10952,7 +11240,7 @@
         <v>179</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="V130" s="2">
         <v>14.126211</v>
@@ -11036,7 +11324,7 @@
         <v>1701</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>30</v>
@@ -11045,6 +11333,9 @@
       <c r="P132" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q132" s="1" t="s">
+        <v>373</v>
+      </c>
       <c r="R132" s="1" t="s">
         <v>35</v>
       </c>
@@ -11052,7 +11343,7 @@
         <v>72</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
       <c r="V132" s="2">
         <v>13.530787999999999</v>
@@ -11090,7 +11381,7 @@
         <v>1701</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="L133" s="1" t="s">
         <v>30</v>
@@ -11099,6 +11390,9 @@
       <c r="P133" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q133" s="1" t="s">
+        <v>373</v>
+      </c>
       <c r="R133" s="1" t="s">
         <v>35</v>
       </c>
@@ -11106,7 +11400,7 @@
         <v>179</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>354</v>
+        <v>375</v>
       </c>
       <c r="V133" s="2">
         <v>13.532709000000001</v>
@@ -11144,7 +11438,7 @@
         <v>1707</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="L134" s="1" t="s">
         <v>30</v>
@@ -11153,6 +11447,9 @@
       <c r="P134" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q134" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="R134" s="1" t="s">
         <v>35</v>
       </c>
@@ -11160,7 +11457,7 @@
         <v>36</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>356</v>
+        <v>378</v>
       </c>
       <c r="V134" s="2">
         <v>13.62003</v>
@@ -11198,7 +11495,7 @@
         <v>1706</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
       <c r="L135" s="1" t="s">
         <v>30</v>
@@ -11207,6 +11504,9 @@
       <c r="P135" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q135" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="R135" s="1" t="s">
         <v>35</v>
       </c>
@@ -11214,7 +11514,7 @@
         <v>72</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>358</v>
+        <v>381</v>
       </c>
       <c r="V135" s="2">
         <v>13.610545</v>
@@ -11252,7 +11552,7 @@
         <v>1102</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="L136" s="1" t="s">
         <v>30</v>
@@ -11264,19 +11564,19 @@
         <v>110201</v>
       </c>
       <c r="O136" s="1" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="P136" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q136" s="1" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="R136" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S136" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V136" s="2">
         <v>16.439831999999999</v>
@@ -11314,26 +11614,26 @@
         <v>1102</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="L137" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N137" s="11"/>
       <c r="O137" s="1" t="s">
-        <v>362</v>
+        <v>385</v>
       </c>
       <c r="P137" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q137" s="1" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="R137" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S137" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V137" s="2">
         <v>16.484898000000001</v>
@@ -11371,7 +11671,7 @@
         <v>1103</v>
       </c>
       <c r="K138" s="9" t="s">
-        <v>363</v>
+        <v>386</v>
       </c>
       <c r="L138" s="1" t="s">
         <v>30</v>
@@ -11383,19 +11683,19 @@
         <v>110303</v>
       </c>
       <c r="O138" s="1" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
       <c r="P138" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q138" s="1" t="s">
-        <v>365</v>
+        <v>388</v>
       </c>
       <c r="R138" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S138" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V138" s="2">
         <v>16.438224000000002</v>
@@ -11433,7 +11733,7 @@
         <v>1410</v>
       </c>
       <c r="K139" s="9" t="s">
-        <v>366</v>
+        <v>389</v>
       </c>
       <c r="L139" s="1" t="s">
         <v>30</v>
@@ -11445,19 +11745,19 @@
         <v>141001</v>
       </c>
       <c r="O139" s="1" t="s">
-        <v>366</v>
+        <v>389</v>
       </c>
       <c r="P139" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q139" s="1" t="s">
-        <v>367</v>
+        <v>390</v>
       </c>
       <c r="R139" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S139" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V139" s="2">
         <v>14.680396999999999</v>
@@ -11495,7 +11795,7 @@
         <v>1406</v>
       </c>
       <c r="K140" s="9" t="s">
-        <v>368</v>
+        <v>391</v>
       </c>
       <c r="L140" s="1" t="s">
         <v>30</v>
@@ -11507,19 +11807,19 @@
         <v>140603</v>
       </c>
       <c r="O140" s="1" t="s">
-        <v>368</v>
+        <v>391</v>
       </c>
       <c r="P140" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q140" s="1" t="s">
-        <v>369</v>
+        <v>392</v>
       </c>
       <c r="R140" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S140" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V140" s="2">
         <v>14.664014</v>
@@ -11557,7 +11857,7 @@
         <v>1415</v>
       </c>
       <c r="K141" s="9" t="s">
-        <v>370</v>
+        <v>393</v>
       </c>
       <c r="L141" s="1" t="s">
         <v>30</v>
@@ -11569,19 +11869,19 @@
         <v>141502</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>370</v>
+        <v>393</v>
       </c>
       <c r="P141" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q141" s="1" t="s">
-        <v>371</v>
+        <v>394</v>
       </c>
       <c r="R141" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S141" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V141" s="2">
         <v>14.487455000000001</v>
@@ -11619,7 +11919,7 @@
         <v>1407</v>
       </c>
       <c r="K142" s="9" t="s">
-        <v>372</v>
+        <v>395</v>
       </c>
       <c r="L142" s="1" t="s">
         <v>30</v>
@@ -11631,19 +11931,19 @@
         <v>140701</v>
       </c>
       <c r="O142" s="1" t="s">
-        <v>372</v>
+        <v>395</v>
       </c>
       <c r="P142" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q142" s="1" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="R142" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S142" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V142" s="2">
         <v>14.484342</v>
@@ -11681,7 +11981,7 @@
         <v>1402</v>
       </c>
       <c r="K143" s="9" t="s">
-        <v>374</v>
+        <v>397</v>
       </c>
       <c r="L143" s="1" t="s">
         <v>30</v>
@@ -11693,19 +11993,19 @@
         <v>140201</v>
       </c>
       <c r="O143" s="1" t="s">
-        <v>375</v>
+        <v>398</v>
       </c>
       <c r="P143" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q143" s="1" t="s">
-        <v>376</v>
+        <v>399</v>
       </c>
       <c r="R143" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S143" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V143" s="2">
         <v>14.477974</v>
@@ -11743,7 +12043,7 @@
         <v>1401</v>
       </c>
       <c r="K144" s="9" t="s">
-        <v>377</v>
+        <v>400</v>
       </c>
       <c r="L144" s="1" t="s">
         <v>30</v>
@@ -11755,19 +12055,19 @@
         <v>140101</v>
       </c>
       <c r="O144" s="1" t="s">
-        <v>377</v>
+        <v>400</v>
       </c>
       <c r="P144" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q144" s="1" t="s">
-        <v>378</v>
+        <v>401</v>
       </c>
       <c r="R144" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S144" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V144" s="2">
         <v>14.43247</v>
@@ -11793,7 +12093,7 @@
         <v>250</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>27</v>
@@ -11802,10 +12102,10 @@
         <v>15</v>
       </c>
       <c r="J145" s="11" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>30</v>
@@ -11814,22 +12114,22 @@
         <v>1</v>
       </c>
       <c r="N145" s="11" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="P145" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q145" s="1" t="s">
-        <v>382</v>
+        <v>405</v>
       </c>
       <c r="R145" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S145" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V145" s="2">
         <v>14.225474</v>
@@ -11855,7 +12155,7 @@
         <v>250</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
@@ -11864,34 +12164,34 @@
         <v>8</v>
       </c>
       <c r="J146" s="11" t="s">
-        <v>383</v>
+        <v>406</v>
       </c>
       <c r="K146" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="L146" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M146" s="1">
+        <v>1</v>
+      </c>
+      <c r="N146" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="O146" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="P146" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q146" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="R146" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S146" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="L146" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M146" s="1">
-        <v>1</v>
-      </c>
-      <c r="N146" s="11" t="s">
-        <v>385</v>
-      </c>
-      <c r="O146" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="P146" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q146" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="R146" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S146" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="V146" s="2">
         <v>14.123517</v>
@@ -11917,7 +12217,7 @@
         <v>250</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>27</v>
@@ -11926,10 +12226,10 @@
         <v>19</v>
       </c>
       <c r="J147" s="11" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>388</v>
+        <v>411</v>
       </c>
       <c r="L147" s="1" t="s">
         <v>30</v>
@@ -11938,22 +12238,22 @@
         <v>1</v>
       </c>
       <c r="N147" s="11" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
       <c r="O147" s="1" t="s">
-        <v>388</v>
+        <v>411</v>
       </c>
       <c r="P147" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q147" s="1" t="s">
-        <v>390</v>
+        <v>413</v>
       </c>
       <c r="R147" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S147" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V147" s="2">
         <v>14.081087999999999</v>
@@ -11979,7 +12279,7 @@
         <v>250</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>27</v>
@@ -11988,10 +12288,10 @@
         <v>5</v>
       </c>
       <c r="J148" s="11" t="s">
-        <v>391</v>
+        <v>414</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>392</v>
+        <v>415</v>
       </c>
       <c r="L148" s="1" t="s">
         <v>30</v>
@@ -12000,22 +12300,22 @@
         <v>1</v>
       </c>
       <c r="N148" s="11" t="s">
-        <v>393</v>
+        <v>416</v>
       </c>
       <c r="O148" s="1" t="s">
-        <v>392</v>
+        <v>415</v>
       </c>
       <c r="P148" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q148" s="1" t="s">
-        <v>394</v>
+        <v>417</v>
       </c>
       <c r="R148" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S148" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V148" s="2">
         <v>13.880433</v>
@@ -12041,7 +12341,7 @@
         <v>250</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>27</v>
@@ -12050,10 +12350,10 @@
         <v>16</v>
       </c>
       <c r="J149" s="11" t="s">
-        <v>395</v>
+        <v>418</v>
       </c>
       <c r="K149" s="1" t="s">
-        <v>396</v>
+        <v>419</v>
       </c>
       <c r="L149" s="1" t="s">
         <v>30</v>
@@ -12062,22 +12362,22 @@
         <v>1</v>
       </c>
       <c r="N149" s="11" t="s">
-        <v>397</v>
+        <v>420</v>
       </c>
       <c r="O149" s="1" t="s">
-        <v>396</v>
+        <v>419</v>
       </c>
       <c r="P149" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q149" s="1" t="s">
-        <v>398</v>
+        <v>421</v>
       </c>
       <c r="R149" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S149" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V149" s="2">
         <v>13.648353999999999</v>
@@ -12103,7 +12403,7 @@
         <v>250</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H150" s="1" t="s">
         <v>27</v>
@@ -12112,10 +12412,10 @@
         <v>14</v>
       </c>
       <c r="J150" s="11" t="s">
-        <v>399</v>
+        <v>422</v>
       </c>
       <c r="K150" s="1" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="L150" s="1" t="s">
         <v>30</v>
@@ -12124,22 +12424,22 @@
         <v>1</v>
       </c>
       <c r="N150" s="11" t="s">
-        <v>401</v>
+        <v>424</v>
       </c>
       <c r="O150" s="1" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="P150" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q150" s="1" t="s">
-        <v>402</v>
+        <v>425</v>
       </c>
       <c r="R150" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S150" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V150" s="2">
         <v>13.586309</v>
@@ -12165,7 +12465,7 @@
         <v>250</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="H151" s="1" t="s">
         <v>27</v>
@@ -12174,10 +12474,10 @@
         <v>7</v>
       </c>
       <c r="J151" s="11" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>404</v>
+        <v>427</v>
       </c>
       <c r="L151" s="1" t="s">
         <v>30</v>
@@ -12186,22 +12486,22 @@
         <v>3</v>
       </c>
       <c r="N151" s="11" t="s">
-        <v>405</v>
+        <v>428</v>
       </c>
       <c r="O151" s="1" t="s">
-        <v>404</v>
+        <v>427</v>
       </c>
       <c r="P151" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q151" s="1" t="s">
-        <v>406</v>
+        <v>429</v>
       </c>
       <c r="R151" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S151" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V151" s="2">
         <v>13.541517000000001</v>
@@ -12236,10 +12536,10 @@
         <v>3</v>
       </c>
       <c r="J152" s="11" t="s">
-        <v>407</v>
+        <v>430</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>408</v>
+        <v>431</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>30</v>
@@ -12248,22 +12548,22 @@
         <v>1</v>
       </c>
       <c r="N152" s="11" t="s">
-        <v>409</v>
+        <v>432</v>
       </c>
       <c r="O152" s="1" t="s">
-        <v>408</v>
+        <v>431</v>
       </c>
       <c r="P152" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q152" s="1" t="s">
-        <v>410</v>
+        <v>433</v>
       </c>
       <c r="R152" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S152" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V152" s="2">
         <v>15.774127999999999</v>
@@ -12298,10 +12598,10 @@
         <v>3</v>
       </c>
       <c r="J153" s="11" t="s">
-        <v>407</v>
+        <v>430</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>408</v>
+        <v>431</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>30</v>
@@ -12310,22 +12610,22 @@
         <v>7</v>
       </c>
       <c r="N153" s="11" t="s">
-        <v>411</v>
+        <v>434</v>
       </c>
       <c r="O153" s="1" t="s">
-        <v>412</v>
+        <v>435</v>
       </c>
       <c r="P153" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q153" s="1" t="s">
-        <v>410</v>
+        <v>433</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S153" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V153" s="2">
         <v>15.663361</v>
@@ -12360,10 +12660,10 @@
         <v>2</v>
       </c>
       <c r="J154" s="11" t="s">
-        <v>413</v>
+        <v>436</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>414</v>
+        <v>437</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>30</v>
@@ -12372,22 +12672,22 @@
         <v>1</v>
       </c>
       <c r="N154" s="11" t="s">
-        <v>415</v>
+        <v>438</v>
       </c>
       <c r="O154" s="1" t="s">
-        <v>416</v>
+        <v>439</v>
       </c>
       <c r="P154" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q154" s="1" t="s">
-        <v>417</v>
+        <v>440</v>
       </c>
       <c r="R154" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S154" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V154" s="2">
         <v>15.610602</v>
@@ -12422,10 +12722,10 @@
         <v>12</v>
       </c>
       <c r="J155" s="11" t="s">
-        <v>418</v>
+        <v>441</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>419</v>
+        <v>442</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>30</v>
@@ -12434,22 +12734,22 @@
         <v>1</v>
       </c>
       <c r="N155" s="11" t="s">
-        <v>420</v>
+        <v>443</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>419</v>
+        <v>442</v>
       </c>
       <c r="P155" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q155" s="1" t="s">
-        <v>421</v>
+        <v>444</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S155" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V155" s="2">
         <v>15.439396</v>
@@ -12484,10 +12784,10 @@
         <v>9</v>
       </c>
       <c r="J156" s="11" t="s">
-        <v>422</v>
+        <v>445</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>423</v>
+        <v>446</v>
       </c>
       <c r="L156" s="1" t="s">
         <v>30</v>
@@ -12496,22 +12796,22 @@
         <v>1</v>
       </c>
       <c r="N156" s="11" t="s">
-        <v>424</v>
+        <v>447</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>423</v>
+        <v>446</v>
       </c>
       <c r="P156" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q156" s="1" t="s">
-        <v>425</v>
+        <v>448</v>
       </c>
       <c r="R156" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S156" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V156" s="2">
         <v>15.329428999999999</v>
@@ -12546,10 +12846,10 @@
         <v>11</v>
       </c>
       <c r="J157" s="11" t="s">
-        <v>426</v>
+        <v>449</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>427</v>
+        <v>450</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>30</v>
@@ -12558,22 +12858,22 @@
         <v>1</v>
       </c>
       <c r="N157" s="11" t="s">
-        <v>428</v>
+        <v>451</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>427</v>
+        <v>450</v>
       </c>
       <c r="P157" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q157" s="1" t="s">
-        <v>429</v>
+        <v>452</v>
       </c>
       <c r="R157" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S157" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V157" s="2">
         <v>15.312935</v>
@@ -12608,10 +12908,10 @@
         <v>5</v>
       </c>
       <c r="J158" s="11" t="s">
-        <v>430</v>
+        <v>453</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>431</v>
+        <v>454</v>
       </c>
       <c r="L158" s="1" t="s">
         <v>30</v>
@@ -12620,22 +12920,22 @@
         <v>1</v>
       </c>
       <c r="N158" s="11" t="s">
-        <v>432</v>
+        <v>455</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>431</v>
+        <v>454</v>
       </c>
       <c r="P158" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q158" s="1" t="s">
-        <v>433</v>
+        <v>456</v>
       </c>
       <c r="R158" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S158" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V158" s="2">
         <v>15.228071</v>
@@ -12670,10 +12970,10 @@
         <v>7</v>
       </c>
       <c r="J159" s="11" t="s">
-        <v>434</v>
+        <v>457</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>435</v>
+        <v>458</v>
       </c>
       <c r="L159" s="1" t="s">
         <v>30</v>
@@ -12682,22 +12982,22 @@
         <v>1</v>
       </c>
       <c r="N159" s="11" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>435</v>
+        <v>458</v>
       </c>
       <c r="P159" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q159" s="1" t="s">
-        <v>437</v>
+        <v>460</v>
       </c>
       <c r="R159" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S159" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V159" s="2">
         <v>15.114108</v>
@@ -12732,10 +13032,10 @@
         <v>10</v>
       </c>
       <c r="J160" s="11" t="s">
-        <v>438</v>
+        <v>461</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>439</v>
+        <v>462</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>30</v>
@@ -12744,22 +13044,22 @@
         <v>1</v>
       </c>
       <c r="N160" s="11" t="s">
-        <v>440</v>
+        <v>463</v>
       </c>
       <c r="O160" s="1" t="s">
-        <v>439</v>
+        <v>462</v>
       </c>
       <c r="P160" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q160" s="1" t="s">
-        <v>441</v>
+        <v>464</v>
       </c>
       <c r="R160" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S160" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V160" s="2">
         <v>14.97907</v>
@@ -12794,10 +13094,10 @@
         <v>3</v>
       </c>
       <c r="J161" s="11" t="s">
-        <v>442</v>
+        <v>465</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>443</v>
+        <v>466</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
@@ -12806,22 +13106,22 @@
         <v>9</v>
       </c>
       <c r="N161" s="11" t="s">
-        <v>444</v>
+        <v>467</v>
       </c>
       <c r="O161" s="1" t="s">
-        <v>445</v>
+        <v>468</v>
       </c>
       <c r="P161" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>446</v>
+        <v>469</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S161" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V161" s="2">
         <v>15.966279</v>
@@ -12856,10 +13156,10 @@
         <v>4</v>
       </c>
       <c r="J162" s="11" t="s">
-        <v>447</v>
+        <v>470</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>448</v>
+        <v>471</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>30</v>
@@ -12868,22 +13168,22 @@
         <v>1</v>
       </c>
       <c r="N162" s="11" t="s">
-        <v>449</v>
+        <v>472</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>448</v>
+        <v>471</v>
       </c>
       <c r="P162" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q162" s="1" t="s">
-        <v>450</v>
+        <v>473</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S162" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V162" s="2">
         <v>15.864474080000001</v>
@@ -12918,10 +13218,10 @@
         <v>10</v>
       </c>
       <c r="J163" s="11" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>452</v>
+        <v>475</v>
       </c>
       <c r="L163" s="1" t="s">
         <v>30</v>
@@ -12930,22 +13230,22 @@
         <v>1</v>
       </c>
       <c r="N163" s="11" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="O163" s="1" t="s">
-        <v>452</v>
+        <v>475</v>
       </c>
       <c r="P163" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q163" s="1" t="s">
-        <v>454</v>
+        <v>477</v>
       </c>
       <c r="R163" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S163" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V163" s="2">
         <v>15.748343</v>
@@ -12980,10 +13280,10 @@
         <v>5</v>
       </c>
       <c r="J164" s="11" t="s">
-        <v>455</v>
+        <v>478</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>456</v>
+        <v>479</v>
       </c>
       <c r="L164" s="1" t="s">
         <v>30</v>
@@ -12992,22 +13292,22 @@
         <v>11</v>
       </c>
       <c r="N164" s="11" t="s">
-        <v>457</v>
+        <v>480</v>
       </c>
       <c r="O164" s="1" t="s">
-        <v>458</v>
+        <v>481</v>
       </c>
       <c r="P164" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q164" s="1" t="s">
-        <v>459</v>
+        <v>482</v>
       </c>
       <c r="R164" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S164" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V164" s="2">
         <v>15.534311000000001</v>
@@ -13042,10 +13342,10 @@
         <v>20</v>
       </c>
       <c r="J165" s="11" t="s">
-        <v>460</v>
+        <v>483</v>
       </c>
       <c r="K165" s="1" t="s">
-        <v>461</v>
+        <v>484</v>
       </c>
       <c r="L165" s="1" t="s">
         <v>30</v>
@@ -13054,22 +13354,22 @@
         <v>1</v>
       </c>
       <c r="N165" s="11" t="s">
-        <v>462</v>
+        <v>485</v>
       </c>
       <c r="O165" s="1" t="s">
-        <v>461</v>
+        <v>484</v>
       </c>
       <c r="P165" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q165" s="1" t="s">
-        <v>463</v>
+        <v>486</v>
       </c>
       <c r="R165" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S165" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V165" s="2">
         <v>14.894002</v>
@@ -13104,10 +13404,10 @@
         <v>21</v>
       </c>
       <c r="J166" s="11" t="s">
-        <v>464</v>
+        <v>487</v>
       </c>
       <c r="K166" s="1" t="s">
-        <v>465</v>
+        <v>488</v>
       </c>
       <c r="L166" s="1" t="s">
         <v>30</v>
@@ -13116,22 +13416,22 @@
         <v>1</v>
       </c>
       <c r="N166" s="11" t="s">
-        <v>466</v>
+        <v>489</v>
       </c>
       <c r="O166" s="1" t="s">
-        <v>465</v>
+        <v>488</v>
       </c>
       <c r="P166" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q166" s="1" t="s">
-        <v>467</v>
+        <v>490</v>
       </c>
       <c r="R166" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S166" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V166" s="2">
         <v>14.690765000000001</v>
@@ -13166,10 +13466,10 @@
         <v>3</v>
       </c>
       <c r="J167" s="11" t="s">
-        <v>468</v>
+        <v>491</v>
       </c>
       <c r="K167" s="1" t="s">
-        <v>469</v>
+        <v>492</v>
       </c>
       <c r="L167" s="1" t="s">
         <v>30</v>
@@ -13178,22 +13478,22 @@
         <v>1</v>
       </c>
       <c r="N167" s="11" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="O167" s="1" t="s">
-        <v>469</v>
+        <v>492</v>
       </c>
       <c r="P167" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q167" s="1" t="s">
-        <v>471</v>
+        <v>494</v>
       </c>
       <c r="R167" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S167" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V167" s="2">
         <v>14.575887</v>
@@ -13228,10 +13528,10 @@
         <v>19</v>
       </c>
       <c r="J168" s="11" t="s">
-        <v>472</v>
+        <v>495</v>
       </c>
       <c r="K168" s="1" t="s">
-        <v>473</v>
+        <v>496</v>
       </c>
       <c r="L168" s="1" t="s">
         <v>30</v>
@@ -13240,22 +13540,22 @@
         <v>1</v>
       </c>
       <c r="N168" s="11" t="s">
-        <v>474</v>
+        <v>497</v>
       </c>
       <c r="O168" s="1" t="s">
-        <v>473</v>
+        <v>496</v>
       </c>
       <c r="P168" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q168" s="1" t="s">
-        <v>475</v>
+        <v>498</v>
       </c>
       <c r="R168" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S168" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V168" s="2">
         <v>14.323912999999999</v>
@@ -13290,29 +13590,29 @@
         <v>6</v>
       </c>
       <c r="J169" s="11" t="s">
-        <v>476</v>
+        <v>499</v>
       </c>
       <c r="K169" s="1" t="s">
-        <v>477</v>
+        <v>500</v>
       </c>
       <c r="L169" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N169" s="11"/>
       <c r="O169" s="1" t="s">
-        <v>477</v>
+        <v>500</v>
       </c>
       <c r="P169" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q169" s="1" t="s">
-        <v>478</v>
+        <v>501</v>
       </c>
       <c r="R169" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S169" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V169" s="2">
         <v>14.645818</v>
@@ -13347,29 +13647,29 @@
         <v>8</v>
       </c>
       <c r="J170" s="11" t="s">
-        <v>479</v>
+        <v>502</v>
       </c>
       <c r="K170" s="1" t="s">
-        <v>480</v>
+        <v>503</v>
       </c>
       <c r="L170" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N170" s="11"/>
       <c r="O170" s="1" t="s">
-        <v>480</v>
+        <v>503</v>
       </c>
       <c r="P170" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q170" s="1" t="s">
-        <v>481</v>
+        <v>504</v>
       </c>
       <c r="R170" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S170" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V170" s="2">
         <v>14.845943</v>
@@ -13404,29 +13704,29 @@
         <v>19</v>
       </c>
       <c r="J171" s="11" t="s">
-        <v>482</v>
+        <v>505</v>
       </c>
       <c r="K171" s="1" t="s">
-        <v>483</v>
+        <v>506</v>
       </c>
       <c r="L171" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N171" s="11"/>
       <c r="O171" s="1" t="s">
-        <v>483</v>
+        <v>506</v>
       </c>
       <c r="P171" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q171" s="1" t="s">
-        <v>484</v>
+        <v>507</v>
       </c>
       <c r="R171" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S171" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V171" s="2">
         <v>15.001557999999999</v>
@@ -13461,10 +13761,10 @@
         <v>13</v>
       </c>
       <c r="J172" s="11" t="s">
-        <v>485</v>
+        <v>508</v>
       </c>
       <c r="K172" s="1" t="s">
-        <v>486</v>
+        <v>509</v>
       </c>
       <c r="L172" s="1" t="s">
         <v>30</v>
@@ -13473,22 +13773,22 @@
         <v>1</v>
       </c>
       <c r="N172" s="11" t="s">
-        <v>487</v>
+        <v>510</v>
       </c>
       <c r="O172" s="1" t="s">
-        <v>488</v>
+        <v>511</v>
       </c>
       <c r="P172" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q172" s="1" t="s">
-        <v>489</v>
+        <v>512</v>
       </c>
       <c r="R172" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S172" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V172" s="2">
         <v>15.061814</v>
@@ -13523,10 +13823,10 @@
         <v>10</v>
       </c>
       <c r="J173" s="11" t="s">
-        <v>490</v>
+        <v>513</v>
       </c>
       <c r="K173" s="1" t="s">
-        <v>491</v>
+        <v>514</v>
       </c>
       <c r="L173" s="1" t="s">
         <v>30</v>
@@ -13535,22 +13835,22 @@
         <v>1</v>
       </c>
       <c r="N173" s="11" t="s">
-        <v>492</v>
+        <v>515</v>
       </c>
       <c r="O173" s="1" t="s">
-        <v>491</v>
+        <v>514</v>
       </c>
       <c r="P173" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q173" s="1" t="s">
-        <v>493</v>
+        <v>516</v>
       </c>
       <c r="R173" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S173" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V173" s="2">
         <v>15.024939</v>
@@ -13585,10 +13885,10 @@
         <v>12</v>
       </c>
       <c r="J174" s="11" t="s">
-        <v>494</v>
+        <v>517</v>
       </c>
       <c r="K174" s="1" t="s">
-        <v>495</v>
+        <v>518</v>
       </c>
       <c r="L174" s="1" t="s">
         <v>30</v>
@@ -13597,22 +13897,22 @@
         <v>1</v>
       </c>
       <c r="N174" s="11" t="s">
-        <v>496</v>
+        <v>519</v>
       </c>
       <c r="O174" s="1" t="s">
-        <v>495</v>
+        <v>518</v>
       </c>
       <c r="P174" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q174" s="1" t="s">
-        <v>497</v>
+        <v>520</v>
       </c>
       <c r="R174" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S174" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V174" s="2">
         <v>13.665829</v>
@@ -13647,10 +13947,10 @@
         <v>8</v>
       </c>
       <c r="J175" s="11" t="s">
-        <v>498</v>
+        <v>521</v>
       </c>
       <c r="K175" s="1" t="s">
-        <v>499</v>
+        <v>522</v>
       </c>
       <c r="L175" s="1" t="s">
         <v>30</v>
@@ -13659,22 +13959,22 @@
         <v>1</v>
       </c>
       <c r="N175" s="11" t="s">
-        <v>500</v>
+        <v>523</v>
       </c>
       <c r="O175" s="1" t="s">
-        <v>499</v>
+        <v>522</v>
       </c>
       <c r="P175" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q175" s="1" t="s">
-        <v>501</v>
+        <v>524</v>
       </c>
       <c r="R175" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S175" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V175" s="2">
         <v>13.568472999999999</v>
@@ -13709,10 +14009,10 @@
         <v>16</v>
       </c>
       <c r="J176" s="11" t="s">
-        <v>502</v>
+        <v>525</v>
       </c>
       <c r="K176" s="1" t="s">
-        <v>503</v>
+        <v>526</v>
       </c>
       <c r="L176" s="1" t="s">
         <v>30</v>
@@ -13721,22 +14021,22 @@
         <v>1</v>
       </c>
       <c r="N176" s="11" t="s">
-        <v>504</v>
+        <v>527</v>
       </c>
       <c r="O176" s="1" t="s">
-        <v>503</v>
+        <v>526</v>
       </c>
       <c r="P176" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q176" s="1" t="s">
-        <v>505</v>
+        <v>528</v>
       </c>
       <c r="R176" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S176" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V176" s="2">
         <v>13.293342000000001</v>
@@ -13771,10 +14071,10 @@
         <v>7</v>
       </c>
       <c r="J177" s="11" t="s">
-        <v>506</v>
+        <v>529</v>
       </c>
       <c r="K177" s="1" t="s">
-        <v>507</v>
+        <v>530</v>
       </c>
       <c r="L177" s="1" t="s">
         <v>30</v>
@@ -13783,22 +14083,22 @@
         <v>1</v>
       </c>
       <c r="N177" s="11" t="s">
-        <v>508</v>
+        <v>531</v>
       </c>
       <c r="O177" s="1" t="s">
-        <v>507</v>
+        <v>530</v>
       </c>
       <c r="P177" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q177" s="1" t="s">
-        <v>509</v>
+        <v>532</v>
       </c>
       <c r="R177" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S177" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V177" s="2">
         <v>13.284371999999999</v>
@@ -13833,10 +14133,10 @@
         <v>9</v>
       </c>
       <c r="J178" s="11" t="s">
-        <v>510</v>
+        <v>533</v>
       </c>
       <c r="K178" s="1" t="s">
-        <v>511</v>
+        <v>534</v>
       </c>
       <c r="L178" s="1" t="s">
         <v>30</v>
@@ -13845,22 +14145,22 @@
         <v>1</v>
       </c>
       <c r="N178" s="11" t="s">
-        <v>512</v>
+        <v>535</v>
       </c>
       <c r="O178" s="1" t="s">
-        <v>511</v>
+        <v>534</v>
       </c>
       <c r="P178" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q178" s="1" t="s">
-        <v>513</v>
+        <v>536</v>
       </c>
       <c r="R178" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S178" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V178" s="2">
         <v>13.203086000000001</v>
@@ -13895,10 +14195,10 @@
         <v>7</v>
       </c>
       <c r="J179" s="11" t="s">
-        <v>506</v>
+        <v>529</v>
       </c>
       <c r="K179" s="1" t="s">
-        <v>507</v>
+        <v>530</v>
       </c>
       <c r="L179" s="1" t="s">
         <v>30</v>
@@ -13907,22 +14207,22 @@
         <v>14</v>
       </c>
       <c r="N179" s="11" t="s">
-        <v>514</v>
+        <v>537</v>
       </c>
       <c r="O179" s="1" t="s">
-        <v>515</v>
+        <v>538</v>
       </c>
       <c r="P179" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q179" s="1" t="s">
-        <v>509</v>
+        <v>532</v>
       </c>
       <c r="R179" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S179" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V179" s="2">
         <v>13.198708</v>
@@ -13957,29 +14257,29 @@
         <v>13</v>
       </c>
       <c r="J180" s="11" t="s">
-        <v>516</v>
+        <v>539</v>
       </c>
       <c r="K180" s="1" t="s">
-        <v>517</v>
+        <v>540</v>
       </c>
       <c r="L180" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N180" s="11"/>
       <c r="O180" s="1" t="s">
-        <v>517</v>
+        <v>540</v>
       </c>
       <c r="P180" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q180" s="1" t="s">
-        <v>518</v>
+        <v>541</v>
       </c>
       <c r="R180" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S180" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V180" s="2">
         <v>13.932454999999999</v>
@@ -14014,10 +14314,10 @@
         <v>11</v>
       </c>
       <c r="J181" s="11" t="s">
-        <v>519</v>
+        <v>542</v>
       </c>
       <c r="K181" s="1" t="s">
-        <v>520</v>
+        <v>543</v>
       </c>
       <c r="L181" s="1" t="s">
         <v>30</v>
@@ -14026,22 +14326,22 @@
         <v>2</v>
       </c>
       <c r="N181" s="11" t="s">
-        <v>521</v>
+        <v>544</v>
       </c>
       <c r="O181" s="1" t="s">
-        <v>520</v>
+        <v>543</v>
       </c>
       <c r="P181" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q181" s="1" t="s">
-        <v>522</v>
+        <v>545</v>
       </c>
       <c r="R181" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S181" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V181" s="2">
         <v>14.915877999999999</v>
@@ -14076,10 +14376,10 @@
         <v>5</v>
       </c>
       <c r="J182" s="11" t="s">
-        <v>523</v>
+        <v>546</v>
       </c>
       <c r="K182" s="1" t="s">
-        <v>524</v>
+        <v>547</v>
       </c>
       <c r="L182" s="1" t="s">
         <v>30</v>
@@ -14088,22 +14388,22 @@
         <v>1</v>
       </c>
       <c r="N182" s="11" t="s">
-        <v>525</v>
+        <v>548</v>
       </c>
       <c r="O182" s="1" t="s">
-        <v>524</v>
+        <v>547</v>
       </c>
       <c r="P182" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q182" s="1" t="s">
-        <v>526</v>
+        <v>549</v>
       </c>
       <c r="R182" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S182" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V182" s="2">
         <v>14.754858</v>
@@ -14138,10 +14438,10 @@
         <v>14</v>
       </c>
       <c r="J183" s="11" t="s">
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="K183" s="1" t="s">
-        <v>528</v>
+        <v>551</v>
       </c>
       <c r="L183" s="1" t="s">
         <v>30</v>
@@ -14150,22 +14450,22 @@
         <v>1</v>
       </c>
       <c r="N183" s="11" t="s">
-        <v>529</v>
+        <v>552</v>
       </c>
       <c r="O183" s="1" t="s">
-        <v>528</v>
+        <v>551</v>
       </c>
       <c r="P183" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q183" s="1" t="s">
-        <v>530</v>
+        <v>553</v>
       </c>
       <c r="R183" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S183" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="V183" s="2">
         <v>14.714986</v>
@@ -14200,10 +14500,10 @@
         <v>19</v>
       </c>
       <c r="J184" s="11" t="s">
-        <v>531</v>
+        <v>554</v>
       </c>
       <c r="K184" s="1" t="s">
-        <v>532</v>
+        <v>555</v>
       </c>
       <c r="L184" s="1" t="s">
         <v>30</v>
@@ -14211,21 +14511,29 @@
       <c r="M184" s="1">
         <v>1</v>
       </c>
-      <c r="N184" s="11"/>
+      <c r="N184" s="11" t="s">
+        <v>556</v>
+      </c>
       <c r="O184" s="1" t="s">
-        <v>532</v>
+        <v>555</v>
       </c>
       <c r="P184" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q184" s="1" t="s">
-        <v>533</v>
+        <v>557</v>
       </c>
       <c r="R184" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S184" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V184" s="2">
+        <v>14.654638</v>
+      </c>
+      <c r="W184" s="2">
+        <v>-87.036589000000006</v>
       </c>
     </row>
     <row r="185" spans="2:23">
@@ -14250,22 +14558,44 @@
       <c r="H185" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J185" s="11"/>
+      <c r="I185" s="1">
+        <v>3</v>
+      </c>
+      <c r="J185" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="K185" s="1" t="s">
+        <v>559</v>
+      </c>
       <c r="L185" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N185" s="11"/>
+      <c r="M185" s="1">
+        <v>1</v>
+      </c>
+      <c r="N185" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="O185" s="1" t="s">
+        <v>559</v>
+      </c>
       <c r="P185" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q185" s="1" t="s">
-        <v>533</v>
+        <v>561</v>
       </c>
       <c r="R185" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S185" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V185" s="2">
+        <v>14.593650999999999</v>
+      </c>
+      <c r="W185" s="2">
+        <v>-87.119091999999995</v>
       </c>
     </row>
     <row r="186" spans="2:23">
@@ -14278,27 +14608,56 @@
       <c r="D186" s="1">
         <v>3</v>
       </c>
-      <c r="E186" s="7"/>
-      <c r="F186" s="10"/>
+      <c r="E186" s="7">
+        <v>9</v>
+      </c>
+      <c r="F186" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="H186" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J186" s="11"/>
+      <c r="I186" s="1">
+        <v>2</v>
+      </c>
+      <c r="J186" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>563</v>
+      </c>
       <c r="L186" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N186" s="11"/>
+      <c r="M186" s="1">
+        <v>4</v>
+      </c>
+      <c r="N186" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="O186" s="1" t="s">
+        <v>565</v>
+      </c>
       <c r="P186" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q186" s="1" t="s">
-        <v>533</v>
+        <v>566</v>
       </c>
       <c r="R186" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S186" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V186" s="2">
+        <v>15.893539000000001</v>
+      </c>
+      <c r="W186" s="2">
+        <v>-84.776458000000005</v>
       </c>
     </row>
     <row r="187" spans="2:23">
@@ -14311,27 +14670,56 @@
       <c r="D187" s="1">
         <v>3</v>
       </c>
-      <c r="E187" s="7"/>
-      <c r="F187" s="10"/>
+      <c r="E187" s="7">
+        <v>9</v>
+      </c>
+      <c r="F187" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="H187" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J187" s="11"/>
+      <c r="I187" s="1">
+        <v>2</v>
+      </c>
+      <c r="J187" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="K187" s="1" t="s">
+        <v>563</v>
+      </c>
       <c r="L187" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N187" s="11"/>
+      <c r="M187" s="1">
+        <v>2</v>
+      </c>
+      <c r="N187" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="O187" s="1" t="s">
+        <v>568</v>
+      </c>
       <c r="P187" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q187" s="1" t="s">
-        <v>533</v>
+        <v>566</v>
       </c>
       <c r="R187" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S187" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V187" s="2">
+        <v>15.799147</v>
+      </c>
+      <c r="W187" s="2">
+        <v>-84.294206000000003</v>
       </c>
     </row>
     <row r="188" spans="2:23">
@@ -14344,27 +14732,56 @@
       <c r="D188" s="1">
         <v>3</v>
       </c>
-      <c r="E188" s="7"/>
-      <c r="F188" s="10"/>
+      <c r="E188" s="7">
+        <v>9</v>
+      </c>
+      <c r="F188" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="H188" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J188" s="11"/>
+      <c r="I188" s="1">
+        <v>3</v>
+      </c>
+      <c r="J188" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>570</v>
+      </c>
       <c r="L188" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N188" s="11"/>
+      <c r="M188" s="1">
+        <v>32</v>
+      </c>
+      <c r="N188" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="O188" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="P188" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q188" s="1" t="s">
-        <v>533</v>
+        <v>573</v>
       </c>
       <c r="R188" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S188" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V188" s="2">
+        <v>15.064120000000001</v>
+      </c>
+      <c r="W188" s="2">
+        <v>-83.298761999999996</v>
       </c>
     </row>
     <row r="189" spans="2:23">
@@ -14377,27 +14794,56 @@
       <c r="D189" s="1">
         <v>3</v>
       </c>
-      <c r="E189" s="7"/>
-      <c r="F189" s="10"/>
+      <c r="E189" s="7">
+        <v>9</v>
+      </c>
+      <c r="F189" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="H189" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J189" s="11"/>
+      <c r="I189" s="1">
+        <v>4</v>
+      </c>
+      <c r="J189" s="11" t="s">
+        <v>574</v>
+      </c>
+      <c r="K189" s="1" t="s">
+        <v>575</v>
+      </c>
       <c r="L189" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N189" s="11"/>
+      <c r="M189" s="1">
+        <v>7</v>
+      </c>
+      <c r="N189" s="11" t="s">
+        <v>576</v>
+      </c>
+      <c r="O189" s="1" t="s">
+        <v>577</v>
+      </c>
       <c r="P189" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q189" s="1" t="s">
-        <v>533</v>
+        <v>578</v>
       </c>
       <c r="R189" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S189" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V189" s="2">
+        <v>15.043042</v>
+      </c>
+      <c r="W189" s="2">
+        <v>-84.874465000000001</v>
       </c>
     </row>
     <row r="190" spans="2:23">
@@ -14410,27 +14856,56 @@
       <c r="D190" s="1">
         <v>3</v>
       </c>
-      <c r="E190" s="7"/>
-      <c r="F190" s="10"/>
+      <c r="E190" s="7">
+        <v>15</v>
+      </c>
+      <c r="F190" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="H190" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J190" s="11"/>
+      <c r="I190" s="1">
+        <v>17</v>
+      </c>
+      <c r="J190" s="11" t="s">
+        <v>579</v>
+      </c>
+      <c r="K190" s="1" t="s">
+        <v>580</v>
+      </c>
       <c r="L190" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N190" s="11"/>
+      <c r="M190" s="1">
+        <v>19</v>
+      </c>
+      <c r="N190" s="11" t="s">
+        <v>581</v>
+      </c>
+      <c r="O190" s="1" t="s">
+        <v>582</v>
+      </c>
       <c r="P190" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q190" s="1" t="s">
-        <v>533</v>
+        <v>583</v>
       </c>
       <c r="R190" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S190" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V190" s="2">
+        <v>15.079923000000001</v>
+      </c>
+      <c r="W190" s="2">
+        <v>-85.832560000000001</v>
       </c>
     </row>
     <row r="191" spans="2:23">
@@ -14443,27 +14918,56 @@
       <c r="D191" s="1">
         <v>3</v>
       </c>
-      <c r="E191" s="7"/>
-      <c r="F191" s="10"/>
+      <c r="E191" s="7">
+        <v>15</v>
+      </c>
+      <c r="F191" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="H191" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J191" s="11"/>
+      <c r="I191" s="1">
+        <v>10</v>
+      </c>
+      <c r="J191" s="11" t="s">
+        <v>584</v>
+      </c>
+      <c r="K191" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L191" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N191" s="11"/>
+      <c r="M191" s="1">
+        <v>1</v>
+      </c>
+      <c r="N191" s="11" t="s">
+        <v>586</v>
+      </c>
+      <c r="O191" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="P191" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q191" s="1" t="s">
-        <v>533</v>
+        <v>587</v>
       </c>
       <c r="R191" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S191" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V191" s="2">
+        <v>15.079139</v>
+      </c>
+      <c r="W191" s="2">
+        <v>-86.418364999999994</v>
       </c>
     </row>
     <row r="192" spans="2:23">
@@ -14476,30 +14980,59 @@
       <c r="D192" s="1">
         <v>3</v>
       </c>
-      <c r="E192" s="7"/>
-      <c r="F192" s="10"/>
+      <c r="E192" s="7">
+        <v>15</v>
+      </c>
+      <c r="F192" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="H192" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J192" s="11"/>
+      <c r="I192" s="1">
+        <v>14</v>
+      </c>
+      <c r="J192" s="11" t="s">
+        <v>588</v>
+      </c>
+      <c r="K192" s="1" t="s">
+        <v>589</v>
+      </c>
       <c r="L192" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N192" s="11"/>
+      <c r="M192" s="1">
+        <v>1</v>
+      </c>
+      <c r="N192" s="11" t="s">
+        <v>590</v>
+      </c>
+      <c r="O192" s="1" t="s">
+        <v>589</v>
+      </c>
       <c r="P192" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q192" s="1" t="s">
-        <v>533</v>
+        <v>591</v>
       </c>
       <c r="R192" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S192" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="193" spans="2:19">
+        <v>384</v>
+      </c>
+      <c r="V192" s="2">
+        <v>15.035551</v>
+      </c>
+      <c r="W192" s="2">
+        <v>-86.819034000000002</v>
+      </c>
+    </row>
+    <row r="193" spans="2:23">
       <c r="B193" s="1" t="s">
         <v>23</v>
       </c>
@@ -14509,30 +15042,59 @@
       <c r="D193" s="1">
         <v>3</v>
       </c>
-      <c r="E193" s="7"/>
-      <c r="F193" s="10"/>
+      <c r="E193" s="7">
+        <v>15</v>
+      </c>
+      <c r="F193" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="H193" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J193" s="11"/>
+      <c r="I193" s="1">
+        <v>12</v>
+      </c>
+      <c r="J193" s="11" t="s">
+        <v>592</v>
+      </c>
+      <c r="K193" s="1" t="s">
+        <v>593</v>
+      </c>
       <c r="L193" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N193" s="11"/>
+      <c r="M193" s="1">
+        <v>1</v>
+      </c>
+      <c r="N193" s="11" t="s">
+        <v>594</v>
+      </c>
+      <c r="O193" s="1" t="s">
+        <v>593</v>
+      </c>
       <c r="P193" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q193" s="1" t="s">
-        <v>533</v>
+        <v>595</v>
       </c>
       <c r="R193" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S193" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="194" spans="2:19">
+        <v>384</v>
+      </c>
+      <c r="V193" s="2">
+        <v>15.028809000000001</v>
+      </c>
+      <c r="W193" s="2">
+        <v>-86.508201999999997</v>
+      </c>
+    </row>
+    <row r="194" spans="2:23">
       <c r="B194" s="1" t="s">
         <v>23</v>
       </c>
@@ -14542,27 +15104,122 @@
       <c r="D194" s="1">
         <v>3</v>
       </c>
-      <c r="E194" s="7"/>
-      <c r="F194" s="10"/>
+      <c r="E194" s="7">
+        <v>15</v>
+      </c>
+      <c r="F194" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="H194" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J194" s="11"/>
+      <c r="I194" s="1">
+        <v>18</v>
+      </c>
+      <c r="J194" s="11" t="s">
+        <v>596</v>
+      </c>
+      <c r="K194" s="1" t="s">
+        <v>597</v>
+      </c>
       <c r="L194" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N194" s="11"/>
+      <c r="M194" s="1">
+        <v>1</v>
+      </c>
+      <c r="N194" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="O194" s="1" t="s">
+        <v>597</v>
+      </c>
       <c r="P194" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q194" s="1" t="s">
-        <v>533</v>
+        <v>599</v>
       </c>
       <c r="R194" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S194" s="1" t="s">
-        <v>361</v>
+        <v>384</v>
+      </c>
+      <c r="V194" s="2">
+        <v>14.644175000000001</v>
+      </c>
+      <c r="W194" s="2">
+        <v>-86.105974000000003</v>
+      </c>
+    </row>
+    <row r="195" spans="2:23">
+      <c r="B195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D195" s="1">
+        <v>3</v>
+      </c>
+      <c r="E195" s="7"/>
+      <c r="F195" s="10"/>
+      <c r="H195" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J195" s="11"/>
+      <c r="L195" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N195" s="11"/>
+      <c r="P195" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q195" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="R195" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S195" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="196" spans="2:23">
+      <c r="B196" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D196" s="1">
+        <v>3</v>
+      </c>
+      <c r="E196" s="7"/>
+      <c r="F196" s="10"/>
+      <c r="H196" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J196" s="11"/>
+      <c r="L196" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N196" s="11"/>
+      <c r="P196" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q196" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="R196" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S196" s="1" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-13-2020 00-49-37
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1713" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{318E6431-4DD6-499D-8600-711C45D284FB}"/>
+  <xr:revisionPtr revIDLastSave="1730" documentId="8_{E1F7758E-E104-448D-A907-EF55592BDEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E665DE87-F202-473E-94AD-F7DEAACB0547}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="HOSPITALES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$196</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HOSPITALES!$A$1:$W$192</definedName>
     <definedName name="_xlnm.Database">HOSPITALES!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2726" uniqueCount="607">
   <si>
     <t>OBJECTID_1</t>
   </si>
@@ -1020,6 +1020,18 @@
     <t>Hospital Tela Integrado</t>
   </si>
   <si>
+    <t>0902</t>
+  </si>
+  <si>
+    <t>Brus Laguna</t>
+  </si>
+  <si>
+    <t>Baltimore</t>
+  </si>
+  <si>
+    <t>HND-0902</t>
+  </si>
+  <si>
     <t>Cesamo de Ibans</t>
   </si>
   <si>
@@ -1047,6 +1059,18 @@
     <t>Clínica de Emergencia Trinidad</t>
   </si>
   <si>
+    <t>1612</t>
+  </si>
+  <si>
+    <t>Macuelizo</t>
+  </si>
+  <si>
+    <t>Sula</t>
+  </si>
+  <si>
+    <t>HND-1612</t>
+  </si>
+  <si>
     <t>Hospital Sula Socorro de lo Atlto</t>
   </si>
   <si>
@@ -1083,6 +1107,15 @@
     <t xml:space="preserve">Yoro </t>
   </si>
   <si>
+    <t>1809</t>
+  </si>
+  <si>
+    <t>Sulaco</t>
+  </si>
+  <si>
+    <t>HND-1809</t>
+  </si>
+  <si>
     <t>Centro de Salud San Antonio Sulaco Yoro</t>
   </si>
   <si>
@@ -1113,9 +1146,6 @@
     <t>Hospital Manuel de Jesus Subirana</t>
   </si>
   <si>
-    <t>ACTS Clinic</t>
-  </si>
-  <si>
     <t>1313</t>
   </si>
   <si>
@@ -1722,21 +1752,12 @@
     <t>HND-0803</t>
   </si>
   <si>
-    <t>0902</t>
-  </si>
-  <si>
-    <t>Brus Laguna</t>
-  </si>
-  <si>
     <t>090204</t>
   </si>
   <si>
     <t>Cocobila</t>
   </si>
   <si>
-    <t>HND-0902</t>
-  </si>
-  <si>
     <t>090202</t>
   </si>
   <si>
@@ -1834,9 +1855,6 @@
   </si>
   <si>
     <t>HND-1518</t>
-  </si>
-  <si>
-    <t>HND-</t>
   </si>
 </sst>
 </file>
@@ -2506,8 +2524,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W196" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:W196" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16499EEC-32B0-41A9-AE9A-46E68A93C723}" name="HOSPITALES_HN" displayName="HOSPITALES_HN" ref="A1:W192" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:W192" xr:uid="{56D59612-14DD-44E0-B196-D6BA93C03EE3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W83">
     <sortCondition ref="S1:S83"/>
   </sortState>
@@ -2837,11 +2855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W196"/>
+  <dimension ref="A1:W195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="G106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K114" sqref="K114"/>
+      <pane ySplit="1" topLeftCell="P178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A194" sqref="A193:XFD194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -10357,13 +10375,27 @@
       <c r="H114" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J114" s="11"/>
+      <c r="I114" s="7">
+        <v>2</v>
+      </c>
+      <c r="J114" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>329</v>
+      </c>
       <c r="L114" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N114" s="11"/>
+      <c r="O114" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="P114" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="Q114" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="R114" s="1" t="s">
         <v>35</v>
@@ -10372,7 +10404,7 @@
         <v>36</v>
       </c>
       <c r="U114" s="1" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="V114" s="2">
         <v>15.908462</v>
@@ -10398,7 +10430,7 @@
         <v>237</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>27</v>
@@ -10407,10 +10439,10 @@
         <v>1</v>
       </c>
       <c r="J115" s="10" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="L115" s="1" t="s">
         <v>30</v>
@@ -10420,7 +10452,7 @@
         <v>33</v>
       </c>
       <c r="Q115" s="1" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="R115" s="1" t="s">
         <v>35</v>
@@ -10429,7 +10461,7 @@
         <v>179</v>
       </c>
       <c r="U115" s="1" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="V115" s="2">
         <v>14.925007000000001</v>
@@ -10455,7 +10487,7 @@
         <v>237</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>27</v>
@@ -10464,10 +10496,10 @@
         <v>26</v>
       </c>
       <c r="J116" s="10" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="L116" s="1" t="s">
         <v>30</v>
@@ -10477,7 +10509,7 @@
         <v>33</v>
       </c>
       <c r="Q116" s="1" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="R116" s="1" t="s">
         <v>35</v>
@@ -10486,7 +10518,7 @@
         <v>72</v>
       </c>
       <c r="U116" s="1" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="V116" s="2">
         <v>15.143121000000001</v>
@@ -10495,7 +10527,7 @@
         <v>-88.237575000000007</v>
       </c>
     </row>
-    <row r="117" spans="2:23">
+    <row r="117" spans="2:23" ht="15">
       <c r="B117" s="1" t="s">
         <v>23</v>
       </c>
@@ -10512,18 +10544,32 @@
         <v>237</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J117" s="11"/>
+      <c r="I117" s="7">
+        <v>12</v>
+      </c>
+      <c r="J117" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>342</v>
+      </c>
       <c r="L117" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N117" s="11"/>
+      <c r="O117" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="P117" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="Q117" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="R117" s="1" t="s">
         <v>35</v>
@@ -10532,7 +10578,7 @@
         <v>179</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="V117" s="2">
         <v>15.247275</v>
@@ -10558,7 +10604,7 @@
         <v>237</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>27</v>
@@ -10567,10 +10613,10 @@
         <v>15</v>
       </c>
       <c r="J118" s="10" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="L118" s="1" t="s">
         <v>30</v>
@@ -10580,7 +10626,7 @@
         <v>33</v>
       </c>
       <c r="Q118" s="1" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="R118" s="1" t="s">
         <v>35</v>
@@ -10589,7 +10635,7 @@
         <v>179</v>
       </c>
       <c r="U118" s="1" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="V118" s="2">
         <v>15.273072000000001</v>
@@ -10615,7 +10661,7 @@
         <v>237</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>27</v>
@@ -10646,7 +10692,7 @@
         <v>179</v>
       </c>
       <c r="U119" s="1" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="V119" s="2">
         <v>15.348732999999999</v>
@@ -10672,7 +10718,7 @@
         <v>250</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>27</v>
@@ -10681,10 +10727,10 @@
         <v>4</v>
       </c>
       <c r="J120" s="10" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="L120" s="1" t="s">
         <v>30</v>
@@ -10694,7 +10740,7 @@
         <v>33</v>
       </c>
       <c r="Q120" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="R120" s="1" t="s">
         <v>35</v>
@@ -10703,7 +10749,7 @@
         <v>179</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="V120" s="2">
         <v>13.861846</v>
@@ -10729,7 +10775,7 @@
         <v>250</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>27</v>
@@ -10738,10 +10784,10 @@
         <v>4</v>
       </c>
       <c r="J121" s="10" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="L121" s="1" t="s">
         <v>30</v>
@@ -10751,7 +10797,7 @@
         <v>33</v>
       </c>
       <c r="Q121" s="1" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="R121" s="1" t="s">
         <v>35</v>
@@ -10760,7 +10806,7 @@
         <v>179</v>
       </c>
       <c r="U121" s="1" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="V121" s="2">
         <v>13.865371</v>
@@ -10786,12 +10832,20 @@
         <v>161</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J122" s="11"/>
+      <c r="I122" s="7">
+        <v>9</v>
+      </c>
+      <c r="J122" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>358</v>
+      </c>
       <c r="L122" s="1" t="s">
         <v>30</v>
       </c>
@@ -10799,6 +10853,9 @@
       <c r="P122" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q122" s="1" t="s">
+        <v>359</v>
+      </c>
       <c r="R122" s="1" t="s">
         <v>35</v>
       </c>
@@ -10806,7 +10863,7 @@
         <v>36</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="V122" s="2">
         <v>14.985823</v>
@@ -10841,10 +10898,10 @@
         <v>11</v>
       </c>
       <c r="J123" s="13" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="L123" s="1" t="s">
         <v>30</v>
@@ -10854,7 +10911,7 @@
         <v>33</v>
       </c>
       <c r="Q123" s="1" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="R123" s="1" t="s">
         <v>35</v>
@@ -10863,7 +10920,7 @@
         <v>36</v>
       </c>
       <c r="U123" s="1" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="V123" s="2">
         <v>15.065429</v>
@@ -10872,7 +10929,7 @@
         <v>-87.277242999999999</v>
       </c>
     </row>
-    <row r="124" spans="2:23">
+    <row r="124" spans="2:23" ht="15">
       <c r="B124" s="1" t="s">
         <v>23</v>
       </c>
@@ -10894,7 +10951,15 @@
       <c r="H124" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J124" s="11"/>
+      <c r="I124" s="8">
+        <v>11</v>
+      </c>
+      <c r="J124" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="L124" s="1" t="s">
         <v>30</v>
       </c>
@@ -10902,6 +10967,9 @@
       <c r="P124" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q124" s="1" t="s">
+        <v>363</v>
+      </c>
       <c r="R124" s="1" t="s">
         <v>35</v>
       </c>
@@ -10909,7 +10977,7 @@
         <v>36</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="V124" s="2">
         <v>15.108616</v>
@@ -10944,7 +11012,7 @@
         <v>1</v>
       </c>
       <c r="J125" s="10" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>162</v>
@@ -10957,7 +11025,7 @@
         <v>33</v>
       </c>
       <c r="Q125" s="1" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="R125" s="1" t="s">
         <v>35</v>
@@ -10966,7 +11034,7 @@
         <v>72</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="V125" s="2">
         <v>15.137855999999999</v>
@@ -11001,7 +11069,7 @@
         <v>1</v>
       </c>
       <c r="J126" s="10" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>162</v>
@@ -11014,7 +11082,7 @@
         <v>33</v>
       </c>
       <c r="Q126" s="1" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="R126" s="1" t="s">
         <v>35</v>
@@ -11023,7 +11091,7 @@
         <v>179</v>
       </c>
       <c r="U126" s="1" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="V126" s="2">
         <v>15.137337</v>
@@ -11032,7 +11100,7 @@
         <v>-87.133142000000007</v>
       </c>
     </row>
-    <row r="127" spans="2:23">
+    <row r="127" spans="2:23" ht="15">
       <c r="B127" s="1" t="s">
         <v>23</v>
       </c>
@@ -11043,18 +11111,26 @@
         <v>3</v>
       </c>
       <c r="E127" s="7">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F127" s="10" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J127" s="11"/>
+      <c r="I127" s="7">
+        <v>13</v>
+      </c>
+      <c r="J127" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>371</v>
+      </c>
       <c r="L127" s="1" t="s">
         <v>30</v>
       </c>
@@ -11062,20 +11138,23 @@
       <c r="P127" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q127" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="R127" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S127" s="1" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="V127" s="2">
-        <v>15.276194</v>
+        <v>14.780340000000001</v>
       </c>
       <c r="W127" s="2">
-        <v>-87.324967999999998</v>
+        <v>-88.588606999999996</v>
       </c>
     </row>
     <row r="128" spans="2:23" ht="15">
@@ -11101,13 +11180,13 @@
         <v>27</v>
       </c>
       <c r="I128" s="7">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J128" s="10" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="L128" s="1" t="s">
         <v>30</v>
@@ -11117,7 +11196,7 @@
         <v>33</v>
       </c>
       <c r="Q128" s="1" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="R128" s="1" t="s">
         <v>35</v>
@@ -11126,13 +11205,13 @@
         <v>36</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="V128" s="2">
-        <v>14.780340000000001</v>
+        <v>14.329539</v>
       </c>
       <c r="W128" s="2">
-        <v>-88.588606999999996</v>
+        <v>-88.522634999999994</v>
       </c>
     </row>
     <row r="129" spans="2:23" ht="15">
@@ -11158,13 +11237,13 @@
         <v>27</v>
       </c>
       <c r="I129" s="7">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="J129" s="10" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="L129" s="1" t="s">
         <v>30</v>
@@ -11174,22 +11253,22 @@
         <v>33</v>
       </c>
       <c r="Q129" s="1" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="R129" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S129" s="1" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="V129" s="2">
-        <v>14.329539</v>
+        <v>14.126211</v>
       </c>
       <c r="W129" s="2">
-        <v>-88.522634999999994</v>
+        <v>-88.543222999999998</v>
       </c>
     </row>
     <row r="130" spans="2:23" ht="15">
@@ -11203,25 +11282,25 @@
         <v>3</v>
       </c>
       <c r="E130" s="7">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F130" s="10" t="s">
-        <v>142</v>
+        <v>276</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>143</v>
+        <v>277</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I130" s="7">
-        <v>6</v>
-      </c>
-      <c r="J130" s="10" t="s">
-        <v>368</v>
+        <v>1</v>
+      </c>
+      <c r="J130" s="12">
+        <v>1701</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="L130" s="1" t="s">
         <v>30</v>
@@ -11231,25 +11310,25 @@
         <v>33</v>
       </c>
       <c r="Q130" s="1" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="R130" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S130" s="1" t="s">
-        <v>179</v>
+        <v>72</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="V130" s="2">
-        <v>14.126211</v>
+        <v>13.530787999999999</v>
       </c>
       <c r="W130" s="2">
-        <v>-88.543222999999998</v>
-      </c>
-    </row>
-    <row r="131" spans="2:23">
+        <v>-87.498217999999994</v>
+      </c>
+    </row>
+    <row r="131" spans="2:23" ht="15">
       <c r="B131" s="1" t="s">
         <v>23</v>
       </c>
@@ -11260,18 +11339,26 @@
         <v>3</v>
       </c>
       <c r="E131" s="7">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F131" s="10" t="s">
-        <v>142</v>
+        <v>276</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>143</v>
+        <v>277</v>
       </c>
       <c r="H131" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J131" s="11"/>
+      <c r="I131" s="7">
+        <v>1</v>
+      </c>
+      <c r="J131" s="12">
+        <v>1701</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>382</v>
+      </c>
       <c r="L131" s="1" t="s">
         <v>30</v>
       </c>
@@ -11279,20 +11366,23 @@
       <c r="P131" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="Q131" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="R131" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S131" s="1" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
       <c r="U131" s="1" t="s">
-        <v>44</v>
+        <v>385</v>
       </c>
       <c r="V131" s="2">
-        <v>14.114020999999999</v>
+        <v>13.532709000000001</v>
       </c>
       <c r="W131" s="2">
-        <v>-88.651722000000007</v>
+        <v>-87.492543999999995</v>
       </c>
     </row>
     <row r="132" spans="2:23" ht="15">
@@ -11318,13 +11408,13 @@
         <v>27</v>
       </c>
       <c r="I132" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J132" s="12">
-        <v>1701</v>
+        <v>1707</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>30</v>
@@ -11334,22 +11424,22 @@
         <v>33</v>
       </c>
       <c r="Q132" s="1" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="R132" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S132" s="1" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="V132" s="2">
-        <v>13.530787999999999</v>
+        <v>13.62003</v>
       </c>
       <c r="W132" s="2">
-        <v>-87.498217999999994</v>
+        <v>-87.657388999999995</v>
       </c>
     </row>
     <row r="133" spans="2:23" ht="15">
@@ -11375,13 +11465,13 @@
         <v>27</v>
       </c>
       <c r="I133" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J133" s="12">
-        <v>1701</v>
+        <v>1706</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="L133" s="1" t="s">
         <v>30</v>
@@ -11391,22 +11481,22 @@
         <v>33</v>
       </c>
       <c r="Q133" s="1" t="s">
-        <v>373</v>
+        <v>390</v>
       </c>
       <c r="R133" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S133" s="1" t="s">
-        <v>179</v>
+        <v>72</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>375</v>
+        <v>391</v>
       </c>
       <c r="V133" s="2">
-        <v>13.532709000000001</v>
+        <v>13.610545</v>
       </c>
       <c r="W133" s="2">
-        <v>-87.492543999999995</v>
+        <v>-87.752651</v>
       </c>
     </row>
     <row r="134" spans="2:23" ht="15">
@@ -11420,53 +11510,58 @@
         <v>3</v>
       </c>
       <c r="E134" s="7">
-        <v>17</v>
-      </c>
-      <c r="F134" s="10" t="s">
-        <v>276</v>
+        <v>11</v>
+      </c>
+      <c r="F134" s="10">
+        <v>11</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>277</v>
+        <v>56</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I134" s="7">
-        <v>7</v>
+      <c r="I134" s="1">
+        <v>2</v>
       </c>
       <c r="J134" s="12">
-        <v>1707</v>
+        <v>1102</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>376</v>
+        <v>392</v>
       </c>
       <c r="L134" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N134" s="11"/>
+      <c r="M134" s="1">
+        <v>1</v>
+      </c>
+      <c r="N134" s="11">
+        <v>110201</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>392</v>
+      </c>
       <c r="P134" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q134" s="1" t="s">
-        <v>377</v>
+        <v>393</v>
       </c>
       <c r="R134" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S134" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U134" s="1" t="s">
-        <v>378</v>
+        <v>394</v>
       </c>
       <c r="V134" s="2">
-        <v>13.62003</v>
+        <v>16.439831999999999</v>
       </c>
       <c r="W134" s="2">
-        <v>-87.657388999999995</v>
-      </c>
-    </row>
-    <row r="135" spans="2:23" ht="15">
+        <v>-85.887030999999993</v>
+      </c>
+    </row>
+    <row r="135" spans="2:23">
       <c r="B135" s="1" t="s">
         <v>23</v>
       </c>
@@ -11477,53 +11572,53 @@
         <v>3</v>
       </c>
       <c r="E135" s="7">
-        <v>17</v>
-      </c>
-      <c r="F135" s="10" t="s">
-        <v>276</v>
+        <v>11</v>
+      </c>
+      <c r="F135" s="10">
+        <v>11</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>277</v>
+        <v>56</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I135" s="7">
-        <v>6</v>
+      <c r="I135" s="1">
+        <v>2</v>
       </c>
       <c r="J135" s="12">
-        <v>1706</v>
+        <v>1102</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="L135" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N135" s="11"/>
+      <c r="O135" s="1" t="s">
+        <v>395</v>
+      </c>
       <c r="P135" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q135" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="R135" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S135" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U135" s="1" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="V135" s="2">
-        <v>13.610545</v>
+        <v>16.484898000000001</v>
       </c>
       <c r="W135" s="2">
-        <v>-87.752651</v>
-      </c>
-    </row>
-    <row r="136" spans="2:23" ht="15">
+        <v>-85.844579999999993</v>
+      </c>
+    </row>
+    <row r="136" spans="2:23">
       <c r="B136" s="1" t="s">
         <v>23</v>
       </c>
@@ -11545,44 +11640,44 @@
       <c r="H136" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I136" s="1">
-        <v>2</v>
-      </c>
-      <c r="J136" s="12">
-        <v>1102</v>
-      </c>
-      <c r="K136" s="1" t="s">
-        <v>382</v>
+      <c r="I136" s="9">
+        <v>3</v>
+      </c>
+      <c r="J136" s="11">
+        <v>1103</v>
+      </c>
+      <c r="K136" s="9" t="s">
+        <v>396</v>
       </c>
       <c r="L136" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M136" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N136" s="11">
-        <v>110201</v>
+        <v>110303</v>
       </c>
       <c r="O136" s="1" t="s">
-        <v>382</v>
+        <v>397</v>
       </c>
       <c r="P136" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q136" s="1" t="s">
-        <v>383</v>
+        <v>398</v>
       </c>
       <c r="R136" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S136" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V136" s="2">
-        <v>16.439831999999999</v>
+        <v>16.438224000000002</v>
       </c>
       <c r="W136" s="2">
-        <v>-85.887030999999993</v>
+        <v>-86.146834999999996</v>
       </c>
     </row>
     <row r="137" spans="2:23">
@@ -11596,50 +11691,55 @@
         <v>3</v>
       </c>
       <c r="E137" s="7">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F137" s="10">
-        <v>11</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+      <c r="G137" s="9" t="s">
+        <v>271</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I137" s="1">
-        <v>2</v>
-      </c>
-      <c r="J137" s="12">
-        <v>1102</v>
-      </c>
-      <c r="K137" s="1" t="s">
-        <v>382</v>
+      <c r="I137" s="9">
+        <v>10</v>
+      </c>
+      <c r="J137" s="11">
+        <v>1410</v>
+      </c>
+      <c r="K137" s="9" t="s">
+        <v>399</v>
       </c>
       <c r="L137" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N137" s="11"/>
+      <c r="M137" s="1">
+        <v>1</v>
+      </c>
+      <c r="N137" s="11">
+        <v>141001</v>
+      </c>
       <c r="O137" s="1" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="P137" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q137" s="1" t="s">
-        <v>383</v>
+        <v>400</v>
       </c>
       <c r="R137" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S137" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V137" s="2">
-        <v>16.484898000000001</v>
+        <v>14.680396999999999</v>
       </c>
       <c r="W137" s="2">
-        <v>-85.844579999999993</v>
+        <v>-89.111785999999995</v>
       </c>
     </row>
     <row r="138" spans="2:23">
@@ -11653,25 +11753,25 @@
         <v>3</v>
       </c>
       <c r="E138" s="7">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F138" s="10">
-        <v>11</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+      <c r="G138" s="9" t="s">
+        <v>271</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I138" s="9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J138" s="11">
-        <v>1103</v>
+        <v>1406</v>
       </c>
       <c r="K138" s="9" t="s">
-        <v>386</v>
+        <v>401</v>
       </c>
       <c r="L138" s="1" t="s">
         <v>30</v>
@@ -11680,28 +11780,28 @@
         <v>3</v>
       </c>
       <c r="N138" s="11">
-        <v>110303</v>
+        <v>140603</v>
       </c>
       <c r="O138" s="1" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="P138" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q138" s="1" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="R138" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S138" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V138" s="2">
-        <v>16.438224000000002</v>
+        <v>14.664014</v>
       </c>
       <c r="W138" s="2">
-        <v>-86.146834999999996</v>
+        <v>-89.069692000000003</v>
       </c>
     </row>
     <row r="139" spans="2:23">
@@ -11727,43 +11827,43 @@
         <v>27</v>
       </c>
       <c r="I139" s="9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J139" s="11">
-        <v>1410</v>
+        <v>1415</v>
       </c>
       <c r="K139" s="9" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="L139" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M139" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N139" s="11">
-        <v>141001</v>
+        <v>141502</v>
       </c>
       <c r="O139" s="1" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="P139" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q139" s="1" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="R139" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S139" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V139" s="2">
-        <v>14.680396999999999</v>
+        <v>14.487455000000001</v>
       </c>
       <c r="W139" s="2">
-        <v>-89.111785999999995</v>
+        <v>-88.915816000000007</v>
       </c>
     </row>
     <row r="140" spans="2:23">
@@ -11789,43 +11889,43 @@
         <v>27</v>
       </c>
       <c r="I140" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J140" s="11">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="K140" s="9" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="L140" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M140" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N140" s="11">
-        <v>140603</v>
+        <v>140701</v>
       </c>
       <c r="O140" s="1" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="P140" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q140" s="1" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="R140" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S140" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V140" s="2">
-        <v>14.664014</v>
+        <v>14.484342</v>
       </c>
       <c r="W140" s="2">
-        <v>-89.069692000000003</v>
+        <v>-89.002711000000005</v>
       </c>
     </row>
     <row r="141" spans="2:23">
@@ -11851,43 +11951,43 @@
         <v>27</v>
       </c>
       <c r="I141" s="9">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="J141" s="11">
-        <v>1415</v>
+        <v>1402</v>
       </c>
       <c r="K141" s="9" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="L141" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M141" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N141" s="11">
-        <v>141502</v>
+        <v>140201</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>393</v>
+        <v>408</v>
       </c>
       <c r="P141" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q141" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S141" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="R141" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S141" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="V141" s="2">
-        <v>14.487455000000001</v>
+        <v>14.477974</v>
       </c>
       <c r="W141" s="2">
-        <v>-88.915816000000007</v>
+        <v>-88.790651999999994</v>
       </c>
     </row>
     <row r="142" spans="2:23">
@@ -11913,13 +12013,13 @@
         <v>27</v>
       </c>
       <c r="I142" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J142" s="11">
-        <v>1407</v>
+        <v>1401</v>
       </c>
       <c r="K142" s="9" t="s">
-        <v>395</v>
+        <v>410</v>
       </c>
       <c r="L142" s="1" t="s">
         <v>30</v>
@@ -11928,28 +12028,28 @@
         <v>1</v>
       </c>
       <c r="N142" s="11">
-        <v>140701</v>
+        <v>140101</v>
       </c>
       <c r="O142" s="1" t="s">
-        <v>395</v>
+        <v>410</v>
       </c>
       <c r="P142" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q142" s="1" t="s">
-        <v>396</v>
+        <v>411</v>
       </c>
       <c r="R142" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S142" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V142" s="2">
-        <v>14.484342</v>
+        <v>14.43247</v>
       </c>
       <c r="W142" s="2">
-        <v>-89.002711000000005</v>
+        <v>-89.182400000000001</v>
       </c>
     </row>
     <row r="143" spans="2:23">
@@ -11963,25 +12063,25 @@
         <v>3</v>
       </c>
       <c r="E143" s="7">
-        <v>14</v>
-      </c>
-      <c r="F143" s="10">
-        <v>14</v>
-      </c>
-      <c r="G143" s="9" t="s">
-        <v>271</v>
+        <v>7</v>
+      </c>
+      <c r="F143" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I143" s="9">
-        <v>2</v>
-      </c>
-      <c r="J143" s="11">
-        <v>1402</v>
-      </c>
-      <c r="K143" s="9" t="s">
-        <v>397</v>
+      <c r="I143" s="1">
+        <v>15</v>
+      </c>
+      <c r="J143" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>413</v>
       </c>
       <c r="L143" s="1" t="s">
         <v>30</v>
@@ -11989,29 +12089,29 @@
       <c r="M143" s="1">
         <v>1</v>
       </c>
-      <c r="N143" s="11">
-        <v>140201</v>
+      <c r="N143" s="11" t="s">
+        <v>414</v>
       </c>
       <c r="O143" s="1" t="s">
-        <v>398</v>
+        <v>413</v>
       </c>
       <c r="P143" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q143" s="1" t="s">
-        <v>399</v>
+        <v>415</v>
       </c>
       <c r="R143" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S143" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V143" s="2">
-        <v>14.477974</v>
+        <v>14.225474</v>
       </c>
       <c r="W143" s="2">
-        <v>-88.790651999999994</v>
+        <v>-86.716131000000004</v>
       </c>
     </row>
     <row r="144" spans="2:23">
@@ -12025,25 +12125,25 @@
         <v>3</v>
       </c>
       <c r="E144" s="7">
-        <v>14</v>
-      </c>
-      <c r="F144" s="10">
-        <v>14</v>
-      </c>
-      <c r="G144" s="9" t="s">
-        <v>271</v>
+        <v>7</v>
+      </c>
+      <c r="F144" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="H144" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I144" s="9">
-        <v>1</v>
-      </c>
-      <c r="J144" s="11">
-        <v>1401</v>
-      </c>
-      <c r="K144" s="9" t="s">
-        <v>400</v>
+      <c r="I144" s="1">
+        <v>8</v>
+      </c>
+      <c r="J144" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>417</v>
       </c>
       <c r="L144" s="1" t="s">
         <v>30</v>
@@ -12051,29 +12151,29 @@
       <c r="M144" s="1">
         <v>1</v>
       </c>
-      <c r="N144" s="11">
-        <v>140101</v>
+      <c r="N144" s="11" t="s">
+        <v>418</v>
       </c>
       <c r="O144" s="1" t="s">
-        <v>400</v>
+        <v>417</v>
       </c>
       <c r="P144" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q144" s="1" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="R144" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S144" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V144" s="2">
-        <v>14.43247</v>
+        <v>14.123517</v>
       </c>
       <c r="W144" s="2">
-        <v>-89.182400000000001</v>
+        <v>-86.866437000000005</v>
       </c>
     </row>
     <row r="145" spans="2:23">
@@ -12093,19 +12193,19 @@
         <v>250</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I145" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J145" s="11" t="s">
-        <v>402</v>
+        <v>420</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>403</v>
+        <v>421</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>30</v>
@@ -12114,28 +12214,28 @@
         <v>1</v>
       </c>
       <c r="N145" s="11" t="s">
-        <v>404</v>
+        <v>422</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>403</v>
+        <v>421</v>
       </c>
       <c r="P145" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q145" s="1" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="R145" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S145" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V145" s="2">
-        <v>14.225474</v>
+        <v>14.081087999999999</v>
       </c>
       <c r="W145" s="2">
-        <v>-86.716131000000004</v>
+        <v>-86.001908</v>
       </c>
     </row>
     <row r="146" spans="2:23">
@@ -12155,19 +12255,19 @@
         <v>250</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I146" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J146" s="11" t="s">
-        <v>406</v>
+        <v>424</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>407</v>
+        <v>425</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>30</v>
@@ -12176,28 +12276,28 @@
         <v>1</v>
       </c>
       <c r="N146" s="11" t="s">
-        <v>408</v>
+        <v>426</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>407</v>
+        <v>425</v>
       </c>
       <c r="P146" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q146" s="1" t="s">
-        <v>409</v>
+        <v>427</v>
       </c>
       <c r="R146" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S146" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V146" s="2">
-        <v>14.123517</v>
+        <v>13.880433</v>
       </c>
       <c r="W146" s="2">
-        <v>-86.866437000000005</v>
+        <v>-86.935871000000006</v>
       </c>
     </row>
     <row r="147" spans="2:23">
@@ -12217,19 +12317,19 @@
         <v>250</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I147" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J147" s="11" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="L147" s="1" t="s">
         <v>30</v>
@@ -12238,28 +12338,28 @@
         <v>1</v>
       </c>
       <c r="N147" s="11" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="O147" s="1" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="P147" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q147" s="1" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="R147" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S147" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V147" s="2">
-        <v>14.081087999999999</v>
+        <v>13.648353999999999</v>
       </c>
       <c r="W147" s="2">
-        <v>-86.001908</v>
+        <v>-87.024221999999995</v>
       </c>
     </row>
     <row r="148" spans="2:23">
@@ -12279,19 +12379,19 @@
         <v>250</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I148" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="J148" s="11" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="L148" s="1" t="s">
         <v>30</v>
@@ -12300,28 +12400,28 @@
         <v>1</v>
       </c>
       <c r="N148" s="11" t="s">
-        <v>416</v>
+        <v>434</v>
       </c>
       <c r="O148" s="1" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="P148" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q148" s="1" t="s">
-        <v>417</v>
+        <v>435</v>
       </c>
       <c r="R148" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S148" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V148" s="2">
-        <v>13.880433</v>
+        <v>13.586309</v>
       </c>
       <c r="W148" s="2">
-        <v>-86.935871000000006</v>
+        <v>-87.119765000000001</v>
       </c>
     </row>
     <row r="149" spans="2:23">
@@ -12341,49 +12441,49 @@
         <v>250</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I149" s="1">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="J149" s="11" t="s">
-        <v>418</v>
+        <v>436</v>
       </c>
       <c r="K149" s="1" t="s">
-        <v>419</v>
+        <v>437</v>
       </c>
       <c r="L149" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M149" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N149" s="11" t="s">
-        <v>420</v>
+        <v>438</v>
       </c>
       <c r="O149" s="1" t="s">
-        <v>419</v>
+        <v>437</v>
       </c>
       <c r="P149" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q149" s="1" t="s">
-        <v>421</v>
+        <v>439</v>
       </c>
       <c r="R149" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S149" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V149" s="2">
-        <v>13.648353999999999</v>
+        <v>13.541517000000001</v>
       </c>
       <c r="W149" s="2">
-        <v>-87.024221999999995</v>
+        <v>-87.065835000000007</v>
       </c>
     </row>
     <row r="150" spans="2:23">
@@ -12397,25 +12497,25 @@
         <v>3</v>
       </c>
       <c r="E150" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F150" s="10" t="s">
-        <v>250</v>
+        <v>84</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>343</v>
+        <v>85</v>
       </c>
       <c r="H150" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I150" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="J150" s="11" t="s">
-        <v>422</v>
+        <v>440</v>
       </c>
       <c r="K150" s="1" t="s">
-        <v>423</v>
+        <v>441</v>
       </c>
       <c r="L150" s="1" t="s">
         <v>30</v>
@@ -12424,28 +12524,28 @@
         <v>1</v>
       </c>
       <c r="N150" s="11" t="s">
-        <v>424</v>
+        <v>442</v>
       </c>
       <c r="O150" s="1" t="s">
-        <v>423</v>
+        <v>441</v>
       </c>
       <c r="P150" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q150" s="1" t="s">
-        <v>425</v>
+        <v>443</v>
       </c>
       <c r="R150" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S150" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V150" s="2">
-        <v>13.586309</v>
+        <v>15.774127999999999</v>
       </c>
       <c r="W150" s="2">
-        <v>-87.119765000000001</v>
+        <v>-88.038325999999998</v>
       </c>
     </row>
     <row r="151" spans="2:23">
@@ -12459,55 +12559,55 @@
         <v>3</v>
       </c>
       <c r="E151" s="7">
+        <v>5</v>
+      </c>
+      <c r="F151" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151" s="1">
+        <v>3</v>
+      </c>
+      <c r="J151" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="K151" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="L151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M151" s="1">
         <v>7</v>
       </c>
-      <c r="F151" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="G151" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="H151" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I151" s="1">
-        <v>7</v>
-      </c>
-      <c r="J151" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="K151" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="L151" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M151" s="1">
-        <v>3</v>
-      </c>
       <c r="N151" s="11" t="s">
-        <v>428</v>
+        <v>444</v>
       </c>
       <c r="O151" s="1" t="s">
-        <v>427</v>
+        <v>445</v>
       </c>
       <c r="P151" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q151" s="1" t="s">
-        <v>429</v>
+        <v>443</v>
       </c>
       <c r="R151" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S151" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V151" s="2">
-        <v>13.541517000000001</v>
+        <v>15.663361</v>
       </c>
       <c r="W151" s="2">
-        <v>-87.065835000000007</v>
+        <v>-88.194593999999995</v>
       </c>
     </row>
     <row r="152" spans="2:23">
@@ -12533,13 +12633,13 @@
         <v>27</v>
       </c>
       <c r="I152" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J152" s="11" t="s">
-        <v>430</v>
+        <v>446</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>431</v>
+        <v>447</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>30</v>
@@ -12548,28 +12648,28 @@
         <v>1</v>
       </c>
       <c r="N152" s="11" t="s">
-        <v>432</v>
+        <v>448</v>
       </c>
       <c r="O152" s="1" t="s">
-        <v>431</v>
+        <v>449</v>
       </c>
       <c r="P152" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q152" s="1" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
       <c r="R152" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S152" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V152" s="2">
-        <v>15.774127999999999</v>
+        <v>15.610602</v>
       </c>
       <c r="W152" s="2">
-        <v>-88.038325999999998</v>
+        <v>-87.951762000000002</v>
       </c>
     </row>
     <row r="153" spans="2:23">
@@ -12595,43 +12695,43 @@
         <v>27</v>
       </c>
       <c r="I153" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J153" s="11" t="s">
-        <v>430</v>
+        <v>451</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>431</v>
+        <v>452</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M153" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N153" s="11" t="s">
-        <v>434</v>
+        <v>453</v>
       </c>
       <c r="O153" s="1" t="s">
-        <v>435</v>
+        <v>452</v>
       </c>
       <c r="P153" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q153" s="1" t="s">
-        <v>433</v>
+        <v>454</v>
       </c>
       <c r="R153" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S153" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V153" s="2">
-        <v>15.663361</v>
+        <v>15.439396</v>
       </c>
       <c r="W153" s="2">
-        <v>-88.194593999999995</v>
+        <v>-87.928895999999995</v>
       </c>
     </row>
     <row r="154" spans="2:23">
@@ -12657,13 +12757,13 @@
         <v>27</v>
       </c>
       <c r="I154" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J154" s="11" t="s">
-        <v>436</v>
+        <v>455</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>437</v>
+        <v>456</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>30</v>
@@ -12672,28 +12772,28 @@
         <v>1</v>
       </c>
       <c r="N154" s="11" t="s">
-        <v>438</v>
+        <v>457</v>
       </c>
       <c r="O154" s="1" t="s">
-        <v>439</v>
+        <v>456</v>
       </c>
       <c r="P154" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q154" s="1" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="R154" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S154" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V154" s="2">
-        <v>15.610602</v>
+        <v>15.329428999999999</v>
       </c>
       <c r="W154" s="2">
-        <v>-87.951762000000002</v>
+        <v>-87.921024000000003</v>
       </c>
     </row>
     <row r="155" spans="2:23">
@@ -12719,13 +12819,13 @@
         <v>27</v>
       </c>
       <c r="I155" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J155" s="11" t="s">
-        <v>441</v>
+        <v>459</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>442</v>
+        <v>460</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>30</v>
@@ -12734,28 +12834,28 @@
         <v>1</v>
       </c>
       <c r="N155" s="11" t="s">
-        <v>443</v>
+        <v>461</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>442</v>
+        <v>460</v>
       </c>
       <c r="P155" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q155" s="1" t="s">
-        <v>444</v>
+        <v>462</v>
       </c>
       <c r="R155" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S155" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V155" s="2">
-        <v>15.439396</v>
+        <v>15.312935</v>
       </c>
       <c r="W155" s="2">
-        <v>-87.928895999999995</v>
+        <v>-87.993703999999994</v>
       </c>
     </row>
     <row r="156" spans="2:23">
@@ -12781,13 +12881,13 @@
         <v>27</v>
       </c>
       <c r="I156" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J156" s="11" t="s">
-        <v>445</v>
+        <v>463</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>446</v>
+        <v>464</v>
       </c>
       <c r="L156" s="1" t="s">
         <v>30</v>
@@ -12796,28 +12896,28 @@
         <v>1</v>
       </c>
       <c r="N156" s="11" t="s">
-        <v>447</v>
+        <v>465</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>446</v>
+        <v>464</v>
       </c>
       <c r="P156" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q156" s="1" t="s">
-        <v>448</v>
+        <v>466</v>
       </c>
       <c r="R156" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S156" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V156" s="2">
-        <v>15.329428999999999</v>
+        <v>15.228071</v>
       </c>
       <c r="W156" s="2">
-        <v>-87.921024000000003</v>
+        <v>-87.964016999999998</v>
       </c>
     </row>
     <row r="157" spans="2:23">
@@ -12843,13 +12943,13 @@
         <v>27</v>
       </c>
       <c r="I157" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J157" s="11" t="s">
-        <v>449</v>
+        <v>467</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>450</v>
+        <v>468</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>30</v>
@@ -12858,28 +12958,28 @@
         <v>1</v>
       </c>
       <c r="N157" s="11" t="s">
-        <v>451</v>
+        <v>469</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>450</v>
+        <v>468</v>
       </c>
       <c r="P157" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q157" s="1" t="s">
-        <v>452</v>
+        <v>470</v>
       </c>
       <c r="R157" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S157" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V157" s="2">
-        <v>15.312935</v>
+        <v>15.114108</v>
       </c>
       <c r="W157" s="2">
-        <v>-87.993703999999994</v>
+        <v>-88.040538999999995</v>
       </c>
     </row>
     <row r="158" spans="2:23">
@@ -12905,13 +13005,13 @@
         <v>27</v>
       </c>
       <c r="I158" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J158" s="11" t="s">
-        <v>453</v>
+        <v>471</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>454</v>
+        <v>472</v>
       </c>
       <c r="L158" s="1" t="s">
         <v>30</v>
@@ -12920,28 +13020,28 @@
         <v>1</v>
       </c>
       <c r="N158" s="11" t="s">
-        <v>455</v>
+        <v>473</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>454</v>
+        <v>472</v>
       </c>
       <c r="P158" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q158" s="1" t="s">
-        <v>456</v>
+        <v>474</v>
       </c>
       <c r="R158" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S158" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V158" s="2">
-        <v>15.228071</v>
+        <v>14.97907</v>
       </c>
       <c r="W158" s="2">
-        <v>-87.964016999999998</v>
+        <v>-87.890918999999997</v>
       </c>
     </row>
     <row r="159" spans="2:23">
@@ -12955,55 +13055,55 @@
         <v>3</v>
       </c>
       <c r="E159" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F159" s="10" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I159" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J159" s="11" t="s">
-        <v>457</v>
+        <v>475</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>458</v>
+        <v>476</v>
       </c>
       <c r="L159" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M159" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="N159" s="11" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>458</v>
+        <v>478</v>
       </c>
       <c r="P159" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q159" s="1" t="s">
-        <v>460</v>
+        <v>479</v>
       </c>
       <c r="R159" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S159" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V159" s="2">
-        <v>15.114108</v>
+        <v>15.966279</v>
       </c>
       <c r="W159" s="2">
-        <v>-88.040538999999995</v>
+        <v>-85.096109999999996</v>
       </c>
     </row>
     <row r="160" spans="2:23">
@@ -13017,25 +13117,25 @@
         <v>3</v>
       </c>
       <c r="E160" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F160" s="10" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I160" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J160" s="11" t="s">
-        <v>461</v>
+        <v>480</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>30</v>
@@ -13044,28 +13144,28 @@
         <v>1</v>
       </c>
       <c r="N160" s="11" t="s">
-        <v>463</v>
+        <v>482</v>
       </c>
       <c r="O160" s="1" t="s">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="P160" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q160" s="1" t="s">
-        <v>464</v>
+        <v>483</v>
       </c>
       <c r="R160" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S160" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V160" s="2">
-        <v>14.97907</v>
+        <v>15.864474080000001</v>
       </c>
       <c r="W160" s="2">
-        <v>-87.890918999999997</v>
+        <v>-85.506744999999995</v>
       </c>
     </row>
     <row r="161" spans="2:23">
@@ -13091,43 +13191,43 @@
         <v>27</v>
       </c>
       <c r="I161" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J161" s="11" t="s">
-        <v>465</v>
+        <v>484</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>466</v>
+        <v>485</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M161" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N161" s="11" t="s">
-        <v>467</v>
+        <v>486</v>
       </c>
       <c r="O161" s="1" t="s">
-        <v>468</v>
+        <v>485</v>
       </c>
       <c r="P161" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>469</v>
+        <v>487</v>
       </c>
       <c r="R161" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S161" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V161" s="2">
-        <v>15.966279</v>
+        <v>15.748343</v>
       </c>
       <c r="W161" s="2">
-        <v>-85.096109999999996</v>
+        <v>-85.735150000000004</v>
       </c>
     </row>
     <row r="162" spans="2:23">
@@ -13153,43 +13253,43 @@
         <v>27</v>
       </c>
       <c r="I162" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J162" s="11" t="s">
-        <v>470</v>
+        <v>488</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>471</v>
+        <v>489</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M162" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N162" s="11" t="s">
-        <v>472</v>
+        <v>490</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>471</v>
+        <v>491</v>
       </c>
       <c r="P162" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q162" s="1" t="s">
-        <v>473</v>
+        <v>492</v>
       </c>
       <c r="R162" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S162" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V162" s="2">
-        <v>15.864474080000001</v>
+        <v>15.534311000000001</v>
       </c>
       <c r="W162" s="2">
-        <v>-85.506744999999995</v>
+        <v>-86.273984999999996</v>
       </c>
     </row>
     <row r="163" spans="2:23">
@@ -13203,25 +13303,25 @@
         <v>3</v>
       </c>
       <c r="E163" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F163" s="10" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="H163" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I163" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J163" s="11" t="s">
-        <v>474</v>
+        <v>493</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>475</v>
+        <v>494</v>
       </c>
       <c r="L163" s="1" t="s">
         <v>30</v>
@@ -13230,28 +13330,28 @@
         <v>1</v>
       </c>
       <c r="N163" s="11" t="s">
-        <v>476</v>
+        <v>495</v>
       </c>
       <c r="O163" s="1" t="s">
-        <v>475</v>
+        <v>494</v>
       </c>
       <c r="P163" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q163" s="1" t="s">
-        <v>477</v>
+        <v>496</v>
       </c>
       <c r="R163" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S163" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V163" s="2">
-        <v>15.748343</v>
+        <v>14.894002</v>
       </c>
       <c r="W163" s="2">
-        <v>-85.735150000000004</v>
+        <v>-87.579126000000002</v>
       </c>
     </row>
     <row r="164" spans="2:23">
@@ -13265,55 +13365,55 @@
         <v>3</v>
       </c>
       <c r="E164" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F164" s="10" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="H164" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I164" s="1">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="J164" s="11" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>479</v>
+        <v>498</v>
       </c>
       <c r="L164" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M164" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="N164" s="11" t="s">
-        <v>480</v>
+        <v>499</v>
       </c>
       <c r="O164" s="1" t="s">
-        <v>481</v>
+        <v>498</v>
       </c>
       <c r="P164" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q164" s="1" t="s">
-        <v>482</v>
+        <v>500</v>
       </c>
       <c r="R164" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S164" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V164" s="2">
-        <v>15.534311000000001</v>
+        <v>14.690765000000001</v>
       </c>
       <c r="W164" s="2">
-        <v>-86.273984999999996</v>
+        <v>-87.965248000000003</v>
       </c>
     </row>
     <row r="165" spans="2:23">
@@ -13339,13 +13439,13 @@
         <v>27</v>
       </c>
       <c r="I165" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="J165" s="11" t="s">
-        <v>483</v>
+        <v>501</v>
       </c>
       <c r="K165" s="1" t="s">
-        <v>484</v>
+        <v>502</v>
       </c>
       <c r="L165" s="1" t="s">
         <v>30</v>
@@ -13354,28 +13454,28 @@
         <v>1</v>
       </c>
       <c r="N165" s="11" t="s">
-        <v>485</v>
+        <v>503</v>
       </c>
       <c r="O165" s="1" t="s">
-        <v>484</v>
+        <v>502</v>
       </c>
       <c r="P165" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q165" s="1" t="s">
-        <v>486</v>
+        <v>504</v>
       </c>
       <c r="R165" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S165" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V165" s="2">
-        <v>14.894002</v>
+        <v>14.575887</v>
       </c>
       <c r="W165" s="2">
-        <v>-87.579126000000002</v>
+        <v>-87.728960000000001</v>
       </c>
     </row>
     <row r="166" spans="2:23">
@@ -13401,13 +13501,13 @@
         <v>27</v>
       </c>
       <c r="I166" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J166" s="11" t="s">
-        <v>487</v>
+        <v>505</v>
       </c>
       <c r="K166" s="1" t="s">
-        <v>488</v>
+        <v>506</v>
       </c>
       <c r="L166" s="1" t="s">
         <v>30</v>
@@ -13416,28 +13516,28 @@
         <v>1</v>
       </c>
       <c r="N166" s="11" t="s">
-        <v>489</v>
+        <v>507</v>
       </c>
       <c r="O166" s="1" t="s">
-        <v>488</v>
+        <v>506</v>
       </c>
       <c r="P166" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q166" s="1" t="s">
-        <v>490</v>
+        <v>508</v>
       </c>
       <c r="R166" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S166" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V166" s="2">
-        <v>14.690765000000001</v>
+        <v>14.323912999999999</v>
       </c>
       <c r="W166" s="2">
-        <v>-87.965248000000003</v>
+        <v>-87.613690000000005</v>
       </c>
     </row>
     <row r="167" spans="2:23">
@@ -13451,55 +13551,50 @@
         <v>3</v>
       </c>
       <c r="E167" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F167" s="10" t="s">
-        <v>188</v>
+        <v>77</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>189</v>
+        <v>78</v>
       </c>
       <c r="H167" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I167" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J167" s="11" t="s">
-        <v>491</v>
+        <v>509</v>
       </c>
       <c r="K167" s="1" t="s">
-        <v>492</v>
+        <v>510</v>
       </c>
       <c r="L167" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M167" s="1">
-        <v>1</v>
-      </c>
-      <c r="N167" s="11" t="s">
-        <v>493</v>
-      </c>
+      <c r="N167" s="11"/>
       <c r="O167" s="1" t="s">
-        <v>492</v>
+        <v>510</v>
       </c>
       <c r="P167" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q167" s="1" t="s">
-        <v>494</v>
+        <v>511</v>
       </c>
       <c r="R167" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S167" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V167" s="2">
-        <v>14.575887</v>
+        <v>14.645818</v>
       </c>
       <c r="W167" s="2">
-        <v>-87.728960000000001</v>
+        <v>-88.873898999999994</v>
       </c>
     </row>
     <row r="168" spans="2:23">
@@ -13513,55 +13608,50 @@
         <v>3</v>
       </c>
       <c r="E168" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F168" s="10" t="s">
-        <v>188</v>
+        <v>77</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>189</v>
+        <v>78</v>
       </c>
       <c r="H168" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I168" s="1">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J168" s="11" t="s">
-        <v>495</v>
+        <v>512</v>
       </c>
       <c r="K168" s="1" t="s">
-        <v>496</v>
+        <v>513</v>
       </c>
       <c r="L168" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M168" s="1">
-        <v>1</v>
-      </c>
-      <c r="N168" s="11" t="s">
-        <v>497</v>
-      </c>
+      <c r="N168" s="11"/>
       <c r="O168" s="1" t="s">
-        <v>496</v>
+        <v>513</v>
       </c>
       <c r="P168" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q168" s="1" t="s">
-        <v>498</v>
+        <v>514</v>
       </c>
       <c r="R168" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S168" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V168" s="2">
-        <v>14.323912999999999</v>
+        <v>14.845943</v>
       </c>
       <c r="W168" s="2">
-        <v>-87.613690000000005</v>
+        <v>-88.831519999999998</v>
       </c>
     </row>
     <row r="169" spans="2:23">
@@ -13587,38 +13677,38 @@
         <v>27</v>
       </c>
       <c r="I169" s="1">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="J169" s="11" t="s">
-        <v>499</v>
+        <v>515</v>
       </c>
       <c r="K169" s="1" t="s">
-        <v>500</v>
+        <v>516</v>
       </c>
       <c r="L169" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N169" s="11"/>
       <c r="O169" s="1" t="s">
-        <v>500</v>
+        <v>516</v>
       </c>
       <c r="P169" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q169" s="1" t="s">
-        <v>501</v>
+        <v>517</v>
       </c>
       <c r="R169" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S169" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V169" s="2">
-        <v>14.645818</v>
+        <v>15.001557999999999</v>
       </c>
       <c r="W169" s="2">
-        <v>-88.873898999999994</v>
+        <v>-88.751771000000005</v>
       </c>
     </row>
     <row r="170" spans="2:23">
@@ -13644,38 +13734,43 @@
         <v>27</v>
       </c>
       <c r="I170" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J170" s="11" t="s">
-        <v>502</v>
+        <v>518</v>
       </c>
       <c r="K170" s="1" t="s">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="L170" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N170" s="11"/>
+      <c r="M170" s="1">
+        <v>1</v>
+      </c>
+      <c r="N170" s="11" t="s">
+        <v>520</v>
+      </c>
       <c r="O170" s="1" t="s">
-        <v>503</v>
+        <v>521</v>
       </c>
       <c r="P170" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q170" s="1" t="s">
-        <v>504</v>
+        <v>522</v>
       </c>
       <c r="R170" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S170" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V170" s="2">
-        <v>14.845943</v>
+        <v>15.061814</v>
       </c>
       <c r="W170" s="2">
-        <v>-88.831519999999998</v>
+        <v>-88.746099000000001</v>
       </c>
     </row>
     <row r="171" spans="2:23">
@@ -13701,38 +13796,43 @@
         <v>27</v>
       </c>
       <c r="I171" s="1">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J171" s="11" t="s">
-        <v>505</v>
+        <v>523</v>
       </c>
       <c r="K171" s="1" t="s">
-        <v>506</v>
+        <v>524</v>
       </c>
       <c r="L171" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N171" s="11"/>
+      <c r="M171" s="1">
+        <v>1</v>
+      </c>
+      <c r="N171" s="11" t="s">
+        <v>525</v>
+      </c>
       <c r="O171" s="1" t="s">
-        <v>506</v>
+        <v>524</v>
       </c>
       <c r="P171" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q171" s="1" t="s">
-        <v>507</v>
+        <v>526</v>
       </c>
       <c r="R171" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S171" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V171" s="2">
-        <v>15.001557999999999</v>
+        <v>15.024939</v>
       </c>
       <c r="W171" s="2">
-        <v>-88.751771000000005</v>
+        <v>-88.835689000000002</v>
       </c>
     </row>
     <row r="172" spans="2:23">
@@ -13746,25 +13846,25 @@
         <v>3</v>
       </c>
       <c r="E172" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F172" s="10" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="H172" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I172" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J172" s="11" t="s">
-        <v>508</v>
+        <v>527</v>
       </c>
       <c r="K172" s="1" t="s">
-        <v>509</v>
+        <v>528</v>
       </c>
       <c r="L172" s="1" t="s">
         <v>30</v>
@@ -13773,28 +13873,28 @@
         <v>1</v>
       </c>
       <c r="N172" s="11" t="s">
-        <v>510</v>
+        <v>529</v>
       </c>
       <c r="O172" s="1" t="s">
-        <v>511</v>
+        <v>528</v>
       </c>
       <c r="P172" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q172" s="1" t="s">
-        <v>512</v>
+        <v>530</v>
       </c>
       <c r="R172" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S172" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V172" s="2">
-        <v>15.061814</v>
+        <v>13.665829</v>
       </c>
       <c r="W172" s="2">
-        <v>-88.746099000000001</v>
+        <v>-87.362111999999996</v>
       </c>
     </row>
     <row r="173" spans="2:23">
@@ -13808,25 +13908,25 @@
         <v>3</v>
       </c>
       <c r="E173" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F173" s="10" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="H173" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I173" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J173" s="11" t="s">
-        <v>513</v>
+        <v>531</v>
       </c>
       <c r="K173" s="1" t="s">
-        <v>514</v>
+        <v>532</v>
       </c>
       <c r="L173" s="1" t="s">
         <v>30</v>
@@ -13835,28 +13935,28 @@
         <v>1</v>
       </c>
       <c r="N173" s="11" t="s">
-        <v>515</v>
+        <v>533</v>
       </c>
       <c r="O173" s="1" t="s">
-        <v>514</v>
+        <v>532</v>
       </c>
       <c r="P173" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q173" s="1" t="s">
-        <v>516</v>
+        <v>534</v>
       </c>
       <c r="R173" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S173" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V173" s="2">
-        <v>15.024939</v>
+        <v>13.568472999999999</v>
       </c>
       <c r="W173" s="2">
-        <v>-88.835689000000002</v>
+        <v>-86.907604000000006</v>
       </c>
     </row>
     <row r="174" spans="2:23">
@@ -13882,13 +13982,13 @@
         <v>27</v>
       </c>
       <c r="I174" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J174" s="11" t="s">
-        <v>517</v>
+        <v>535</v>
       </c>
       <c r="K174" s="1" t="s">
-        <v>518</v>
+        <v>536</v>
       </c>
       <c r="L174" s="1" t="s">
         <v>30</v>
@@ -13897,28 +13997,28 @@
         <v>1</v>
       </c>
       <c r="N174" s="11" t="s">
-        <v>519</v>
+        <v>537</v>
       </c>
       <c r="O174" s="1" t="s">
-        <v>518</v>
+        <v>536</v>
       </c>
       <c r="P174" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q174" s="1" t="s">
-        <v>520</v>
+        <v>538</v>
       </c>
       <c r="R174" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S174" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V174" s="2">
-        <v>13.665829</v>
+        <v>13.293342000000001</v>
       </c>
       <c r="W174" s="2">
-        <v>-87.362111999999996</v>
+        <v>-87.111866000000006</v>
       </c>
     </row>
     <row r="175" spans="2:23">
@@ -13944,13 +14044,13 @@
         <v>27</v>
       </c>
       <c r="I175" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J175" s="11" t="s">
-        <v>521</v>
+        <v>539</v>
       </c>
       <c r="K175" s="1" t="s">
-        <v>522</v>
+        <v>540</v>
       </c>
       <c r="L175" s="1" t="s">
         <v>30</v>
@@ -13959,28 +14059,28 @@
         <v>1</v>
       </c>
       <c r="N175" s="11" t="s">
-        <v>523</v>
+        <v>541</v>
       </c>
       <c r="O175" s="1" t="s">
-        <v>522</v>
+        <v>540</v>
       </c>
       <c r="P175" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q175" s="1" t="s">
-        <v>524</v>
+        <v>542</v>
       </c>
       <c r="R175" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S175" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V175" s="2">
-        <v>13.568472999999999</v>
+        <v>13.284371999999999</v>
       </c>
       <c r="W175" s="2">
-        <v>-86.907604000000006</v>
+        <v>-87.312591999999995</v>
       </c>
     </row>
     <row r="176" spans="2:23">
@@ -14006,13 +14106,13 @@
         <v>27</v>
       </c>
       <c r="I176" s="1">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="J176" s="11" t="s">
-        <v>525</v>
+        <v>543</v>
       </c>
       <c r="K176" s="1" t="s">
-        <v>526</v>
+        <v>544</v>
       </c>
       <c r="L176" s="1" t="s">
         <v>30</v>
@@ -14021,28 +14121,28 @@
         <v>1</v>
       </c>
       <c r="N176" s="11" t="s">
-        <v>527</v>
+        <v>545</v>
       </c>
       <c r="O176" s="1" t="s">
-        <v>526</v>
+        <v>544</v>
       </c>
       <c r="P176" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q176" s="1" t="s">
-        <v>528</v>
+        <v>546</v>
       </c>
       <c r="R176" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S176" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V176" s="2">
-        <v>13.293342000000001</v>
+        <v>13.203086000000001</v>
       </c>
       <c r="W176" s="2">
-        <v>-87.111866000000006</v>
+        <v>-87.138760000000005</v>
       </c>
     </row>
     <row r="177" spans="2:23">
@@ -14071,40 +14171,40 @@
         <v>7</v>
       </c>
       <c r="J177" s="11" t="s">
-        <v>529</v>
+        <v>539</v>
       </c>
       <c r="K177" s="1" t="s">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="L177" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M177" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N177" s="11" t="s">
-        <v>531</v>
+        <v>547</v>
       </c>
       <c r="O177" s="1" t="s">
-        <v>530</v>
+        <v>548</v>
       </c>
       <c r="P177" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q177" s="1" t="s">
-        <v>532</v>
+        <v>542</v>
       </c>
       <c r="R177" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S177" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V177" s="2">
-        <v>13.284371999999999</v>
+        <v>13.198708</v>
       </c>
       <c r="W177" s="2">
-        <v>-87.312591999999995</v>
+        <v>-87.375152999999997</v>
       </c>
     </row>
     <row r="178" spans="2:23">
@@ -14118,55 +14218,50 @@
         <v>3</v>
       </c>
       <c r="E178" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F178" s="10" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="H178" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I178" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J178" s="11" t="s">
-        <v>533</v>
+        <v>549</v>
       </c>
       <c r="K178" s="1" t="s">
-        <v>534</v>
+        <v>550</v>
       </c>
       <c r="L178" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M178" s="1">
-        <v>1</v>
-      </c>
-      <c r="N178" s="11" t="s">
-        <v>535</v>
-      </c>
+      <c r="N178" s="11"/>
       <c r="O178" s="1" t="s">
-        <v>534</v>
+        <v>550</v>
       </c>
       <c r="P178" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q178" s="1" t="s">
-        <v>536</v>
+        <v>551</v>
       </c>
       <c r="R178" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S178" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V178" s="2">
-        <v>13.203086000000001</v>
+        <v>13.932454999999999</v>
       </c>
       <c r="W178" s="2">
-        <v>-87.138760000000005</v>
+        <v>-87.297745000000006</v>
       </c>
     </row>
     <row r="179" spans="2:23">
@@ -14180,55 +14275,55 @@
         <v>3</v>
       </c>
       <c r="E179" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F179" s="10" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="H179" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I179" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J179" s="11" t="s">
-        <v>529</v>
+        <v>552</v>
       </c>
       <c r="K179" s="1" t="s">
-        <v>530</v>
+        <v>553</v>
       </c>
       <c r="L179" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M179" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="N179" s="11" t="s">
-        <v>537</v>
+        <v>554</v>
       </c>
       <c r="O179" s="1" t="s">
-        <v>538</v>
+        <v>553</v>
       </c>
       <c r="P179" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q179" s="1" t="s">
-        <v>532</v>
+        <v>555</v>
       </c>
       <c r="R179" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S179" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V179" s="2">
-        <v>13.198708</v>
+        <v>14.915877999999999</v>
       </c>
       <c r="W179" s="2">
-        <v>-87.375152999999997</v>
+        <v>-87.194401999999997</v>
       </c>
     </row>
     <row r="180" spans="2:23">
@@ -14254,38 +14349,43 @@
         <v>27</v>
       </c>
       <c r="I180" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J180" s="11" t="s">
-        <v>539</v>
+        <v>556</v>
       </c>
       <c r="K180" s="1" t="s">
-        <v>540</v>
+        <v>557</v>
       </c>
       <c r="L180" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N180" s="11"/>
+      <c r="M180" s="1">
+        <v>1</v>
+      </c>
+      <c r="N180" s="11" t="s">
+        <v>558</v>
+      </c>
       <c r="O180" s="1" t="s">
-        <v>540</v>
+        <v>557</v>
       </c>
       <c r="P180" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q180" s="1" t="s">
-        <v>541</v>
+        <v>559</v>
       </c>
       <c r="R180" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S180" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V180" s="2">
-        <v>13.932454999999999</v>
+        <v>14.754858</v>
       </c>
       <c r="W180" s="2">
-        <v>-87.297745000000006</v>
+        <v>-87.188080999999997</v>
       </c>
     </row>
     <row r="181" spans="2:23">
@@ -14311,43 +14411,43 @@
         <v>27</v>
       </c>
       <c r="I181" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J181" s="11" t="s">
-        <v>542</v>
+        <v>560</v>
       </c>
       <c r="K181" s="1" t="s">
-        <v>543</v>
+        <v>561</v>
       </c>
       <c r="L181" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M181" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N181" s="11" t="s">
-        <v>544</v>
+        <v>562</v>
       </c>
       <c r="O181" s="1" t="s">
-        <v>543</v>
+        <v>561</v>
       </c>
       <c r="P181" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q181" s="1" t="s">
-        <v>545</v>
+        <v>563</v>
       </c>
       <c r="R181" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S181" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V181" s="2">
-        <v>14.915877999999999</v>
+        <v>14.714986</v>
       </c>
       <c r="W181" s="2">
-        <v>-87.194401999999997</v>
+        <v>-86.942893999999995</v>
       </c>
     </row>
     <row r="182" spans="2:23">
@@ -14373,13 +14473,13 @@
         <v>27</v>
       </c>
       <c r="I182" s="1">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="J182" s="11" t="s">
-        <v>546</v>
+        <v>564</v>
       </c>
       <c r="K182" s="1" t="s">
-        <v>547</v>
+        <v>565</v>
       </c>
       <c r="L182" s="1" t="s">
         <v>30</v>
@@ -14388,28 +14488,28 @@
         <v>1</v>
       </c>
       <c r="N182" s="11" t="s">
-        <v>548</v>
+        <v>566</v>
       </c>
       <c r="O182" s="1" t="s">
-        <v>547</v>
+        <v>565</v>
       </c>
       <c r="P182" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q182" s="1" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="R182" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S182" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V182" s="2">
-        <v>14.754858</v>
+        <v>14.654638</v>
       </c>
       <c r="W182" s="2">
-        <v>-87.188080999999997</v>
+        <v>-87.036589000000006</v>
       </c>
     </row>
     <row r="183" spans="2:23">
@@ -14435,13 +14535,13 @@
         <v>27</v>
       </c>
       <c r="I183" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="J183" s="11" t="s">
-        <v>550</v>
+        <v>568</v>
       </c>
       <c r="K183" s="1" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
       <c r="L183" s="1" t="s">
         <v>30</v>
@@ -14450,28 +14550,28 @@
         <v>1</v>
       </c>
       <c r="N183" s="11" t="s">
-        <v>552</v>
+        <v>570</v>
       </c>
       <c r="O183" s="1" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
       <c r="P183" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q183" s="1" t="s">
-        <v>553</v>
+        <v>571</v>
       </c>
       <c r="R183" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S183" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V183" s="2">
-        <v>14.714986</v>
+        <v>14.593650999999999</v>
       </c>
       <c r="W183" s="2">
-        <v>-86.942893999999995</v>
+        <v>-87.119091999999995</v>
       </c>
     </row>
     <row r="184" spans="2:23">
@@ -14485,55 +14585,55 @@
         <v>3</v>
       </c>
       <c r="E184" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F184" s="10" t="s">
-        <v>38</v>
+        <v>282</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>39</v>
+        <v>283</v>
       </c>
       <c r="H184" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I184" s="1">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="J184" s="11" t="s">
-        <v>554</v>
+        <v>328</v>
       </c>
       <c r="K184" s="1" t="s">
-        <v>555</v>
+        <v>329</v>
       </c>
       <c r="L184" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M184" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N184" s="11" t="s">
-        <v>556</v>
+        <v>572</v>
       </c>
       <c r="O184" s="1" t="s">
-        <v>555</v>
+        <v>573</v>
       </c>
       <c r="P184" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q184" s="1" t="s">
-        <v>557</v>
+        <v>331</v>
       </c>
       <c r="R184" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S184" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V184" s="2">
-        <v>14.654638</v>
+        <v>15.893539000000001</v>
       </c>
       <c r="W184" s="2">
-        <v>-87.036589000000006</v>
+        <v>-84.776458000000005</v>
       </c>
     </row>
     <row r="185" spans="2:23">
@@ -14547,55 +14647,55 @@
         <v>3</v>
       </c>
       <c r="E185" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F185" s="10" t="s">
-        <v>38</v>
+        <v>282</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>39</v>
+        <v>283</v>
       </c>
       <c r="H185" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I185" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J185" s="11" t="s">
-        <v>558</v>
+        <v>328</v>
       </c>
       <c r="K185" s="1" t="s">
-        <v>559</v>
+        <v>329</v>
       </c>
       <c r="L185" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M185" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N185" s="11" t="s">
-        <v>560</v>
+        <v>574</v>
       </c>
       <c r="O185" s="1" t="s">
-        <v>559</v>
+        <v>575</v>
       </c>
       <c r="P185" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q185" s="1" t="s">
-        <v>561</v>
+        <v>331</v>
       </c>
       <c r="R185" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S185" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V185" s="2">
-        <v>14.593650999999999</v>
+        <v>15.799147</v>
       </c>
       <c r="W185" s="2">
-        <v>-87.119091999999995</v>
+        <v>-84.294206000000003</v>
       </c>
     </row>
     <row r="186" spans="2:23">
@@ -14621,43 +14721,43 @@
         <v>27</v>
       </c>
       <c r="I186" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J186" s="11" t="s">
-        <v>562</v>
+        <v>576</v>
       </c>
       <c r="K186" s="1" t="s">
-        <v>563</v>
+        <v>577</v>
       </c>
       <c r="L186" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M186" s="1">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="N186" s="11" t="s">
-        <v>564</v>
+        <v>578</v>
       </c>
       <c r="O186" s="1" t="s">
-        <v>565</v>
+        <v>579</v>
       </c>
       <c r="P186" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q186" s="1" t="s">
-        <v>566</v>
+        <v>580</v>
       </c>
       <c r="R186" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S186" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V186" s="2">
-        <v>15.893539000000001</v>
+        <v>15.064120000000001</v>
       </c>
       <c r="W186" s="2">
-        <v>-84.776458000000005</v>
+        <v>-83.298761999999996</v>
       </c>
     </row>
     <row r="187" spans="2:23">
@@ -14683,43 +14783,43 @@
         <v>27</v>
       </c>
       <c r="I187" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J187" s="11" t="s">
-        <v>562</v>
+        <v>581</v>
       </c>
       <c r="K187" s="1" t="s">
-        <v>563</v>
+        <v>582</v>
       </c>
       <c r="L187" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M187" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N187" s="11" t="s">
-        <v>567</v>
+        <v>583</v>
       </c>
       <c r="O187" s="1" t="s">
-        <v>568</v>
+        <v>584</v>
       </c>
       <c r="P187" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q187" s="1" t="s">
-        <v>566</v>
+        <v>585</v>
       </c>
       <c r="R187" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S187" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V187" s="2">
-        <v>15.799147</v>
+        <v>15.043042</v>
       </c>
       <c r="W187" s="2">
-        <v>-84.294206000000003</v>
+        <v>-84.874465000000001</v>
       </c>
     </row>
     <row r="188" spans="2:23">
@@ -14733,55 +14833,55 @@
         <v>3</v>
       </c>
       <c r="E188" s="7">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F188" s="10" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>283</v>
+        <v>155</v>
       </c>
       <c r="H188" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I188" s="1">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="J188" s="11" t="s">
-        <v>569</v>
+        <v>586</v>
       </c>
       <c r="K188" s="1" t="s">
-        <v>570</v>
+        <v>587</v>
       </c>
       <c r="L188" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M188" s="1">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="N188" s="11" t="s">
-        <v>571</v>
+        <v>588</v>
       </c>
       <c r="O188" s="1" t="s">
-        <v>572</v>
+        <v>589</v>
       </c>
       <c r="P188" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q188" s="1" t="s">
-        <v>573</v>
+        <v>590</v>
       </c>
       <c r="R188" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S188" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V188" s="2">
-        <v>15.064120000000001</v>
+        <v>15.079923000000001</v>
       </c>
       <c r="W188" s="2">
-        <v>-83.298761999999996</v>
+        <v>-85.832560000000001</v>
       </c>
     </row>
     <row r="189" spans="2:23">
@@ -14795,55 +14895,55 @@
         <v>3</v>
       </c>
       <c r="E189" s="7">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F189" s="10" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>283</v>
+        <v>155</v>
       </c>
       <c r="H189" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I189" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J189" s="11" t="s">
-        <v>574</v>
+        <v>591</v>
       </c>
       <c r="K189" s="1" t="s">
-        <v>575</v>
+        <v>592</v>
       </c>
       <c r="L189" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M189" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N189" s="11" t="s">
-        <v>576</v>
+        <v>593</v>
       </c>
       <c r="O189" s="1" t="s">
-        <v>577</v>
+        <v>592</v>
       </c>
       <c r="P189" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q189" s="1" t="s">
-        <v>578</v>
+        <v>594</v>
       </c>
       <c r="R189" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S189" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V189" s="2">
-        <v>15.043042</v>
+        <v>15.079139</v>
       </c>
       <c r="W189" s="2">
-        <v>-84.874465000000001</v>
+        <v>-86.418364999999994</v>
       </c>
     </row>
     <row r="190" spans="2:23">
@@ -14869,43 +14969,43 @@
         <v>27</v>
       </c>
       <c r="I190" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J190" s="11" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
       <c r="K190" s="1" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="L190" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M190" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="N190" s="11" t="s">
-        <v>581</v>
+        <v>597</v>
       </c>
       <c r="O190" s="1" t="s">
-        <v>582</v>
+        <v>596</v>
       </c>
       <c r="P190" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q190" s="1" t="s">
-        <v>583</v>
+        <v>598</v>
       </c>
       <c r="R190" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S190" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V190" s="2">
-        <v>15.079923000000001</v>
+        <v>15.035551</v>
       </c>
       <c r="W190" s="2">
-        <v>-85.832560000000001</v>
+        <v>-86.819034000000002</v>
       </c>
     </row>
     <row r="191" spans="2:23">
@@ -14931,13 +15031,13 @@
         <v>27</v>
       </c>
       <c r="I191" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J191" s="11" t="s">
-        <v>584</v>
+        <v>599</v>
       </c>
       <c r="K191" s="1" t="s">
-        <v>585</v>
+        <v>600</v>
       </c>
       <c r="L191" s="1" t="s">
         <v>30</v>
@@ -14946,28 +15046,28 @@
         <v>1</v>
       </c>
       <c r="N191" s="11" t="s">
-        <v>586</v>
+        <v>601</v>
       </c>
       <c r="O191" s="1" t="s">
-        <v>585</v>
+        <v>600</v>
       </c>
       <c r="P191" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q191" s="1" t="s">
-        <v>587</v>
+        <v>602</v>
       </c>
       <c r="R191" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S191" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V191" s="2">
-        <v>15.079139</v>
+        <v>15.028809000000001</v>
       </c>
       <c r="W191" s="2">
-        <v>-86.418364999999994</v>
+        <v>-86.508201999999997</v>
       </c>
     </row>
     <row r="192" spans="2:23">
@@ -14993,13 +15093,13 @@
         <v>27</v>
       </c>
       <c r="I192" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J192" s="11" t="s">
-        <v>588</v>
+        <v>603</v>
       </c>
       <c r="K192" s="1" t="s">
-        <v>589</v>
+        <v>604</v>
       </c>
       <c r="L192" s="1" t="s">
         <v>30</v>
@@ -15008,220 +15108,33 @@
         <v>1</v>
       </c>
       <c r="N192" s="11" t="s">
-        <v>590</v>
+        <v>605</v>
       </c>
       <c r="O192" s="1" t="s">
-        <v>589</v>
+        <v>604</v>
       </c>
       <c r="P192" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q192" s="1" t="s">
-        <v>591</v>
+        <v>606</v>
       </c>
       <c r="R192" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S192" s="1" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="V192" s="2">
-        <v>15.035551</v>
+        <v>14.644175000000001</v>
       </c>
       <c r="W192" s="2">
-        <v>-86.819034000000002</v>
-      </c>
-    </row>
-    <row r="193" spans="2:23">
-      <c r="B193" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C193" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D193" s="1">
-        <v>3</v>
-      </c>
-      <c r="E193" s="7">
-        <v>15</v>
-      </c>
-      <c r="F193" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="G193" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H193" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I193" s="1">
-        <v>12</v>
-      </c>
-      <c r="J193" s="11" t="s">
-        <v>592</v>
-      </c>
-      <c r="K193" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="L193" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M193" s="1">
-        <v>1</v>
-      </c>
-      <c r="N193" s="11" t="s">
-        <v>594</v>
-      </c>
-      <c r="O193" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P193" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q193" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="R193" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S193" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="V193" s="2">
-        <v>15.028809000000001</v>
-      </c>
-      <c r="W193" s="2">
-        <v>-86.508201999999997</v>
-      </c>
-    </row>
-    <row r="194" spans="2:23">
-      <c r="B194" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C194" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D194" s="1">
-        <v>3</v>
-      </c>
-      <c r="E194" s="7">
-        <v>15</v>
-      </c>
-      <c r="F194" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="G194" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H194" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I194" s="1">
-        <v>18</v>
-      </c>
-      <c r="J194" s="11" t="s">
-        <v>596</v>
-      </c>
-      <c r="K194" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="L194" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M194" s="1">
-        <v>1</v>
-      </c>
-      <c r="N194" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="O194" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="P194" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q194" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="R194" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S194" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="V194" s="2">
-        <v>14.644175000000001</v>
-      </c>
-      <c r="W194" s="2">
         <v>-86.105974000000003</v>
       </c>
     </row>
-    <row r="195" spans="2:23">
-      <c r="B195" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C195" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D195" s="1">
-        <v>3</v>
-      </c>
-      <c r="E195" s="7"/>
-      <c r="F195" s="10"/>
-      <c r="H195" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J195" s="11"/>
-      <c r="L195" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N195" s="11"/>
-      <c r="P195" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q195" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="R195" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S195" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="196" spans="2:23">
-      <c r="B196" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C196" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D196" s="1">
-        <v>3</v>
-      </c>
-      <c r="E196" s="7"/>
-      <c r="F196" s="10"/>
-      <c r="H196" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J196" s="11"/>
-      <c r="L196" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N196" s="11"/>
-      <c r="P196" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q196" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="R196" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S196" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
+    <row r="193" ht="15"/>
+    <row r="194" ht="15"/>
+    <row r="195" ht="15"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U83">
     <sortCondition ref="R2:R83"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-15-2020 04-05-57
</commit_message>
<xml_diff>
--- a/datacovidhn/SALUD_HN.xlsx
+++ b/datacovidhn/SALUD_HN.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -2858,8 +2858,8 @@
   <dimension ref="A1:W195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="P178" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A194" sqref="A193:XFD194"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>

</xml_diff>